<commit_message>
Tasks: Update the tasks list
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E7BCE42-4EA4-451B-9083-A646CE9EA9A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A40F74-3502-4997-ACFC-F495C7A15712}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="21435" windowHeight="16680" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="1950" yWindow="600" windowWidth="21435" windowHeight="16680" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -280,6 +280,207 @@
   </si>
   <si>
     <t>Add TabView</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>Add Status Bar</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>Add Status Bar contents and bind to ShellViewModel</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Bluebeam</t>
+  </si>
+  <si>
+    <t>Ask G</t>
+  </si>
+  <si>
+    <t>G: What is this?  Need direction on this.</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Add Facility View and ViewModel</t>
+  </si>
+  <si>
+    <t>Add 'Identity' items</t>
+  </si>
+  <si>
+    <t>Add 'Faility Comment' TextBox</t>
+  </si>
+  <si>
+    <t>Add 'Photos thumbnails' Listbox</t>
+  </si>
+  <si>
+    <t>Add 'Address' items</t>
+  </si>
+  <si>
+    <t>Add 'Point of contact' items</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Add left justified Label style</t>
+  </si>
+  <si>
+    <t>Add center justified Label style</t>
+  </si>
+  <si>
+    <t>Add right justified Label style</t>
+  </si>
+  <si>
+    <t>Add bold Label stytle</t>
+  </si>
+  <si>
+    <t>Add gray BG black bounded Label style</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Add Inventory View and ViewModel</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>IS1</t>
+  </si>
+  <si>
+    <t>I-Section</t>
+  </si>
+  <si>
+    <t>Add InventorySection View and ViewModel</t>
+  </si>
+  <si>
+    <t>Add Section Name list control</t>
+  </si>
+  <si>
+    <t>Add Section ComboBox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Equipment Category caption and bind to VM which changes </t>
+  </si>
+  <si>
+    <t>IS2</t>
+  </si>
+  <si>
+    <t>IS3</t>
+  </si>
+  <si>
+    <t>IS4</t>
+  </si>
+  <si>
+    <t>IS4.Q1</t>
+  </si>
+  <si>
+    <t>G: What are the rules for Category caption change?</t>
+  </si>
+  <si>
+    <t>Add Category ComboBox</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add Component Type Label and ComboBox</t>
+  </si>
+  <si>
+    <t>Add Quantity</t>
+  </si>
+  <si>
+    <t>Add year Installed</t>
+  </si>
+  <si>
+    <t>Add Functional Area</t>
+  </si>
+  <si>
+    <t>Add Not Energy</t>
+  </si>
+  <si>
+    <t>Add Painted</t>
+  </si>
+  <si>
+    <t>Add Section Comment</t>
+  </si>
+  <si>
+    <t>Add Remember</t>
+  </si>
+  <si>
+    <t>Add Photos</t>
+  </si>
+  <si>
+    <t>Add Photos List</t>
+  </si>
+  <si>
+    <t>Add current inspector date</t>
+  </si>
+  <si>
+    <t>Add Cancel button</t>
+  </si>
+  <si>
+    <t>Add Delete Section button</t>
+  </si>
+  <si>
+    <t>Add 'Add Section' button</t>
+  </si>
+  <si>
+    <t>IS5</t>
+  </si>
+  <si>
+    <t>IS6</t>
+  </si>
+  <si>
+    <t>IS7</t>
+  </si>
+  <si>
+    <t>IS8</t>
+  </si>
+  <si>
+    <t>IS9</t>
+  </si>
+  <si>
+    <t>IS10</t>
+  </si>
+  <si>
+    <t>IS11</t>
+  </si>
+  <si>
+    <t>IS12</t>
+  </si>
+  <si>
+    <t>IS13</t>
+  </si>
+  <si>
+    <t>IS14</t>
+  </si>
+  <si>
+    <t>IS15</t>
+  </si>
+  <si>
+    <t>IS16</t>
+  </si>
+  <si>
+    <t>IS17</t>
+  </si>
+  <si>
+    <t>IS18</t>
+  </si>
+  <si>
+    <t>IS19</t>
   </si>
 </sst>
 </file>
@@ -631,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,328 +857,603 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>54</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B37" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C37" t="s">
         <v>58</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>62</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>63</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C42" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C43" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>71</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C44" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>75</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C46" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>77</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C47" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>79</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>81</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>83</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C50" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>144</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>147</v>
+      </c>
+      <c r="C80" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>149</v>
+      </c>
+      <c r="C82" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications to the ShellView.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC1FC54-FF22-450A-B60E-C4F445D249D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C1F3A-86C8-4D98-AD03-4F44820F926F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="14700" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="3045" yWindow="15075" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="274">
   <si>
     <t>ID</t>
   </si>
@@ -532,9 +532,6 @@
   </si>
   <si>
     <t>Need better definition of tree items / filters.</t>
-  </si>
-  <si>
-    <t>Done ?</t>
   </si>
   <si>
     <t>Tear-off sidebar?</t>
@@ -785,18 +782,12 @@
     <t>L5.Q1.1</t>
   </si>
   <si>
-    <t>rlh - no. Save to user setting string.</t>
-  </si>
-  <si>
     <t>L12.Q1.1</t>
   </si>
   <si>
     <t>L12.Q1</t>
   </si>
   <si>
-    <t>rlh - See L5. Save to user setting string.</t>
-  </si>
-  <si>
     <t>Save/Retrieve Build Config contents to user sesttings string resources</t>
   </si>
   <si>
@@ -812,18 +803,12 @@
     <t>L31.FB.R1</t>
   </si>
   <si>
-    <t>rlh - Increased the text box and combo box font size. However, the validation error string will be a little more difficult. It can be done, just not a trvial change. Will do this later.</t>
-  </si>
-  <si>
     <t>Partially addressed</t>
   </si>
   <si>
     <t>L32.FB.R1</t>
   </si>
   <si>
-    <t>rlh - Changed the TextBox from to allow wrapping. When a wrap occurs then the box gets taller to accommodate the text.</t>
-  </si>
-  <si>
     <t>Addressed</t>
   </si>
   <si>
@@ -834,6 +819,57 @@
   </si>
   <si>
     <t>rlh - Replaced the existing logo with a new one. New image is *much* nicer.</t>
+  </si>
+  <si>
+    <t>S15.Q1.1</t>
+  </si>
+  <si>
+    <t>rlh - yes</t>
+  </si>
+  <si>
+    <t>S17.FB.1</t>
+  </si>
+  <si>
+    <t>S21.FB.1</t>
+  </si>
+  <si>
+    <t>Added the toolbar buttons but 'currently selected' indication is not yet implemented</t>
+  </si>
+  <si>
+    <t>Removed the spurious Toolbar and updated the remaining one.</t>
+  </si>
+  <si>
+    <t>no. Save to user setting string.</t>
+  </si>
+  <si>
+    <t>See L5. Save to user setting string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Increased the text box and combo box font size. However, the validation error string will be a little more difficult. It can be done, just not a trvial change. Will do this later.</t>
+  </si>
+  <si>
+    <t>Changed the TextBox from to allow wrapping. When a wrap occurs then the box gets taller to accommodate the text.</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>S18.FB.1</t>
+  </si>
+  <si>
+    <t>This is possible but not trivial. Will delay implementation until after more functional things have been completed.</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>In process</t>
+  </si>
+  <si>
+    <t>S22.FB.1</t>
+  </si>
+  <si>
+    <t>The 'add system and delete system icon' thing is a little confusing. Can you elaborate on that?</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,7 +1295,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>103</v>
@@ -1267,7 +1303,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>104</v>
@@ -1275,7 +1311,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>105</v>
@@ -1283,7 +1319,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>106</v>
@@ -1291,29 +1327,29 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,7 +1377,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
@@ -1349,10 +1385,10 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
@@ -1396,7 +1432,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
@@ -1411,18 +1447,18 @@
         <v>152</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,7 +1537,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
@@ -1510,10 +1546,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,7 +1616,7 @@
         <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1669,7 @@
         <v>154</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,10 +1718,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
@@ -1693,10 +1729,10 @@
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>7</v>
@@ -1707,13 +1743,13 @@
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E48" s="5">
         <v>43554</v>
@@ -1721,10 +1757,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>7</v>
@@ -1735,10 +1771,10 @@
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>7</v>
@@ -1749,10 +1785,10 @@
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>7</v>
@@ -1763,13 +1799,13 @@
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E52" s="5">
         <v>43554</v>
@@ -1777,10 +1813,10 @@
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E53" s="5">
         <v>43554</v>
@@ -1788,13 +1824,13 @@
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E54" s="5">
         <v>43554</v>
@@ -1802,10 +1838,10 @@
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>7</v>
@@ -1816,10 +1852,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1861,6 +1897,9 @@
       <c r="C61" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="D61" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -1870,6 +1909,9 @@
       <c r="C62" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="D62" s="2" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -1879,6 +1921,9 @@
       <c r="C63" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="D63" s="2" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -1991,6 +2036,9 @@
       <c r="C74" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D74" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -1999,19 +2047,21 @@
       <c r="C75" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>169</v>
+      <c r="D75" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D76" s="4"/>
+        <v>172</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -2054,154 +2104,207 @@
       <c r="C80" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>171</v>
+      <c r="D80" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="3"/>
+      <c r="C82" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E85" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D89" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E90" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C87" s="2" t="s">
+    </row>
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E92" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
+    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="96" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="97" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="4" t="s">
-        <v>189</v>
+      <c r="D98" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>7</v>
@@ -2209,10 +2312,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>7</v>
@@ -2220,254 +2323,296 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>208</v>
+        <v>97</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B102" s="3"/>
+      <c r="C102" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>224</v>
+        <v>98</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>227</v>
+        <v>99</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>107</v>
+        <v>222</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C129" s="2" t="s">
+    </row>
+    <row r="134" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="C134" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="D134" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D130" s="2" t="s">
+    </row>
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="C135" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C131" s="2" t="s">
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="C136" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sticky window placement.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C1F3A-86C8-4D98-AD03-4F44820F926F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B764C-4E6E-4A28-B193-113D91C3BC1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="15075" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="2100" yWindow="1155" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="288">
   <si>
     <t>ID</t>
   </si>
@@ -870,6 +870,48 @@
   </si>
   <si>
     <t>The 'add system and delete system icon' thing is a little confusing. Can you elaborate on that?</t>
+  </si>
+  <si>
+    <t>Toolbar</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Add buttons that show and hide depending upon the currently active tab control</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>Ask G for an image for Copy Inventory button</t>
+  </si>
+  <si>
+    <t>Ask G for an image for Copy Inspection button</t>
+  </si>
+  <si>
+    <t>Ask G for an image for Copy Sections button</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>Modify the Tab item style to be fat finger compatible and more colorful on selection.</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>Remember and reassert window placement between sessions</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2285,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>272</v>
       </c>
@@ -2257,65 +2299,64 @@
         <v>43554</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E93" s="5"/>
+    </row>
+    <row r="94" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C94" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="98" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="99" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>184</v>
+        <v>92</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>7</v>
@@ -2323,296 +2364,364 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="4" t="s">
-        <v>188</v>
+      <c r="A102" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>7</v>
+      <c r="A104" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>207</v>
+        <v>98</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>226</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>108</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+    <row r="136" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D136" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E141" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug: Shell briefly flashes before Login is displayed. Should not.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B764C-4E6E-4A28-B193-113D91C3BC1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B9F301-19B7-438B-A157-BC678EABBB6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1155" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="3045" yWindow="15075" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="290">
   <si>
     <t>ID</t>
   </si>
@@ -912,6 +912,12 @@
   </si>
   <si>
     <t>Remember and reassert window placement between sessions</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>Bug: Before Login shows, the Shell briefly flashes. It should not.</t>
   </si>
 </sst>
 </file>
@@ -1293,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,52 +2328,55 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="95" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="100" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>183</v>
+        <v>92</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>7</v>
@@ -2375,10 +2384,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>7</v>
@@ -2386,41 +2395,41 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="D104" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4" t="s">
+      <c r="B105" s="3"/>
+      <c r="C105" s="4" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>7</v>
@@ -2428,299 +2437,310 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>207</v>
+        <v>99</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+    <row r="137" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E141" s="5">
-        <v>43554</v>
+        <v>275</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" s="5">
+        <v>43554</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>283</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor change to Toolbar numbering
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B9F301-19B7-438B-A157-BC678EABBB6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745C9282-6401-4471-928D-37C3D1779F4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="15075" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="289">
   <si>
     <t>ID</t>
   </si>
@@ -749,9 +749,6 @@
     <t>G: • Section Name, Equip Cat and Component Type only need a single line - rlh: From the notes it looks like these values cannot be directory edited by the user. Instead, the user selects a member for a list of possibilities. Accordingly, DropDown ComboBox's are being used for these items, not Labels or TextBoxes.</t>
   </si>
   <si>
-    <t>Possible misunderstanding. Need to ask G.</t>
-  </si>
-  <si>
     <t>IS23.FB</t>
   </si>
   <si>
@@ -890,9 +887,6 @@
     <t>T4</t>
   </si>
   <si>
-    <t>T5</t>
-  </si>
-  <si>
     <t>Ask G for an image for Copy Inventory button</t>
   </si>
   <si>
@@ -918,6 +912,9 @@
   </si>
   <si>
     <t>Bug: Before Login shows, the Shell briefly flashes. It should not.</t>
+  </si>
+  <si>
+    <t>Possible misunderstanding. Need to ask G. Waiting for response</t>
   </si>
 </sst>
 </file>
@@ -1301,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1324,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,7 +1422,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
@@ -1433,10 +1430,10 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
@@ -1480,7 +1477,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
@@ -1495,18 +1492,18 @@
         <v>152</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1582,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
@@ -1594,10 +1591,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1664,7 +1661,7 @@
         <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,7 +1714,7 @@
         <v>154</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,7 +1794,7 @@
         <v>193</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E48" s="5">
         <v>43554</v>
@@ -1805,10 +1802,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>7</v>
@@ -1853,7 +1850,7 @@
         <v>196</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E52" s="5">
         <v>43554</v>
@@ -1861,10 +1858,10 @@
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E53" s="5">
         <v>43554</v>
@@ -1878,7 +1875,7 @@
         <v>197</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E54" s="5">
         <v>43554</v>
@@ -1886,10 +1883,10 @@
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>7</v>
@@ -1900,10 +1897,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="E56" s="5"/>
     </row>
@@ -1958,7 +1955,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1970,7 +1967,7 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,7 +2105,7 @@
         <v>172</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,19 +2150,19 @@
         <v>166</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,10 +2190,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>7</v>
@@ -2213,7 +2210,7 @@
         <v>214</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E85" s="5">
         <v>43554</v>
@@ -2221,13 +2218,13 @@
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2266,18 +2263,18 @@
         <v>216</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="D90" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E90" s="5">
         <v>43554</v>
@@ -2293,13 +2290,13 @@
     </row>
     <row r="92" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="D92" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E92" s="5">
         <v>43554</v>
@@ -2307,19 +2304,19 @@
     </row>
     <row r="93" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>7</v>
@@ -2330,10 +2327,10 @@
     </row>
     <row r="95" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>7</v>
@@ -2342,7 +2339,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>220</v>
       </c>
@@ -2353,7 +2350,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>88</v>
       </c>
@@ -2366,9 +2363,12 @@
       <c r="D99" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>92</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>183</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>184</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>185</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>189</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>186</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>187</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>206</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>222</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>224</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>225</v>
       </c>
@@ -2662,6 +2662,12 @@
       <c r="C135" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="D135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
@@ -2679,39 +2685,39 @@
         <v>232</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>233</v>
+        <v>288</v>
+      </c>
+      <c r="E137" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="B141" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>7</v>
@@ -2722,26 +2728,44 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E143" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E144" s="5">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E145" s="5">
+        <v>43537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to wire the new Views to the buttons that launch them. Starting to include the MVVM compliant dialog result ex method.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745C9282-6401-4471-928D-37C3D1779F4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54662C88-4965-4E6E-995D-2BE97761CAB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="15075" windowWidth="18945" windowHeight="16560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="1245" yWindow="17310" windowWidth="21840" windowHeight="13770" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="378">
   <si>
     <t>ID</t>
   </si>
@@ -915,6 +915,273 @@
   </si>
   <si>
     <t>Possible misunderstanding. Need to ask G. Waiting for response</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>Add View and ViewModel class skeletons</t>
+  </si>
+  <si>
+    <t>CM2</t>
+  </si>
+  <si>
+    <t>Add toolbar and connect images to each button</t>
+  </si>
+  <si>
+    <t>CM3</t>
+  </si>
+  <si>
+    <t>Get more info on what data and controls are in the View from G.</t>
+  </si>
+  <si>
+    <t>Comment Popup</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>Comment on Inspection</t>
+  </si>
+  <si>
+    <t>CI1</t>
+  </si>
+  <si>
+    <t>Add View and ViewModel class skeletons.</t>
+  </si>
+  <si>
+    <t>Add radio buttons</t>
+  </si>
+  <si>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>Create a style for radio buttons so that they match the spec</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Copy Commentary</t>
+  </si>
+  <si>
+    <t>CC1</t>
+  </si>
+  <si>
+    <t>CC2</t>
+  </si>
+  <si>
+    <t>CC3</t>
+  </si>
+  <si>
+    <t>Add Related to current row</t>
+  </si>
+  <si>
+    <t>Add Source row</t>
+  </si>
+  <si>
+    <t>CC4</t>
+  </si>
+  <si>
+    <t>Add Rated as row</t>
+  </si>
+  <si>
+    <t>CC5</t>
+  </si>
+  <si>
+    <t>Add Search term row</t>
+  </si>
+  <si>
+    <t>CC6</t>
+  </si>
+  <si>
+    <t>Add Facility code DCR Comment data grid</t>
+  </si>
+  <si>
+    <t>CC7</t>
+  </si>
+  <si>
+    <t>Add bottom button row</t>
+  </si>
+  <si>
+    <t>Copy Inventory</t>
+  </si>
+  <si>
+    <t>CI2</t>
+  </si>
+  <si>
+    <t>CI3</t>
+  </si>
+  <si>
+    <t>CI4</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CN1</t>
+  </si>
+  <si>
+    <t>CN2</t>
+  </si>
+  <si>
+    <t>Add Source Facility row</t>
+  </si>
+  <si>
+    <t>CN3</t>
+  </si>
+  <si>
+    <t>Add Target Facility row</t>
+  </si>
+  <si>
+    <t>CN4</t>
+  </si>
+  <si>
+    <t>Add Section Name row</t>
+  </si>
+  <si>
+    <t>CN5</t>
+  </si>
+  <si>
+    <t>Add Systems to copy rows</t>
+  </si>
+  <si>
+    <t>CN6</t>
+  </si>
+  <si>
+    <t>Add Options cluster</t>
+  </si>
+  <si>
+    <t>CN7</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Photo Managerment</t>
+  </si>
+  <si>
+    <t>PM1</t>
+  </si>
+  <si>
+    <t>PM2</t>
+  </si>
+  <si>
+    <t>Add Pending cluster</t>
+  </si>
+  <si>
+    <t>PM3</t>
+  </si>
+  <si>
+    <t>Add Existing cluster</t>
+  </si>
+  <si>
+    <t>PM4</t>
+  </si>
+  <si>
+    <t>Add Details cluster</t>
+  </si>
+  <si>
+    <t>PM5</t>
+  </si>
+  <si>
+    <t>Add Title and Description data collection elements</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>Camera UI/Capture Photo</t>
+  </si>
+  <si>
+    <t>CP1</t>
+  </si>
+  <si>
+    <t>CP2</t>
+  </si>
+  <si>
+    <t>Add toolbar and buttons</t>
+  </si>
+  <si>
+    <t>CP3</t>
+  </si>
+  <si>
+    <t>Add Image area</t>
+  </si>
+  <si>
+    <t>CP4</t>
+  </si>
+  <si>
+    <t>Connect Cancel and OK buttons</t>
+  </si>
+  <si>
+    <t>CP5</t>
+  </si>
+  <si>
+    <t>Customize toolbar button appearance</t>
+  </si>
+  <si>
+    <t>Add System</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>AS1</t>
+  </si>
+  <si>
+    <t>AS2</t>
+  </si>
+  <si>
+    <t>Add label, combo and buttons to View</t>
+  </si>
+  <si>
+    <t>AS3</t>
+  </si>
+  <si>
+    <t>Connect OK and Cancel buttons to ViewModel</t>
+  </si>
+  <si>
+    <t>AS4</t>
+  </si>
+  <si>
+    <t>Connect Shell buttons to show the View</t>
+  </si>
+  <si>
+    <t>CP6</t>
+  </si>
+  <si>
+    <t>PM6</t>
+  </si>
+  <si>
+    <t>CN8</t>
+  </si>
+  <si>
+    <t>CC8</t>
+  </si>
+  <si>
+    <t>CI5</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Add New Component</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t>AC3</t>
+  </si>
+  <si>
+    <t>AC4</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,6 +3035,514 @@
         <v>43537</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E150" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E162" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B171" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B182" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E183" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B190" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E192" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E193" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B198" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E199" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B205" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update to tasks files.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54662C88-4965-4E6E-995D-2BE97761CAB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565DFBBD-791D-4F3F-8E2B-2038774A0BBE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="17310" windowWidth="21840" windowHeight="13770" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="24675" yWindow="4680" windowWidth="23205" windowHeight="23535" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="381">
   <si>
     <t>ID</t>
   </si>
@@ -965,9 +965,6 @@
     <t>CC</t>
   </si>
   <si>
-    <t>Copy Commentary</t>
-  </si>
-  <si>
     <t>CC1</t>
   </si>
   <si>
@@ -1182,6 +1179,18 @@
   </si>
   <si>
     <t>AC4</t>
+  </si>
+  <si>
+    <t>Copy Comment</t>
+  </si>
+  <si>
+    <t>CM5</t>
+  </si>
+  <si>
+    <t>Ask G to clarify, what launches the Comment Popup?</t>
+  </si>
+  <si>
+    <t>Connect Inspection's 'Inspection Comment' button to launch  popup.</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:E210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,37 +3093,34 @@
         <v>302</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>298</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E155" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>7</v>
@@ -3125,61 +3131,67 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C162" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E162" s="5">
-        <v>43555</v>
+        <v>377</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E163" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>309</v>
@@ -3187,212 +3199,206 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>370</v>
+        <v>316</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>324</v>
+      <c r="B172" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E172" s="5">
-        <v>43555</v>
+        <v>318</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>326</v>
+        <v>300</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B182" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B183" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C183" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D183" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E183" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>340</v>
+        <v>300</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E184" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B190" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B191" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C191" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D191" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E191" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>351</v>
+        <v>300</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>7</v>
@@ -3403,10 +3409,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>7</v>
@@ -3417,56 +3423,56 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E194" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="C196" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B198" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C198" s="2" t="s">
+      <c r="C197" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B199" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>360</v>
-      </c>
       <c r="C199" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E199" s="5">
-        <v>43555</v>
+        <v>357</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>362</v>
+        <v>300</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>7</v>
@@ -3477,48 +3483,48 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C202" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B205" s="1" t="s">
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B206" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E206" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>362</v>
+        <v>300</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>7</v>
@@ -3529,18 +3535,32 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E208" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked various View controls. Added a class to encapsulate property change notification that can be used as a base for models that need to broadcast changes.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E730C7D1-86C3-4C2D-8F61-B96F8FD73B45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C5256-8B31-46B2-A3BE-8EBA26B8289B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33840" yWindow="4140" windowWidth="23205" windowHeight="23535" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="31635" yWindow="15810" windowWidth="23205" windowHeight="16020" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="509">
   <si>
     <t>ID</t>
   </si>
@@ -1309,21 +1309,12 @@
     <t>Add Cancel Edit, Delete Detail, Add Detail and Copy Detail image buttons</t>
   </si>
   <si>
-    <t>ID21</t>
-  </si>
-  <si>
     <t>Relocate ID20's buttons so that all are on the same row</t>
   </si>
   <si>
     <t>Inventory Details</t>
   </si>
   <si>
-    <t>ID22</t>
-  </si>
-  <si>
-    <t>Current Selection should be soft yellow, not gray</t>
-  </si>
-  <si>
     <t>Inventory Section</t>
   </si>
   <si>
@@ -1358,9 +1349,6 @@
   </si>
   <si>
     <t>IS29.FB</t>
-  </si>
-  <si>
-    <t>Put bottom four buttons all on a single row instead of two rows.</t>
   </si>
   <si>
     <t>IN</t>
@@ -1610,12 +1598,51 @@
   <si>
     <t>GD: If there is more than a single section (named N/A) then the user will be able to pick which section to view/edit. NO functionality in Mockup expected. That is for Prototype stage. So for Section, the CAN select from already-existing section names for the current facility OR type in a new Section anme. ComboBox needed. Please do note the Gree Arrow that is a button that the user can tap for quickly cycling through existing sections. In prototype we will suppres that arrow if tehere is only 1 section. The Ma/Equip category is a picklist only. No ability to type in text. FYI: Will present options given the current cComponent type. The Component Tye is also a pickly only. FYI: will present options given the mat/equp category selection in picklist aboce.</t>
   </si>
+  <si>
+    <t>IS30</t>
+  </si>
+  <si>
+    <t>Ask G: Need an image for 'down button'.</t>
+  </si>
+  <si>
+    <t>DOne</t>
+  </si>
+  <si>
+    <t>ID20.FB</t>
+  </si>
+  <si>
+    <t>Section Comment should be soft yellow, not gray</t>
+  </si>
+  <si>
+    <t>Detail Comment should be soft yellow, not gray</t>
+  </si>
+  <si>
+    <t>ID21.FB</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <r>
+      <t>Bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Width, Depth and Floor Height should be editable but are not.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1672,6 +1699,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1719,7 +1753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1737,9 +1771,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1753,6 +1784,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2067,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E286"/>
+  <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,7 +2299,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>88</v>
@@ -2278,10 +2313,10 @@
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2801,7 +2836,7 @@
       <c r="A81" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="8" t="s">
         <v>342</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -2843,312 +2878,397 @@
       <c r="A84" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="9" t="s">
         <v>349</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E84" s="5">
-        <v>43557</v>
-      </c>
+      <c r="E84" s="5"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C85" s="8"/>
+      <c r="A85" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E85" s="5"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+      <c r="D92" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="C94" s="2" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="D97" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="D98" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="D99" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="D100" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="D101" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C102" s="6" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="D103" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="D104" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="D105" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C106" s="6" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="D107" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C108" s="2" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="D108" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C109" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="D109" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C110" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="D110" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C111" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="D111" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="2" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="D112" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C113" s="2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="D113" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C114" s="2" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="D114" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C115" s="2" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="D115" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C116" s="2" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="D116" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C116" s="7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="7"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C119" s="7"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C120" s="7"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="5">
+        <v>43558</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="5">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>116</v>
       </c>
@@ -3159,20 +3279,23 @@
         <v>87</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>118</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,6 +3305,9 @@
       <c r="C129" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="D129" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
@@ -3190,6 +3316,9 @@
       <c r="C130" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="D130" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="131" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
@@ -3198,6 +3327,9 @@
       <c r="C131" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="D131" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="132" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
@@ -3206,6 +3338,9 @@
       <c r="C132" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="D132" s="2" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="133" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
@@ -3214,6 +3349,9 @@
       <c r="C133" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="D133" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="134" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
@@ -3222,6 +3360,9 @@
       <c r="C134" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="D134" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
@@ -3230,6 +3371,9 @@
       <c r="C135" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="D135" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
@@ -3238,6 +3382,9 @@
       <c r="C136" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="D136" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
@@ -3246,6 +3393,9 @@
       <c r="C137" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="D137" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="138" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
@@ -3254,6 +3404,9 @@
       <c r="C138" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="D138" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="139" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
@@ -3262,6 +3415,9 @@
       <c r="C139" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="D139" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
@@ -3270,6 +3426,9 @@
       <c r="C140" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="D140" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
@@ -3278,6 +3437,9 @@
       <c r="C141" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="D141" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
@@ -3286,6 +3448,9 @@
       <c r="C142" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="D142" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
@@ -3325,10 +3490,10 @@
     </row>
     <row r="146" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="E146" s="5"/>
     </row>
@@ -3350,80 +3515,92 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" s="5">
+        <v>43558</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E152" s="5">
+        <v>43558</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>431</v>
+        <v>504</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" s="5">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>432</v>
+      <c r="B157" s="1" t="s">
+        <v>426</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E157" s="5">
-        <v>43555</v>
+        <v>427</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>7</v>
@@ -3434,10 +3611,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>7</v>
@@ -3448,10 +3625,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>7</v>
@@ -3462,10 +3639,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>7</v>
@@ -3476,10 +3653,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>7</v>
@@ -3490,10 +3667,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>7</v>
@@ -3504,10 +3681,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>7</v>
@@ -3518,10 +3695,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>7</v>
@@ -3532,10 +3709,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>7</v>
@@ -3546,10 +3723,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>7</v>
@@ -3560,10 +3737,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>7</v>
@@ -3574,10 +3751,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>7</v>
@@ -3588,10 +3765,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>7</v>
@@ -3602,10 +3779,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>7</v>
@@ -3616,10 +3793,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>7</v>
@@ -3630,83 +3807,86 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>464</v>
+        <v>459</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C176" t="s">
-        <v>471</v>
+        <v>465</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="C177" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B181" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D180" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
+      <c r="D181" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C182" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>7</v>
@@ -3714,10 +3894,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>7</v>
@@ -3725,10 +3905,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>7</v>
@@ -3736,10 +3916,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>7</v>
@@ -3747,10 +3927,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>7</v>
@@ -3758,10 +3938,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>7</v>
@@ -3769,10 +3949,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>7</v>
@@ -3780,10 +3960,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>7</v>
@@ -3791,10 +3971,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>7</v>
@@ -3802,10 +3982,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>7</v>
@@ -3813,46 +3993,46 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C193" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B193" s="3"/>
-      <c r="C193" s="4" t="s">
+      <c r="B194" s="3"/>
+      <c r="C194" s="4" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>30</v>
+        <v>205</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>7</v>
+        <v>220</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>7</v>
@@ -3860,10 +4040,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>7</v>
@@ -3871,10 +4051,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>7</v>
@@ -3882,10 +4062,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>7</v>
@@ -3893,29 +4073,29 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>7</v>
@@ -3923,44 +4103,44 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C204" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D203" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="3" t="s">
+      <c r="D204" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B204" s="3"/>
-      <c r="C204" s="4" t="s">
+      <c r="B205" s="3"/>
+      <c r="C205" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D204" s="2" t="s">
+      <c r="D205" s="2" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>7</v>
@@ -3968,10 +4148,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>7</v>
@@ -3979,10 +4159,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>7</v>
@@ -3990,63 +4170,60 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="C210" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D209" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
+      <c r="D210" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C211" t="s">
         <v>166</v>
       </c>
-      <c r="D210" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E210" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="D211" s="2" t="s">
-        <v>212</v>
+        <v>7</v>
       </c>
       <c r="E211" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>7</v>
+        <v>212</v>
       </c>
       <c r="E212" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>7</v>
@@ -4057,10 +4234,10 @@
     </row>
     <row r="214" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>7</v>
@@ -4071,13 +4248,13 @@
     </row>
     <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>210</v>
+        <v>7</v>
       </c>
       <c r="E215" s="5">
         <v>43554</v>
@@ -4085,10 +4262,13 @@
     </row>
     <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>221</v>
+        <v>170</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="E216" s="5">
         <v>43554</v>
@@ -4096,13 +4276,10 @@
     </row>
     <row r="217" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E217" s="5">
         <v>43554</v>
@@ -4110,58 +4287,58 @@
     </row>
     <row r="218" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>7</v>
+        <v>212</v>
       </c>
       <c r="E218" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E219" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C220" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E219" s="5"/>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E220" s="5"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B221" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C221" s="7" t="s">
-        <v>476</v>
-      </c>
+      <c r="E221" s="5"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C222" s="7" t="s">
+      <c r="B222" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="D222" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E222" s="5">
-        <v>43555</v>
+      <c r="C222" s="2" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C223" s="7" t="s">
         <v>478</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>473</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>7</v>
@@ -4172,10 +4349,10 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="C224" s="7" t="s">
         <v>479</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>7</v>
@@ -4186,46 +4363,40 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C225" s="7" t="s">
         <v>480</v>
       </c>
+      <c r="C225" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E225" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C226" s="7"/>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C227" s="7"/>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B228" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>487</v>
+      <c r="A226" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="C229" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="D229" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E229" s="5">
-        <v>43555</v>
+      <c r="B229" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C230" s="7" t="s">
-        <v>478</v>
+        <v>484</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>487</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>7</v>
@@ -4236,10 +4407,10 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>479</v>
+        <v>485</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>7</v>
@@ -4249,101 +4420,98 @@
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C232" s="7"/>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C233" s="7"/>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E234" s="5"/>
+      <c r="A232" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E232" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B235" s="1" t="s">
+      <c r="E235" s="5"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B236" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C235" s="2" t="s">
+      <c r="C236" s="2" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E236" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>294</v>
+        <v>255</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E237" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C242" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B243" s="1" t="s">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B244" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C243" s="2" t="s">
+      <c r="C244" s="2" t="s">
         <v>337</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>7</v>
@@ -4351,50 +4519,50 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="C247" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D246" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B247" s="3"/>
-      <c r="C247" s="4" t="s">
-        <v>354</v>
+      <c r="D247" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B249" s="3"/>
+      <c r="C249" s="4" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C249" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>7</v>
@@ -4402,10 +4570,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>7</v>
@@ -4413,10 +4581,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>7</v>
@@ -4424,10 +4592,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>7</v>
@@ -4435,10 +4603,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>7</v>
@@ -4446,52 +4614,52 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C255" s="2" t="s">
+      <c r="C256" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256" s="3" t="s">
+      <c r="D256" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B256" s="3"/>
-      <c r="C256" s="6" t="s">
+      <c r="B257" s="3"/>
+      <c r="C257" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="D256" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A257" s="3"/>
-      <c r="B257" s="3"/>
-      <c r="C257" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="D257" s="12"/>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D258" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D257" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="3"/>
+      <c r="B258" s="3"/>
+      <c r="C258" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="D258" s="11"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>7</v>
@@ -4499,10 +4667,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>7</v>
@@ -4510,10 +4678,10 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>7</v>
@@ -4521,10 +4689,10 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>7</v>
@@ -4532,24 +4700,21 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>178</v>
+        <v>84</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>356</v>
+        <v>85</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E263" s="5">
-        <v>43554</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>219</v>
+        <v>356</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>7</v>
@@ -4560,57 +4725,57 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>357</v>
+        <v>219</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="E265" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>224</v>
+        <v>357</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="E266" s="5">
+        <v>43554</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C267" s="6" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E268" s="5">
-        <v>43554</v>
+        <v>489</v>
+      </c>
+      <c r="C268" s="6" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>7</v>
@@ -4619,109 +4784,109 @@
         <v>43554</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E270" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C270" s="7" t="s">
+      <c r="C271" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D270" s="2" t="s">
+      <c r="D271" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C272" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D271" s="2" t="s">
+      <c r="D272" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E271" s="5">
+      <c r="E272" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
+    <row r="273" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C272" s="7" t="s">
+      <c r="C273" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A273" s="1" t="s">
+    <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C273" s="6" t="s">
+      <c r="C274" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="D273" s="2" t="s">
+      <c r="D274" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E273" s="5">
+      <c r="E274" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A274" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="C274" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E274" s="5"/>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>238</v>
+        <v>491</v>
+      </c>
+      <c r="C275" s="6" t="s">
+        <v>492</v>
       </c>
       <c r="E275" s="5"/>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>362</v>
+        <v>237</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>363</v>
+        <v>238</v>
       </c>
       <c r="E276" s="5"/>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E277" s="5"/>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>239</v>
+        <v>364</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D278" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E278" s="5">
-        <v>43555</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="E278" s="5"/>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>7</v>
@@ -4730,59 +4895,59 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B282" s="1" t="s">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E280" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B283" s="1" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A283" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C283" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D283" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E283" s="5">
-        <v>43554</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C284" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="E284" s="5">
-        <v>43555</v>
+        <v>43554</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C285" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>225</v>
       </c>
       <c r="E285" s="5">
-        <v>43537</v>
+        <v>43555</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C286" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>225</v>
@@ -4791,9 +4956,23 @@
         <v>43537</v>
       </c>
     </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C287" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E287" s="5">
+        <v>43537</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C257:D257"/>
+    <mergeCell ref="C258:D258"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Git says the file has changed.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C5256-8B31-46B2-A3BE-8EBA26B8289B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA971637-C098-489A-AA2B-735B5F505FE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31635" yWindow="15810" windowWidth="23205" windowHeight="16020" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="30225" yWindow="14715" windowWidth="23205" windowHeight="16020" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="514">
   <si>
     <t>ID</t>
   </si>
@@ -687,9 +687,6 @@
   </si>
   <si>
     <t>Addressed</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>L28.FB.1</t>
@@ -1637,12 +1634,30 @@
       <t>: Width, Depth and Floor Height should be editable but are not.</t>
     </r>
   </si>
+  <si>
+    <t>Last Activity</t>
+  </si>
+  <si>
+    <t>Fixe</t>
+  </si>
+  <si>
+    <t>S23.2.1</t>
+  </si>
+  <si>
+    <t>Not happy with color. Needs more work</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>Wireframe shows tabs as a series of different blue shades.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1699,13 +1714,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1753,7 +1761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1784,10 +1792,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2102,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E287"/>
+  <dimension ref="A1:E288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,23 +2134,23 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>213</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -2157,10 +2161,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -2171,34 +2175,34 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -2209,10 +2213,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
@@ -2223,18 +2227,18 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2242,7 +2246,7 @@
         <v>98</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2252,6 +2256,9 @@
       <c r="C16" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -2260,6 +2267,9 @@
       <c r="C17" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2268,6 +2278,9 @@
       <c r="C18" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2276,6 +2289,9 @@
       <c r="C19" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -2283,6 +2299,9 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2299,7 +2318,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>88</v>
@@ -2313,26 +2332,26 @@
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>7</v>
@@ -2343,74 +2362,110 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>263</v>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>266</v>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>268</v>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>270</v>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>272</v>
+      <c r="D33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>7</v>
@@ -2421,10 +2476,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>7</v>
@@ -2435,42 +2490,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>7</v>
@@ -2481,10 +2536,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>7</v>
@@ -2495,45 +2550,45 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>7</v>
@@ -2544,74 +2599,74 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>7</v>
@@ -2622,10 +2677,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>7</v>
@@ -2636,10 +2691,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>7</v>
@@ -2650,26 +2705,26 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,7 +2794,7 @@
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>7</v>
@@ -2781,7 +2836,7 @@
         <v>179</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>7</v>
@@ -2795,7 +2850,7 @@
         <v>188</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>7</v>
@@ -2809,7 +2864,7 @@
         <v>189</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>7</v>
@@ -2823,7 +2878,7 @@
         <v>190</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>7</v>
@@ -2834,10 +2889,10 @@
     </row>
     <row r="81" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>7</v>
@@ -2848,10 +2903,10 @@
     </row>
     <row r="82" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>7</v>
@@ -2862,10 +2917,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>7</v>
@@ -2876,27 +2931,29 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>349</v>
-      </c>
       <c r="D84" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E84" s="5"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C85" t="s">
         <v>507</v>
       </c>
-      <c r="C85" s="13" t="s">
-        <v>508</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E85" s="5"/>
+        <v>509</v>
+      </c>
+      <c r="E85" s="5">
+        <v>43558</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
@@ -2906,7 +2963,7 @@
         <v>185</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2935,10 +2992,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>7</v>
@@ -2946,18 +3003,18 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>7</v>
@@ -2965,10 +3022,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>7</v>
@@ -2976,10 +3033,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>7</v>
@@ -2987,10 +3044,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>7</v>
@@ -2998,10 +3055,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>7</v>
@@ -3009,10 +3066,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>7</v>
@@ -3020,10 +3077,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>7</v>
@@ -3031,18 +3088,18 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C102" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>7</v>
@@ -3050,10 +3107,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>7</v>
@@ -3061,10 +3118,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>7</v>
@@ -3072,18 +3129,18 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>7</v>
@@ -3091,10 +3148,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>7</v>
@@ -3102,10 +3159,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>7</v>
@@ -3113,10 +3170,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>399</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>7</v>
@@ -3124,10 +3181,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>7</v>
@@ -3135,10 +3192,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>403</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>7</v>
@@ -3146,10 +3203,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>7</v>
@@ -3157,10 +3214,10 @@
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>7</v>
@@ -3168,10 +3225,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>7</v>
@@ -3179,10 +3236,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>7</v>
@@ -3190,10 +3247,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>7</v>
@@ -3204,10 +3261,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>7</v>
@@ -3221,7 +3278,7 @@
         <v>108</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3281,10 +3338,10 @@
     </row>
     <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C127" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,7 +3396,7 @@
         <v>122</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3482,7 +3539,7 @@
         <v>196</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E145" s="5">
         <v>43555</v>
@@ -3490,10 +3547,10 @@
     </row>
     <row r="146" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="E146" s="5"/>
     </row>
@@ -3515,10 +3572,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>7</v>
@@ -3529,26 +3586,26 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C151" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>7</v>
@@ -3559,18 +3616,18 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>7</v>
@@ -3581,26 +3638,26 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C155" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="C155" s="6" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>7</v>
@@ -3611,10 +3668,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C159" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>7</v>
@@ -3625,10 +3682,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>7</v>
@@ -3639,10 +3696,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>7</v>
@@ -3653,10 +3710,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C162" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>7</v>
@@ -3667,10 +3724,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>7</v>
@@ -3681,10 +3738,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>7</v>
@@ -3695,10 +3752,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>7</v>
@@ -3709,10 +3766,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>7</v>
@@ -3723,10 +3780,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>7</v>
@@ -3737,10 +3794,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>449</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>7</v>
@@ -3751,10 +3808,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C169" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>7</v>
@@ -3765,10 +3822,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>7</v>
@@ -3779,10 +3836,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>455</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>7</v>
@@ -3793,10 +3850,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>7</v>
@@ -3807,10 +3864,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>7</v>
@@ -3821,50 +3878,50 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C177" t="s">
         <v>466</v>
-      </c>
-      <c r="C177" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C178" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C179" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,7 +4081,7 @@
         <v>205</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4220,10 +4277,10 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C213" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C213" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>7</v>
@@ -4279,7 +4336,7 @@
         <v>209</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E217" s="5">
         <v>43554</v>
@@ -4304,7 +4361,7 @@
         <v>211</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>7</v>
@@ -4327,18 +4384,18 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B222" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>7</v>
@@ -4349,10 +4406,10 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>7</v>
@@ -4363,10 +4420,10 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>7</v>
@@ -4377,26 +4434,26 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B229" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C229" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>7</v>
@@ -4407,10 +4464,10 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>7</v>
@@ -4421,10 +4478,10 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>7</v>
@@ -4438,18 +4495,18 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B236" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C236" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>7</v>
@@ -4460,42 +4517,42 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C238" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C239" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C240" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C241" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,7 +4560,7 @@
         <v>56</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -4545,7 +4602,7 @@
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -4554,7 +4611,7 @@
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -4640,7 +4697,7 @@
       </c>
       <c r="B257" s="3"/>
       <c r="C257" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>7</v>
@@ -4650,7 +4707,7 @@
       <c r="A258" s="3"/>
       <c r="B258" s="3"/>
       <c r="C258" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D258" s="11"/>
     </row>
@@ -4714,7 +4771,7 @@
         <v>178</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>7</v>
@@ -4725,10 +4782,10 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>7</v>
@@ -4742,10 +4799,10 @@
         <v>180</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E266" s="5">
         <v>43554</v>
@@ -4753,21 +4810,21 @@
     </row>
     <row r="267" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C267" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C267" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="D267" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="268" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C268" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="C268" s="6" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -4775,7 +4832,7 @@
         <v>181</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>7</v>
@@ -4789,7 +4846,7 @@
         <v>182</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>7</v>
@@ -4803,21 +4860,21 @@
         <v>183</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C272" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C272" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="D272" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E272" s="5">
         <v>43554</v>
@@ -4828,18 +4885,18 @@
         <v>184</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C274" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E274" s="5">
         <v>43554</v>
@@ -4847,60 +4904,65 @@
     </row>
     <row r="275" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C275" s="6" t="s">
         <v>491</v>
-      </c>
-      <c r="C275" s="6" t="s">
-        <v>492</v>
       </c>
       <c r="E275" s="5"/>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C276" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C276" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="E276" s="5"/>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C277" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C277" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="E277" s="5"/>
+      <c r="D277" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E277" s="5">
+        <v>43559</v>
+      </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C278" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="E278" s="5"/>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D279" s="2" t="s">
-        <v>7</v>
+        <v>510</v>
+      </c>
+      <c r="C279" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="D279" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="E279" s="5">
-        <v>43555</v>
+        <v>43559</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>7</v>
@@ -4909,64 +4971,92 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B283" s="1" t="s">
-        <v>228</v>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E281" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C282" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="D282" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E282" s="5">
+        <v>43559</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A284" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C284" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D284" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E284" s="5">
-        <v>43554</v>
+      <c r="B284" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C285" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C285" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="D285" s="2" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="E285" s="5">
-        <v>43555</v>
+        <v>43554</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C286" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E286" s="5">
-        <v>43537</v>
+        <v>43555</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C287" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E287" s="5">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C288" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E288" s="5">
         <v>43537</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the task list. Tweaked Inspection View per task list.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E750A22D-6414-4ABA-B569-2D30F97EFF06}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E214AC-BD09-4122-A58C-277586E32AF9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="23205" windowHeight="12180" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="32625" yWindow="210" windowWidth="23205" windowHeight="16020" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="632">
   <si>
     <t>ID</t>
   </si>
@@ -1466,9 +1466,6 @@
   </si>
   <si>
     <t>IN18.FB</t>
-  </si>
-  <si>
-    <t>Change text on grid buttons to agree with their captions</t>
   </si>
   <si>
     <t>IN19.FB</t>
@@ -1689,9 +1686,6 @@
     <t>IS34</t>
   </si>
   <si>
-    <t>Year Installed edit should be Yellow if Extimated clicked</t>
-  </si>
-  <si>
     <t>IS35</t>
   </si>
   <si>
@@ -1945,6 +1939,72 @@
   </si>
   <si>
     <t>Ask G: What is 'auto stamping'?</t>
+  </si>
+  <si>
+    <t>ID33</t>
+  </si>
+  <si>
+    <t>Ask G: How should a click on 'Cancel Edit' work?</t>
+  </si>
+  <si>
+    <t>ID34</t>
+  </si>
+  <si>
+    <t>Ask G: How should a click on 'Delete Detail' work?</t>
+  </si>
+  <si>
+    <t>ID35</t>
+  </si>
+  <si>
+    <t>Ask G: How should Add Detail work?</t>
+  </si>
+  <si>
+    <t>ID36</t>
+  </si>
+  <si>
+    <t>Ask G: How should Copy Detail work?</t>
+  </si>
+  <si>
+    <t>Year Installed edit should be Yellow if Estimated clicked</t>
+  </si>
+  <si>
+    <t>IS43</t>
+  </si>
+  <si>
+    <t>Year P/C and P/C Type should be in a Gray background box</t>
+  </si>
+  <si>
+    <t>IS44</t>
+  </si>
+  <si>
+    <t>Hook Cancel Edit button click to an action</t>
+  </si>
+  <si>
+    <t>IS45</t>
+  </si>
+  <si>
+    <t>Hook Delete Section to an action</t>
+  </si>
+  <si>
+    <t>IS46</t>
+  </si>
+  <si>
+    <t>Hook Add Section to an action</t>
+  </si>
+  <si>
+    <t>IS47</t>
+  </si>
+  <si>
+    <t>Ask G: What should Cancel Edit, Delete Section and Add section do?</t>
+  </si>
+  <si>
+    <t>Change text color off grid buttons to agree with their captions</t>
+  </si>
+  <si>
+    <t>IN30</t>
+  </si>
+  <si>
+    <t>Make the bottom buttons the same as other Views and compatible with Wireframe</t>
   </si>
 </sst>
 </file>
@@ -2061,7 +2121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2085,19 +2145,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2105,6 +2156,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2421,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E357"/>
+  <dimension ref="A1:E367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2616,7 +2673,7 @@
         <v>103</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2633,7 +2690,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>88</v>
@@ -2647,10 +2704,10 @@
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2879,7 +2936,7 @@
         <v>333</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2892,34 +2949,34 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>607</v>
+        <v>604</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>609</v>
+        <v>606</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>611</v>
+        <v>608</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3280,7 +3337,7 @@
       <c r="A92" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C92" s="10" t="s">
         <v>348</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -3290,13 +3347,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C93" t="s">
         <v>502</v>
       </c>
-      <c r="C93" t="s">
-        <v>503</v>
-      </c>
       <c r="D93" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E93" s="5">
         <v>43558</v>
@@ -3323,10 +3380,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3358,10 +3415,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>7</v>
@@ -3422,7 +3479,10 @@
         <v>375</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>224</v>
+        <v>7</v>
+      </c>
+      <c r="E110" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,7 +3522,7 @@
       <c r="A114" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="9" t="s">
         <v>384</v>
       </c>
     </row>
@@ -3503,7 +3563,7 @@
       <c r="A118" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C118" s="9" t="s">
         <v>384</v>
       </c>
     </row>
@@ -3619,7 +3679,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>411</v>
@@ -3633,10 +3693,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>7</v>
@@ -3647,7 +3707,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>414</v>
@@ -3661,29 +3721,35 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>415</v>
       </c>
+      <c r="D132" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" s="5">
+        <v>43562</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="C133" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>416</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>513</v>
+        <v>516</v>
+      </c>
+      <c r="C134" s="9" t="s">
+        <v>512</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>224</v>
@@ -3691,230 +3757,260 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C135" s="16" t="s">
-        <v>544</v>
+        <v>541</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E137" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E139" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E140" s="5">
+        <v>43561</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E141" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" s="5">
+        <v>43561</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" s="5">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>413</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C153" s="6" t="s">
+      <c r="C157" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D153" s="2" t="s">
+      <c r="D157" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
+    <row r="158" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C158" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="C154" s="6" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+    </row>
+    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D155" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+      <c r="D159" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D156" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+      <c r="D160" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D157" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+      <c r="D161" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>7</v>
@@ -3922,43 +4018,43 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>7</v>
+        <v>496</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>7</v>
@@ -3966,10 +4062,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>7</v>
@@ -3977,10 +4073,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>7</v>
@@ -3988,412 +4084,431 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E170" s="5">
-        <v>43555</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E172" s="5">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>494</v>
+        <v>147</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E173" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="174" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E174" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>417</v>
+        <v>195</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>418</v>
+        <v>196</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>7</v>
+        <v>242</v>
       </c>
       <c r="E176" s="5">
-        <v>43558</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>419</v>
+        <v>493</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+      <c r="E177" s="5"/>
+    </row>
+    <row r="178" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>421</v>
+        <v>197</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>499</v>
+        <v>198</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E178" s="5">
-        <v>43557</v>
+        <v>43562</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="C179" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>224</v>
+        <v>199</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C180" s="14" t="s">
-        <v>520</v>
+        <v>417</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" s="5">
+        <v>43558</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C181" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E181" s="5">
-        <v>43557</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C182" s="15" t="s">
-        <v>524</v>
+        <v>421</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>498</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
       <c r="E182" s="5">
         <v>43557</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>525</v>
-      </c>
-      <c r="B183"/>
-      <c r="C183" t="s">
-        <v>526</v>
-      </c>
-      <c r="D183"/>
+      <c r="A183" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E183" s="5">
+        <v>43562</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B184"/>
-      <c r="C184" s="12" t="s">
-        <v>528</v>
+        <v>518</v>
+      </c>
+      <c r="C184" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
       <c r="E184" s="5">
-        <v>43561</v>
+        <v>43562</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="B185"/>
-      <c r="C185" t="s">
-        <v>530</v>
-      </c>
-      <c r="D185"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E185" s="5">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="B186"/>
-      <c r="C186" t="s">
-        <v>532</v>
-      </c>
-      <c r="D186"/>
+        <v>522</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>523</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E186" s="5">
+        <v>43557</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>533</v>
+      <c r="A187" t="s">
+        <v>524</v>
       </c>
       <c r="B187"/>
       <c r="C187" t="s">
-        <v>534</v>
-      </c>
-      <c r="D187"/>
+        <v>618</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" s="5">
+        <v>43562</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="B188"/>
-      <c r="C188" t="s">
-        <v>536</v>
-      </c>
-      <c r="D188"/>
+      <c r="C188" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E188" s="5">
+        <v>43561</v>
+      </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="B189"/>
       <c r="C189" t="s">
-        <v>538</v>
-      </c>
-      <c r="D189"/>
+        <v>528</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E189" s="5">
+        <v>43561</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="B190"/>
       <c r="C190" t="s">
-        <v>540</v>
-      </c>
-      <c r="D190"/>
+        <v>530</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E190" s="5">
+        <v>43562</v>
+      </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="B191"/>
       <c r="C191" t="s">
-        <v>542</v>
-      </c>
-      <c r="D191"/>
+        <v>532</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="5">
+        <v>43561</v>
+      </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C192"/>
-      <c r="E192" s="5"/>
+      <c r="A192" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B192"/>
+      <c r="C192" t="s">
+        <v>534</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E192" s="5">
+        <v>43562</v>
+      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B193" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>423</v>
+      <c r="A193" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B193"/>
+      <c r="C193" t="s">
+        <v>536</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E193" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>425</v>
+        <v>537</v>
+      </c>
+      <c r="B194"/>
+      <c r="C194" t="s">
+        <v>538</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E194" s="5">
-        <v>43555</v>
+        <v>43562</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>427</v>
+        <v>539</v>
+      </c>
+      <c r="B195"/>
+      <c r="C195" t="s">
+        <v>540</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E195" s="5">
-        <v>43555</v>
+        <v>43562</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>429</v>
+        <v>619</v>
+      </c>
+      <c r="B196"/>
+      <c r="C196" t="s">
+        <v>620</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E196" s="5">
-        <v>43555</v>
+        <v>43562</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E197" s="5">
-        <v>43555</v>
-      </c>
+        <v>621</v>
+      </c>
+      <c r="B197"/>
+      <c r="C197" t="s">
+        <v>622</v>
+      </c>
+      <c r="D197"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E198" s="5">
-        <v>43555</v>
-      </c>
+        <v>623</v>
+      </c>
+      <c r="B198"/>
+      <c r="C198" t="s">
+        <v>624</v>
+      </c>
+      <c r="D198"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E199" s="5">
-        <v>43555</v>
-      </c>
+        <v>625</v>
+      </c>
+      <c r="B199"/>
+      <c r="C199" t="s">
+        <v>626</v>
+      </c>
+      <c r="D199"/>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E200" s="5">
-        <v>43555</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="B200"/>
+      <c r="C200" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="D200"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E201" s="5">
-        <v>43555</v>
-      </c>
+      <c r="B201"/>
+      <c r="C201"/>
+      <c r="D201"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E202" s="5">
-        <v>43555</v>
-      </c>
+      <c r="C202"/>
+      <c r="E202" s="5"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>442</v>
+      <c r="B203" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E203" s="5">
-        <v>43555</v>
+        <v>423</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>7</v>
@@ -4404,10 +4519,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>7</v>
@@ -4418,10 +4533,10 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>7</v>
@@ -4432,10 +4547,10 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>451</v>
+        <v>431</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>7</v>
@@ -4446,10 +4561,10 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>452</v>
+        <v>432</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>7</v>
@@ -4460,10 +4575,10 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>455</v>
+        <v>435</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>7</v>
@@ -4474,262 +4589,363 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>456</v>
+        <v>439</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E210" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>458</v>
+        <v>438</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E211" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>459</v>
+        <v>441</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E212" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C213" t="s">
-        <v>463</v>
+        <v>442</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E213" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E214" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E215" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="C216" s="11" t="s">
-        <v>564</v>
+        <v>448</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E216" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>565</v>
+        <v>450</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>566</v>
+        <v>451</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E217" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>567</v>
+        <v>452</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>568</v>
+        <v>453</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E218" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>569</v>
+        <v>454</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>570</v>
+        <v>455</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E219" s="5">
+        <v>43555</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>571</v>
+        <v>457</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>572</v>
+        <v>456</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E220" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>573</v>
+        <v>460</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>574</v>
+        <v>458</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>575</v>
+        <v>461</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>576</v>
+        <v>459</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>578</v>
+        <v>462</v>
+      </c>
+      <c r="C223" t="s">
+        <v>463</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E224" s="5">
+        <v>43561</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E227" s="5">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E228" s="5">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E229" s="5">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E230" s="5">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E234" s="5">
+        <v>43560</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C235" s="2" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D234" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D235" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" s="5">
+        <v>43561</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>20</v>
+        <v>630</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>10</v>
+        <v>631</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>7</v>
+      <c r="E236" s="5">
+        <v>43562</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>7</v>
@@ -4737,35 +4953,43 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B246" s="3"/>
-      <c r="C246" s="4" t="s">
-        <v>148</v>
+      <c r="A246" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>205</v>
+        <v>21</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>219</v>
+        <v>11</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>19</v>
+        <v>207</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>7</v>
@@ -4773,10 +4997,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>7</v>
@@ -4784,10 +5008,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>7</v>
@@ -4795,10 +5019,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>7</v>
@@ -4806,10 +5030,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>7</v>
@@ -4817,18 +5041,21 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>7</v>
@@ -4836,1011 +5063,1110 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B256" s="3"/>
+      <c r="C256" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C255" s="2" t="s">
+      <c r="C265" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
+      <c r="D265" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C256" s="2" t="s">
+      <c r="C266" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D256" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A257" s="3" t="s">
+      <c r="D266" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B257" s="3"/>
-      <c r="C257" s="4" t="s">
+      <c r="B267" s="3"/>
+      <c r="C267" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D257" s="2" t="s">
+      <c r="D267" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C258" s="2" t="s">
+      <c r="C268" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D258" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
+      <c r="D268" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C259" s="2" t="s">
+      <c r="C269" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D259" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
+      <c r="D269" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C260" s="2" t="s">
+      <c r="C270" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D260" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
+      <c r="D270" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C261" s="2" t="s">
+      <c r="C271" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D261" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
+      <c r="D271" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C272" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D262" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
+      <c r="D272" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C273" t="s">
         <v>166</v>
       </c>
-      <c r="D263" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E263" s="5">
+      <c r="D273" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E273" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
+    <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C274" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D264" s="2" t="s">
+      <c r="D274" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E264" s="5">
+      <c r="E274" s="5">
         <v>43554</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D265" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E265" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D266" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E266" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E267" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="268" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E268" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="269" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E269" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="270" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C270" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D270" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E270" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D271" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E271" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E272" s="5"/>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E273" s="5"/>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B274" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E275" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E276" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E277" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E278" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E279" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E280" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E281" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E282" s="5"/>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E283" s="5"/>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B284" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E285" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C275" s="2" t="s">
+      <c r="C286" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D275" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E275" s="5">
+      <c r="D286" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E286" s="5">
         <v>43555</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C276" s="2" t="s">
+      <c r="C287" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="D276" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E276" s="5">
+      <c r="D287" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E287" s="5">
         <v>43555</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C277" s="2" t="s">
+      <c r="C288" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="D277" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E277" s="5">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A278" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A279" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A280" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="C280" s="2" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A281" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="C281" s="2" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B288" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>480</v>
+        <v>596</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D289" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E289" s="5">
-        <v>43555</v>
+        <v>597</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>481</v>
+        <v>598</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="D290" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E290" s="5">
-        <v>43555</v>
+        <v>599</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>482</v>
+        <v>600</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D291" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E291" s="5">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="C293" s="11" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="C296" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="1" t="s">
-        <v>594</v>
+      <c r="B298" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="E298" s="5"/>
+        <v>478</v>
+      </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>596</v>
+        <v>479</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="E299" s="5"/>
+        <v>482</v>
+      </c>
+      <c r="D299" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E299" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E300" s="5"/>
+      <c r="A300" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D300" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E300" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E301" s="5"/>
+      <c r="A301" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E301" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E302" s="5"/>
+      <c r="A302" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E303" s="5"/>
+      <c r="A303" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C303" s="9" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E304" s="5"/>
+      <c r="A304" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B305" s="1" t="s">
-        <v>289</v>
+      <c r="A305" s="1" t="s">
+        <v>585</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>290</v>
+        <v>588</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>291</v>
+        <v>587</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D306" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E306" s="5">
-        <v>43555</v>
+        <v>586</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>292</v>
+        <v>590</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>293</v>
+        <v>591</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>294</v>
+        <v>592</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>593</v>
+      </c>
+      <c r="E308" s="5"/>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>296</v>
+        <v>594</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>297</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="E309" s="5"/>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A310" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C310" s="2" t="s">
-        <v>299</v>
-      </c>
+      <c r="E310" s="5"/>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A311" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C311" s="2" t="s">
-        <v>319</v>
-      </c>
+      <c r="E311" s="5"/>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E312" s="5"/>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B313" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>336</v>
-      </c>
+      <c r="E313" s="5"/>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D314" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="E314" s="5"/>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="1" t="s">
-        <v>60</v>
+      <c r="B315" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D315" s="2" t="s">
-        <v>7</v>
+        <v>290</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>61</v>
+        <v>291</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>59</v>
+        <v>254</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E316" s="5">
+        <v>43555</v>
+      </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B317" s="3"/>
-      <c r="C317" s="4" t="s">
-        <v>353</v>
+      <c r="A317" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B318" s="3"/>
-      <c r="C318" s="4" t="s">
-        <v>354</v>
+      <c r="A318" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>62</v>
+        <v>296</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D319" s="2" t="s">
-        <v>7</v>
+        <v>297</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B323" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B327" s="3"/>
+      <c r="C327" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B328" s="3"/>
+      <c r="C328" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D329" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C320" s="2" t="s">
+      <c r="C330" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D320" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="1" t="s">
+      <c r="D330" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="C331" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D321" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A322" s="1" t="s">
+      <c r="D331" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="C332" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D322" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A323" s="1" t="s">
+      <c r="D332" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C323" s="2" t="s">
+      <c r="C333" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D323" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="1" t="s">
+      <c r="D333" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C324" s="2" t="s">
+      <c r="C334" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D324" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A325" s="1" t="s">
+      <c r="D334" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C325" s="2" t="s">
+      <c r="C335" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D325" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="326" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A326" s="3" t="s">
+      <c r="D335" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A336" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B326" s="3"/>
-      <c r="C326" s="6" t="s">
+      <c r="B336" s="3"/>
+      <c r="C336" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="D326" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="327" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A327" s="3"/>
-      <c r="B327" s="3"/>
-      <c r="C327" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="D327" s="10"/>
-    </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A328" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C328" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D328" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C329" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D329" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A330" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C330" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D330" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A331" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C331" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D331" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C332" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D332" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A333" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C333" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D333" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E333" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A334" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C334" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D334" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E334" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A335" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C335" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D335" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E335" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="336" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A336" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C336" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="D336" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A337" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C337" s="6" t="s">
-        <v>486</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A337" s="3"/>
+      <c r="B337" s="3"/>
+      <c r="C337" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="D337" s="15"/>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>357</v>
+        <v>77</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E338" s="5">
-        <v>43554</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>182</v>
+        <v>78</v>
       </c>
       <c r="C339" s="2" t="s">
-        <v>358</v>
+        <v>79</v>
       </c>
       <c r="D339" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E339" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="340" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="C340" s="2" t="s">
-        <v>359</v>
+        <v>81</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>216</v>
+        <v>82</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E341" s="5">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="342" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>184</v>
+        <v>84</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="343" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C343" s="6" t="s">
-        <v>338</v>
+        <v>178</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="E343" s="5">
         <v>43554</v>
       </c>
     </row>
-    <row r="344" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="C344" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="E344" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E344" s="5">
+        <v>43554</v>
+      </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>236</v>
+        <v>180</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E345" s="5"/>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E345" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>361</v>
+        <v>222</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>362</v>
+        <v>223</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E346" s="5">
-        <v>43559</v>
-      </c>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C347" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="E347" s="5"/>
+        <v>484</v>
+      </c>
+      <c r="C347" s="6" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C348" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="D348" s="6" t="s">
-        <v>225</v>
+        <v>181</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D348" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E348" s="5">
-        <v>43559</v>
+        <v>43554</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>238</v>
+        <v>182</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>239</v>
+        <v>358</v>
       </c>
       <c r="D349" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E349" s="5">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>241</v>
+        <v>359</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E350" s="5">
-        <v>43555</v>
+        <v>224</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C351" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="D351" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D351" s="2" t="s">
         <v>225</v>
       </c>
       <c r="E351" s="5">
-        <v>43559</v>
-      </c>
-    </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B353" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C353" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E353" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C354" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D354" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E354" s="5">
-        <v>43554</v>
-      </c>
+        <v>486</v>
+      </c>
+      <c r="C354" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="E354" s="5"/>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C355" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D355" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E355" s="5">
-        <v>43555</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E355" s="5"/>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C356" s="11" t="s">
-        <v>234</v>
+        <v>361</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
       <c r="E356" s="5">
-        <v>43555</v>
+        <v>43559</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E357" s="5"/>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C358" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="D358" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E358" s="5">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E359" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E360" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C361" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="D361" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E361" s="5">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B363" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E364" s="5">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C365" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E365" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C366" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E366" s="5">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C357" s="11" t="s">
+      <c r="C367" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D357" s="2" t="s">
+      <c r="D367" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E357" s="5">
+      <c r="E367" s="5">
         <v>43555</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C327:D327"/>
+    <mergeCell ref="C337:D337"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Bluebeam file open.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill_\source\Projects\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB7E43-4D2A-4665-99E9-CF702D04BC6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CA1D9F-7628-4761-9C44-211C41370E1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="659">
   <si>
     <t>ID</t>
   </si>
@@ -2051,9 +2057,6 @@
     <t>IS22.1</t>
   </si>
   <si>
-    <t>Done, needs content, in process</t>
-  </si>
-  <si>
     <t>Fixed.</t>
   </si>
   <si>
@@ -2074,12 +2077,33 @@
   <si>
     <t>Do we need to make custom "Message Box" for thoses single-line questions? It's related to that whole "fat-fingers" style. There are some Material-Design concepts we could use. 
 Here are some examples</t>
+  </si>
+  <si>
+    <t>Needs content, in process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Tasks: </t>
+  </si>
+  <si>
+    <t>Done:</t>
+  </si>
+  <si>
+    <t>In Process:</t>
+  </si>
+  <si>
+    <t>Of the remaining tasks:</t>
+  </si>
+  <si>
+    <t>Pending:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2209,7 +2233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2273,16 +2297,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2296,7 +2356,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2320,44 +2379,82 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="2" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2669,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:E375"/>
+  <dimension ref="A1:E382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="P98" sqref="P98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2680,7 +2777,7 @@
     <col min="1" max="2" width="8.7265625" style="1"/>
     <col min="3" max="3" width="84.81640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="32" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2700,41 +2797,32 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E2" s="1"/>
-    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>649</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="16" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>650</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14" t="s">
-        <v>653</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="23" t="s">
-        <v>652</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E6" s="1"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
@@ -2754,7 +2842,7 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2768,7 +2856,7 @@
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2779,8 +2867,11 @@
       <c r="C11" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>7</v>
+      <c r="D11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="35">
+        <v>43563</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2790,8 +2881,11 @@
       <c r="C12" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>7</v>
+      <c r="D12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="35">
+        <v>43563</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2812,7 +2906,7 @@
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2826,7 +2920,7 @@
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2837,6 +2931,12 @@
       <c r="C17" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="D17" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="35">
+        <v>43563</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
@@ -2845,8 +2945,11 @@
       <c r="C18" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>647</v>
+      <c r="D18" s="21" t="s">
+        <v>646</v>
+      </c>
+      <c r="E18" s="35">
+        <v>43563</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2934,7 +3037,7 @@
       <c r="D28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2945,8 +3048,11 @@
       <c r="C29" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>225</v>
+      <c r="D29" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="35">
+        <v>43563</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2967,7 +3073,7 @@
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2981,7 +3087,7 @@
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -2995,7 +3101,7 @@
       <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3009,7 +3115,7 @@
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3023,7 +3129,7 @@
       <c r="D36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3037,7 +3143,7 @@
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3051,7 +3157,7 @@
       <c r="D38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3064,11 +3170,11 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="13" t="s">
         <v>632</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="14" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="16" t="s">
         <v>633</v>
       </c>
     </row>
@@ -3090,7 +3196,7 @@
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3104,7 +3210,7 @@
       <c r="D44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3125,11 +3231,11 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="13" t="s">
         <v>634</v>
       </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="14" t="s">
+      <c r="B47" s="13"/>
+      <c r="C47" s="16" t="s">
         <v>635</v>
       </c>
     </row>
@@ -3140,19 +3246,22 @@
       <c r="C48" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>7</v>
+      <c r="D48" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="35">
+        <v>43563</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="14" t="s">
         <v>636</v>
       </c>
-      <c r="B49" s="17"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="18" t="s">
         <v>637</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="22" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3174,7 +3283,7 @@
       <c r="D52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3188,7 +3297,7 @@
       <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3218,7 +3327,7 @@
       <c r="C56" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3229,7 +3338,7 @@
       <c r="C57" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="22" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3237,7 +3346,7 @@
       <c r="A58" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="8" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3245,7 +3354,7 @@
       <c r="A59" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>607</v>
       </c>
     </row>
@@ -3253,7 +3362,7 @@
       <c r="A60" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>609</v>
       </c>
     </row>
@@ -3275,7 +3384,7 @@
       <c r="D63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3286,8 +3395,8 @@
       <c r="C64" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D64" s="19" t="s">
-        <v>646</v>
+      <c r="D64" s="22" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -3297,8 +3406,8 @@
       <c r="C65" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D65" s="19" t="s">
-        <v>646</v>
+      <c r="D65" s="22" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -3308,8 +3417,8 @@
       <c r="C66" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D66" s="19" t="s">
-        <v>646</v>
+      <c r="D66" s="22" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -3319,8 +3428,8 @@
       <c r="C67" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D67" s="19" t="s">
-        <v>646</v>
+      <c r="D67" s="22" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -3330,19 +3439,19 @@
       <c r="C68" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="13" t="s">
         <v>641</v>
       </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="14" t="s">
+      <c r="B69" s="13"/>
+      <c r="C69" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="22" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3353,7 +3462,7 @@
       <c r="C70" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3364,7 +3473,7 @@
       <c r="C71" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D71" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3386,7 +3495,7 @@
       <c r="D75" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3400,7 +3509,7 @@
       <c r="D76" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3414,7 +3523,7 @@
       <c r="D77" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3425,7 +3534,7 @@
       <c r="C78" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3436,7 +3545,7 @@
       <c r="C79" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D79" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3447,7 +3556,7 @@
       <c r="C80" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D80" s="18" t="s">
+      <c r="D80" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3466,7 +3575,7 @@
       <c r="D83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3480,7 +3589,7 @@
       <c r="D84" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3494,7 +3603,7 @@
       <c r="D85" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3508,7 +3617,7 @@
       <c r="D86" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3523,7 +3632,7 @@
       <c r="D87" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E87" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3537,7 +3646,7 @@
       <c r="D88" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3551,7 +3660,7 @@
       <c r="D89" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="5">
+      <c r="E89" s="34">
         <v>43553</v>
       </c>
     </row>
@@ -3565,7 +3674,7 @@
       <c r="D90" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="5">
+      <c r="E90" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3579,7 +3688,7 @@
       <c r="D91" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="5">
+      <c r="E91" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -3593,7 +3702,7 @@
       <c r="D92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="5">
+      <c r="E92" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -3607,7 +3716,7 @@
       <c r="D93" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="5">
+      <c r="E93" s="34">
         <v>43556</v>
       </c>
     </row>
@@ -3615,13 +3724,13 @@
       <c r="A94" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="7" t="s">
         <v>341</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E94" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -3635,7 +3744,7 @@
       <c r="D95" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -3649,7 +3758,7 @@
       <c r="D96" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -3657,13 +3766,13 @@
       <c r="A97" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="9" t="s">
         <v>348</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E97" s="5"/>
+      <c r="E97" s="34"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
@@ -3675,22 +3784,22 @@
       <c r="D98" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98" s="34">
         <v>43558</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="15" t="s">
+      <c r="A99" s="13" t="s">
         <v>639</v>
       </c>
-      <c r="B99" s="15"/>
-      <c r="C99" s="20" t="s">
+      <c r="B99" s="13"/>
+      <c r="C99" s="19" t="s">
         <v>640</v>
       </c>
-      <c r="E99" s="5"/>
+      <c r="E99" s="34"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C100" s="7"/>
+      <c r="C100" s="6"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
@@ -3753,12 +3862,12 @@
       <c r="D110" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E110" s="5">
+      <c r="E110" s="34">
         <v>41370</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E111" s="5"/>
+      <c r="E111" s="34"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B112" s="1" t="s">
@@ -3811,7 +3920,7 @@
       <c r="D116" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E116" s="5">
+      <c r="E116" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -3852,7 +3961,7 @@
       <c r="A120" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="8" t="s">
         <v>384</v>
       </c>
     </row>
@@ -3893,7 +4002,7 @@
       <c r="A124" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C124" s="8" t="s">
         <v>384</v>
       </c>
     </row>
@@ -4017,7 +4126,7 @@
       <c r="D135" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E135" s="5">
+      <c r="E135" s="34">
         <v>43558</v>
       </c>
     </row>
@@ -4031,7 +4140,7 @@
       <c r="D136" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E136" s="5">
+      <c r="E136" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -4045,7 +4154,7 @@
       <c r="D137" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E137" s="5">
+      <c r="E137" s="34">
         <v>43558</v>
       </c>
     </row>
@@ -4059,7 +4168,7 @@
       <c r="D138" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E138" s="5">
+      <c r="E138" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4078,7 +4187,7 @@
       <c r="A140" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C140" s="9" t="s">
+      <c r="C140" s="8" t="s">
         <v>512</v>
       </c>
       <c r="D140" s="2" t="s">
@@ -4089,7 +4198,7 @@
       <c r="A141" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="C141" s="13" t="s">
+      <c r="C141" s="12" t="s">
         <v>542</v>
       </c>
     </row>
@@ -4111,7 +4220,7 @@
       <c r="D143" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E143" s="5">
+      <c r="E143" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4125,7 +4234,7 @@
       <c r="D144" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E144" s="5">
+      <c r="E144" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4139,7 +4248,7 @@
       <c r="D145" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E145" s="5">
+      <c r="E145" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4153,7 +4262,7 @@
       <c r="D146" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E146" s="5">
+      <c r="E146" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -4167,7 +4276,7 @@
       <c r="D147" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E147" s="5">
+      <c r="E147" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4181,7 +4290,7 @@
       <c r="D148" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E148" s="5">
+      <c r="E148" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -4195,7 +4304,7 @@
       <c r="D149" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E149" s="5">
+      <c r="E149" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4203,7 +4312,7 @@
       <c r="A150" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C150" s="9" t="s">
+      <c r="C150" s="8" t="s">
         <v>611</v>
       </c>
     </row>
@@ -4211,7 +4320,7 @@
       <c r="A151" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C151" s="9" t="s">
+      <c r="C151" s="8" t="s">
         <v>613</v>
       </c>
     </row>
@@ -4219,7 +4328,7 @@
       <c r="A152" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="C152" s="9" t="s">
+      <c r="C152" s="8" t="s">
         <v>615</v>
       </c>
     </row>
@@ -4227,7 +4336,7 @@
       <c r="A153" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="C153" s="9" t="s">
+      <c r="C153" s="8" t="s">
         <v>617</v>
       </c>
     </row>
@@ -4287,7 +4396,7 @@
       <c r="A163" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C163" s="6" t="s">
+      <c r="C163" s="5" t="s">
         <v>117</v>
       </c>
       <c r="D163" s="2" t="s">
@@ -4298,7 +4407,7 @@
       <c r="A164" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C164" s="6" t="s">
+      <c r="C164" s="5" t="s">
         <v>492</v>
       </c>
     </row>
@@ -4477,7 +4586,7 @@
       <c r="D180" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E180" s="5">
+      <c r="E180" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4499,7 +4608,7 @@
       <c r="D182" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E182" s="5">
+      <c r="E182" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4510,18 +4619,18 @@
       <c r="C183" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="E183" s="5"/>
+      <c r="E183" s="34"/>
     </row>
     <row r="184" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A184" s="15" t="s">
+      <c r="A184" s="13" t="s">
         <v>645</v>
       </c>
-      <c r="B184" s="15"/>
-      <c r="C184" s="14" t="s">
+      <c r="B184" s="13"/>
+      <c r="C184" s="16" t="s">
         <v>642</v>
       </c>
-      <c r="D184"/>
-      <c r="E184" s="5"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="34"/>
     </row>
     <row r="185" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
@@ -4533,7 +4642,7 @@
       <c r="D185" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E185" s="5">
+      <c r="E185" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4555,7 +4664,7 @@
       <c r="D187" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E187" s="5">
+      <c r="E187" s="34">
         <v>43558</v>
       </c>
     </row>
@@ -4577,7 +4686,7 @@
       <c r="D189" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E189" s="5">
+      <c r="E189" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -4585,13 +4694,13 @@
       <c r="A190" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C190" s="9" t="s">
+      <c r="C190" s="8" t="s">
         <v>517</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="E190" s="5">
+      <c r="E190" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4599,13 +4708,13 @@
       <c r="A191" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" s="10" t="s">
         <v>519</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E191" s="5">
+      <c r="E191" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4613,13 +4722,13 @@
       <c r="A192" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C192" s="12" t="s">
+      <c r="C192" s="11" t="s">
         <v>521</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E192" s="5">
+      <c r="E192" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -4627,13 +4736,13 @@
       <c r="A193" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C193" s="12" t="s">
+      <c r="C193" s="11" t="s">
         <v>523</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E193" s="5">
+      <c r="E193" s="34">
         <v>43557</v>
       </c>
     </row>
@@ -4648,7 +4757,7 @@
       <c r="D194" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E194" s="5">
+      <c r="E194" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4657,13 +4766,13 @@
         <v>525</v>
       </c>
       <c r="B195"/>
-      <c r="C195" s="10" t="s">
+      <c r="C195" s="9" t="s">
         <v>526</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E195" s="5">
+      <c r="E195" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -4678,7 +4787,7 @@
       <c r="D196" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E196" s="5">
+      <c r="E196" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -4693,7 +4802,7 @@
       <c r="D197" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E197" s="5">
+      <c r="E197" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4708,7 +4817,7 @@
       <c r="D198" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E198" s="5">
+      <c r="E198" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -4723,7 +4832,7 @@
       <c r="D199" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E199" s="5">
+      <c r="E199" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4735,10 +4844,10 @@
       <c r="C200" t="s">
         <v>536</v>
       </c>
-      <c r="D200" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E200" s="5">
+      <c r="D200" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4753,7 +4862,7 @@
       <c r="D201" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E201" s="5">
+      <c r="E201" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4768,7 +4877,7 @@
       <c r="D202" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E202" s="5">
+      <c r="E202" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4783,7 +4892,7 @@
       <c r="D203" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E203" s="5">
+      <c r="E203" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -4797,11 +4906,11 @@
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A205" s="15" t="s">
+      <c r="A205" s="13" t="s">
         <v>644</v>
       </c>
-      <c r="B205" s="20"/>
-      <c r="C205" s="14" t="s">
+      <c r="B205" s="15"/>
+      <c r="C205" s="16" t="s">
         <v>643</v>
       </c>
     </row>
@@ -4813,7 +4922,7 @@
       <c r="C206" t="s">
         <v>624</v>
       </c>
-      <c r="D206"/>
+      <c r="D206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
@@ -4823,26 +4932,26 @@
       <c r="C207" t="s">
         <v>626</v>
       </c>
-      <c r="D207"/>
+      <c r="D207" s="1"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>627</v>
       </c>
       <c r="B208"/>
-      <c r="C208" s="10" t="s">
+      <c r="C208" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="D208"/>
+      <c r="D208" s="1"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B209"/>
       <c r="C209"/>
-      <c r="D209"/>
+      <c r="D209" s="1"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C210"/>
-      <c r="E210" s="5"/>
+      <c r="E210" s="34"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B211" s="1" t="s">
@@ -4862,7 +4971,7 @@
       <c r="D212" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E212" s="5">
+      <c r="E212" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4876,7 +4985,7 @@
       <c r="D213" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E213" s="5">
+      <c r="E213" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4890,7 +4999,7 @@
       <c r="D214" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E214" s="5">
+      <c r="E214" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4904,7 +5013,7 @@
       <c r="D215" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E215" s="5">
+      <c r="E215" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4918,7 +5027,7 @@
       <c r="D216" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E216" s="5">
+      <c r="E216" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4932,7 +5041,7 @@
       <c r="D217" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E217" s="5">
+      <c r="E217" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4946,7 +5055,7 @@
       <c r="D218" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E218" s="5">
+      <c r="E218" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4960,7 +5069,7 @@
       <c r="D219" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E219" s="5">
+      <c r="E219" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4974,7 +5083,7 @@
       <c r="D220" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E220" s="5">
+      <c r="E220" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -4988,7 +5097,7 @@
       <c r="D221" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E221" s="5">
+      <c r="E221" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5002,7 +5111,7 @@
       <c r="D222" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E222" s="5">
+      <c r="E222" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5016,7 +5125,7 @@
       <c r="D223" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E223" s="5">
+      <c r="E223" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5030,7 +5139,7 @@
       <c r="D224" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E224" s="5">
+      <c r="E224" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5044,7 +5153,7 @@
       <c r="D225" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E225" s="5">
+      <c r="E225" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5058,7 +5167,7 @@
       <c r="D226" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E226" s="5">
+      <c r="E226" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5072,7 +5181,7 @@
       <c r="D227" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E227" s="5">
+      <c r="E227" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5086,7 +5195,7 @@
       <c r="D228" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E228" s="5">
+      <c r="E228" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5133,7 +5242,7 @@
       <c r="D232" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E232" s="5">
+      <c r="E232" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -5149,7 +5258,7 @@
       <c r="A234" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C234" s="9" t="s">
+      <c r="C234" s="8" t="s">
         <v>562</v>
       </c>
     </row>
@@ -5163,7 +5272,7 @@
       <c r="D235" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E235" s="5">
+      <c r="E235" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5177,7 +5286,7 @@
       <c r="D236" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E236" s="5">
+      <c r="E236" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5191,7 +5300,7 @@
       <c r="D237" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E237" s="5">
+      <c r="E237" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5205,7 +5314,7 @@
       <c r="D238" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E238" s="5">
+      <c r="E238" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5246,7 +5355,7 @@
       <c r="D242" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E242" s="5">
+      <c r="E242" s="34">
         <v>43560</v>
       </c>
     </row>
@@ -5260,7 +5369,7 @@
       <c r="D243" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E243" s="5">
+      <c r="E243" s="34">
         <v>43561</v>
       </c>
     </row>
@@ -5274,7 +5383,7 @@
       <c r="D244" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E244" s="5">
+      <c r="E244" s="34">
         <v>43562</v>
       </c>
     </row>
@@ -5611,7 +5720,7 @@
       <c r="D281" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E281" s="5">
+      <c r="E281" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5625,7 +5734,7 @@
       <c r="D282" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E282" s="5">
+      <c r="E282" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5639,7 +5748,7 @@
       <c r="D283" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E283" s="5">
+      <c r="E283" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5653,7 +5762,7 @@
       <c r="D284" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E284" s="5">
+      <c r="E284" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5667,7 +5776,7 @@
       <c r="D285" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E285" s="5">
+      <c r="E285" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5681,7 +5790,7 @@
       <c r="D286" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E286" s="5">
+      <c r="E286" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5692,7 +5801,7 @@
       <c r="C287" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E287" s="5">
+      <c r="E287" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5706,7 +5815,7 @@
       <c r="D288" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E288" s="5">
+      <c r="E288" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5720,7 +5829,7 @@
       <c r="D289" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E289" s="5">
+      <c r="E289" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -5731,10 +5840,10 @@
       <c r="C290" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E290" s="5"/>
+      <c r="E290" s="34"/>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E291" s="5"/>
+      <c r="E291" s="34"/>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B292" s="1" t="s">
@@ -5754,7 +5863,7 @@
       <c r="D293" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E293" s="5">
+      <c r="E293" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5768,7 +5877,7 @@
       <c r="D294" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E294" s="5">
+      <c r="E294" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5782,7 +5891,7 @@
       <c r="D295" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E295" s="5">
+      <c r="E295" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5810,7 +5919,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="299" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
         <v>600</v>
       </c>
@@ -5836,7 +5945,7 @@
       <c r="D307" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E307" s="5">
+      <c r="E307" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5850,7 +5959,7 @@
       <c r="D308" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E308" s="5">
+      <c r="E308" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5864,7 +5973,7 @@
       <c r="D309" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E309" s="5">
+      <c r="E309" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -5880,7 +5989,7 @@
       <c r="A311" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="C311" s="9" t="s">
+      <c r="C311" s="8" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5923,7 +6032,7 @@
       <c r="C316" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="E316" s="5"/>
+      <c r="E316" s="34"/>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
@@ -5932,22 +6041,22 @@
       <c r="C317" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="E317" s="5"/>
+      <c r="E317" s="34"/>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E318" s="5"/>
+      <c r="E318" s="34"/>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E319" s="5"/>
+      <c r="E319" s="34"/>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E320" s="5"/>
+      <c r="E320" s="34"/>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E321" s="5"/>
+      <c r="E321" s="34"/>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E322" s="5"/>
+      <c r="E322" s="34"/>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B323" s="1" t="s">
@@ -5967,7 +6076,7 @@
       <c r="D324" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E324" s="5">
+      <c r="E324" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -6152,7 +6261,7 @@
         <v>153</v>
       </c>
       <c r="B344" s="3"/>
-      <c r="C344" s="6" t="s">
+      <c r="C344" s="5" t="s">
         <v>339</v>
       </c>
       <c r="D344" s="2" t="s">
@@ -6162,10 +6271,10 @@
     <row r="345" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
-      <c r="C345" s="21" t="s">
+      <c r="C345" s="32" t="s">
         <v>483</v>
       </c>
-      <c r="D345" s="22"/>
+      <c r="D345" s="33"/>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
@@ -6232,7 +6341,7 @@
       <c r="D351" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E351" s="5">
+      <c r="E351" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6246,7 +6355,7 @@
       <c r="D352" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E352" s="5">
+      <c r="E352" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6260,7 +6369,7 @@
       <c r="D353" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E353" s="5">
+      <c r="E353" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6279,7 +6388,7 @@
       <c r="A355" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="C355" s="6" t="s">
+      <c r="C355" s="5" t="s">
         <v>485</v>
       </c>
     </row>
@@ -6293,7 +6402,7 @@
       <c r="D356" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E356" s="5">
+      <c r="E356" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6307,7 +6416,7 @@
       <c r="D357" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E357" s="5">
+      <c r="E357" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6332,7 +6441,7 @@
       <c r="D359" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E359" s="5">
+      <c r="E359" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6348,13 +6457,13 @@
       <c r="A361" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C361" s="6" t="s">
+      <c r="C361" s="5" t="s">
         <v>338</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E361" s="5">
+      <c r="E361" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6362,10 +6471,10 @@
       <c r="A362" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C362" s="6" t="s">
+      <c r="C362" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="E362" s="5"/>
+      <c r="E362" s="34"/>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
@@ -6374,7 +6483,7 @@
       <c r="C363" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E363" s="5"/>
+      <c r="E363" s="34"/>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="1" t="s">
@@ -6386,7 +6495,7 @@
       <c r="D364" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E364" s="5">
+      <c r="E364" s="34">
         <v>43559</v>
       </c>
     </row>
@@ -6397,19 +6506,19 @@
       <c r="C365" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E365" s="5"/>
+      <c r="E365" s="34"/>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C366" s="6" t="s">
+      <c r="C366" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="D366" s="6" t="s">
+      <c r="D366" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E366" s="5">
+      <c r="E366" s="34">
         <v>43559</v>
       </c>
     </row>
@@ -6423,7 +6532,7 @@
       <c r="D367" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E367" s="5">
+      <c r="E367" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -6437,7 +6546,7 @@
       <c r="D368" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E368" s="5">
+      <c r="E368" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -6445,13 +6554,13 @@
       <c r="A369" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C369" s="6" t="s">
+      <c r="C369" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="D369" s="6" t="s">
+      <c r="D369" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E369" s="5">
+      <c r="E369" s="34">
         <v>43559</v>
       </c>
     </row>
@@ -6470,7 +6579,7 @@
       <c r="D372" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E372" s="5">
+      <c r="E372" s="34">
         <v>43554</v>
       </c>
     </row>
@@ -6478,13 +6587,13 @@
       <c r="A373" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C373" s="9" t="s">
+      <c r="C373" s="8" t="s">
         <v>233</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E373" s="5">
+      <c r="E373" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -6492,13 +6601,13 @@
       <c r="A374" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C374" s="9" t="s">
+      <c r="C374" s="8" t="s">
         <v>234</v>
       </c>
       <c r="D374" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E374" s="5">
+      <c r="E374" s="34">
         <v>43555</v>
       </c>
     </row>
@@ -6506,14 +6615,73 @@
       <c r="A375" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C375" s="9" t="s">
+      <c r="C375" s="8" t="s">
         <v>235</v>
       </c>
       <c r="D375" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E375" s="5">
+      <c r="E375" s="34">
         <v>43555</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="378" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A378" s="27"/>
+      <c r="B378" s="27"/>
+      <c r="C378" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="D378" s="29">
+        <f>COUNTA($D$1:$D376)</f>
+        <v>242</v>
+      </c>
+      <c r="E378" s="36"/>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C379" s="24" t="s">
+        <v>655</v>
+      </c>
+      <c r="D379" s="25">
+        <f>COUNTIF($D$1:$D377, "=Done")</f>
+        <v>207</v>
+      </c>
+      <c r="E379" s="26">
+        <f>$D379/$D$378</f>
+        <v>0.85537190082644632</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C380" s="30" t="s">
+        <v>657</v>
+      </c>
+      <c r="D380" s="25"/>
+      <c r="E380" s="26"/>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C381" s="31" t="s">
+        <v>656</v>
+      </c>
+      <c r="D381" s="25">
+        <f>COUNTIF($D$1:$D378, "=In process")</f>
+        <v>8</v>
+      </c>
+      <c r="E381" s="26">
+        <f>$D381/($D$378 - $D$379)</f>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C382" s="31" t="s">
+        <v>658</v>
+      </c>
+      <c r="D382" s="25">
+        <f>COUNTIF($D$1:$D379, "=Pending")</f>
+        <v>10</v>
+      </c>
+      <c r="E382" s="26">
+        <f>$D382/($D$378 - $D$379)</f>
+        <v>0.2857142857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S18.FB2: Make status contents bigger and make two rows tall. Add BRED filename to it.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE67B509-B41B-4C56-A7EC-790863A1D5F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B919B1F1-6321-4212-BEAE-9C8466DDEB68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24720" yWindow="6960" windowWidth="18180" windowHeight="22560" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="1980" yWindow="16185" windowWidth="19845" windowHeight="14670" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F414" authorId="0" shapeId="0" xr:uid="{219F0334-9C0D-4B0E-9917-EC384D011BEF}">
+    <comment ref="F416" authorId="0" shapeId="0" xr:uid="{219F0334-9C0D-4B0E-9917-EC384D011BEF}">
       <text>
         <r>
           <rPr>
@@ -795,7 +795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2497" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="782">
   <si>
     <t>ID</t>
   </si>
@@ -3281,6 +3281,86 @@
   </si>
   <si>
     <t>The difference in color of the last two tab headers needs to be greater. Make the last much darker blue.</t>
+  </si>
+  <si>
+    <t>Colors adjusted. Good enough?</t>
+  </si>
+  <si>
+    <r>
+      <t>Inspection Mode tooltip: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mode"</t>
+    </r>
+  </si>
+  <si>
+    <t>T6.Q1</t>
+  </si>
+  <si>
+    <t>Inventory Mode'? Not 'Inspection Model'?</t>
+  </si>
+  <si>
+    <t>Tooltip is 'Inspection Mode'.</t>
+  </si>
+  <si>
+    <t>Tooltip is 'Inventory Mode'.</t>
+  </si>
+  <si>
+    <t>T3.Q1</t>
+  </si>
+  <si>
+    <t>No Copy Inspection image supplied with the last delivery. Still Pending?</t>
+  </si>
+  <si>
+    <t>S28.1</t>
+  </si>
+  <si>
+    <t>S27.1</t>
+  </si>
+  <si>
+    <t>New images have been applied</t>
+  </si>
+  <si>
+    <t>Implemented something closer to the real thing.</t>
+  </si>
+  <si>
+    <t>S22.FB1</t>
+  </si>
+  <si>
+    <t>S22.FB1.1</t>
+  </si>
+  <si>
+    <t>S22.FB1.2</t>
+  </si>
+  <si>
+    <t>S22.FB1.3</t>
+  </si>
+  <si>
+    <t>S18.FB1</t>
+  </si>
+  <si>
+    <t>S18.FB1.1</t>
+  </si>
+  <si>
+    <t>S18.FB2</t>
   </si>
 </sst>
 </file>
@@ -3429,7 +3509,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3489,6 +3569,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3602,7 +3688,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3764,6 +3850,31 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4086,10 +4197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:F445"/>
+  <dimension ref="A1:F451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="C424" sqref="C424"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D407" sqref="D407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8362,7 +8474,7 @@
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>180</v>
+        <v>779</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>356</v>
@@ -8376,90 +8488,78 @@
     </row>
     <row r="407" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>222</v>
+        <v>780</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D407" s="2" t="s">
-        <v>225</v>
-      </c>
     </row>
     <row r="408" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A408" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C408" s="5" t="s">
+      <c r="A408" s="67" t="s">
+        <v>781</v>
+      </c>
+      <c r="B408" s="67"/>
+      <c r="C408" s="64" t="s">
         <v>484</v>
       </c>
+      <c r="D408" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E408" s="65">
+        <v>43568</v>
+      </c>
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A409" s="1" t="s">
+      <c r="C409" s="5"/>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C410" s="5"/>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C409" s="2" t="s">
+      <c r="C411" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D409" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E409" s="31">
+      <c r="D411" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E411" s="31">
         <v>43554</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A410" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C410" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D410" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E410" s="31">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="411" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A411" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C411" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D411" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>217</v>
+        <v>358</v>
       </c>
       <c r="D412" s="2" t="s">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="E412" s="31">
         <v>43554</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="414" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="D413" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C414" s="5" t="s">
-        <v>338</v>
+        <v>216</v>
+      </c>
+      <c r="C414" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="D414" s="2" t="s">
         <v>225</v>
@@ -8467,102 +8567,107 @@
       <c r="E414" s="31">
         <v>43554</v>
       </c>
-      <c r="F414" s="43" t="s">
-        <v>743</v>
-      </c>
     </row>
     <row r="415" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C415" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="C415" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D415" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E415" s="31">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C416" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D416" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E416" s="31">
+        <v>43554</v>
+      </c>
+      <c r="F416" s="43" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C417" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="E415" s="31"/>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A416" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C416" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E416" s="31"/>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A417" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C417" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D417" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E417" s="31">
-        <v>43559</v>
-      </c>
+      <c r="D417" t="s">
+        <v>7</v>
+      </c>
+      <c r="E417" s="31"/>
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C418" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="E418" s="31"/>
+        <v>778</v>
+      </c>
+      <c r="C418" s="71" t="s">
+        <v>774</v>
+      </c>
+      <c r="D418" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E418" s="31">
+        <v>43559</v>
+      </c>
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C419" s="38" t="s">
-        <v>504</v>
-      </c>
-      <c r="D419" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D419" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E419" s="31">
         <v>43559</v>
       </c>
-      <c r="F419" s="43" t="s">
-        <v>744</v>
-      </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>238</v>
+        <v>361</v>
       </c>
       <c r="C420" s="2" t="s">
-        <v>239</v>
+        <v>362</v>
       </c>
       <c r="D420" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E420" s="31">
-        <v>43555</v>
+        <v>43559</v>
       </c>
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>240</v>
+        <v>363</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D421" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E421" s="31">
-        <v>43555</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="E421" s="31"/>
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C422" s="38" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D422" s="38" t="s">
         <v>7</v>
@@ -8574,218 +8679,311 @@
         <v>744</v>
       </c>
     </row>
-    <row r="423" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D423" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E423" s="31">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D424" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E424" s="31">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C425" s="38" t="s">
+        <v>506</v>
+      </c>
+      <c r="D425" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E425" s="31">
+        <v>43559</v>
+      </c>
+      <c r="F425" s="43" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="C423" s="5" t="s">
+      <c r="C426" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="D423" s="38"/>
-      <c r="E423" s="31"/>
-      <c r="F423" s="43"/>
-    </row>
-    <row r="424" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A424" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="C424" s="5" t="s">
-        <v>762</v>
-      </c>
-      <c r="D424" s="38"/>
-      <c r="E424" s="31"/>
-      <c r="F424" s="43"/>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C425" s="38"/>
-      <c r="D425" s="38"/>
-      <c r="E425" s="31"/>
-      <c r="F425" s="43"/>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C426" s="38"/>
       <c r="D426" s="38"/>
       <c r="E426" s="31"/>
-      <c r="F426" s="43"/>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C427" s="38"/>
-      <c r="D427" s="38"/>
-      <c r="E427" s="31"/>
-      <c r="F427" s="43"/>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C428" s="38"/>
-      <c r="D428" s="38"/>
-      <c r="E428" s="31"/>
-      <c r="F428" s="43"/>
+      <c r="A427" s="69" t="s">
+        <v>772</v>
+      </c>
+      <c r="B427" s="69"/>
+      <c r="C427" s="69" t="s">
+        <v>773</v>
+      </c>
+      <c r="D427" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E427" s="69">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A428" s="67" t="s">
+        <v>761</v>
+      </c>
+      <c r="B428" s="67"/>
+      <c r="C428" s="63" t="s">
+        <v>762</v>
+      </c>
+      <c r="D428" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E428" s="65">
+        <v>43568</v>
+      </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C429" s="38"/>
+      <c r="A429" s="67" t="s">
+        <v>771</v>
+      </c>
+      <c r="C429" s="63" t="s">
+        <v>763</v>
+      </c>
       <c r="D429" s="38"/>
       <c r="E429" s="31"/>
-      <c r="F429" s="43"/>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C430" s="38"/>
       <c r="D430" s="38"/>
       <c r="E430" s="31"/>
-      <c r="F430" s="43"/>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C431" s="38"/>
       <c r="D431" s="38"/>
       <c r="E431" s="31"/>
-      <c r="F431" s="43"/>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C432" s="38"/>
+      <c r="D432" s="38"/>
+      <c r="E432" s="31"/>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B433" s="1" t="s">
+      <c r="C433" s="38"/>
+      <c r="D433" s="38"/>
+      <c r="E433" s="31"/>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C434" s="38"/>
+      <c r="D434" s="38"/>
+      <c r="E434" s="31"/>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C435" s="38"/>
+      <c r="D435" s="38"/>
+      <c r="E435" s="31"/>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437" s="45"/>
+      <c r="B437" s="45" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A434" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C434" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D434" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E434" s="31">
-        <v>43554</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A435" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C435" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D435" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E435" s="31">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A436" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C436" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="D436" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E436" s="31">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A437" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C437" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D437" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E437" s="31">
-        <v>43555</v>
-      </c>
+      <c r="C437" s="70"/>
+      <c r="D437" s="70"/>
+      <c r="E437" s="45"/>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C438" s="11" t="s">
-        <v>746</v>
-      </c>
-      <c r="E438"/>
-      <c r="F438" s="47"/>
+        <v>228</v>
+      </c>
+      <c r="C438" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D438" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E438" s="31">
+        <v>43554</v>
+      </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C439" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E439" s="31">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C440" t="s">
+        <v>234</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E440" s="31">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441" s="67" t="s">
+        <v>769</v>
+      </c>
+      <c r="B441" s="67"/>
+      <c r="C441" s="63" t="s">
+        <v>770</v>
+      </c>
+      <c r="E441" s="31"/>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C442" t="s">
+        <v>235</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E442" s="31">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C443"/>
+      <c r="E443" s="31"/>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C444" t="s">
+        <v>746</v>
+      </c>
+      <c r="D444" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="E444" s="46">
+        <v>43537</v>
+      </c>
+      <c r="F444" s="47"/>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="B439" s="1" t="s">
+      <c r="B445" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C439" s="11" t="s">
-        <v>748</v>
-      </c>
-      <c r="E439"/>
-      <c r="F439" s="47"/>
-    </row>
-    <row r="440" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C440" s="11"/>
-      <c r="E440"/>
-      <c r="F440" s="47"/>
-    </row>
-    <row r="441" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A441" s="26"/>
-      <c r="B441" s="26"/>
-      <c r="C441" s="27" t="s">
+      <c r="C445" s="11" t="s">
+        <v>764</v>
+      </c>
+      <c r="F445" s="47"/>
+    </row>
+    <row r="446" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A446" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C446" s="66" t="s">
+        <v>766</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="E446" s="46">
+        <v>43537</v>
+      </c>
+      <c r="F446" s="47"/>
+    </row>
+    <row r="447" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A447" s="26"/>
+      <c r="B447" s="26"/>
+      <c r="C447" s="27" t="s">
         <v>651</v>
       </c>
-      <c r="D441" s="28">
-        <f>COUNTA($D$1:$D438)</f>
-        <v>245</v>
-      </c>
-      <c r="E441" s="33"/>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C442" s="23" t="s">
+      <c r="D447" s="28">
+        <f>COUNTA($D$1:$D444)</f>
+        <v>252</v>
+      </c>
+      <c r="E447" s="33"/>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C448" s="23" t="s">
         <v>652</v>
       </c>
-      <c r="D442" s="24">
-        <f>COUNTIF($D$1:$D439, "=Done")</f>
-        <v>209</v>
-      </c>
-      <c r="E442" s="25">
-        <f>$D442/$D$441</f>
-        <v>0.85306122448979593</v>
-      </c>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C443" s="29" t="s">
+      <c r="D448" s="24">
+        <f>COUNTIF($D$1:$D444, "=Done")</f>
+        <v>218</v>
+      </c>
+      <c r="E448" s="25">
+        <f>$D448/$D$447</f>
+        <v>0.86507936507936511</v>
+      </c>
+    </row>
+    <row r="449" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C449" s="29" t="s">
         <v>654</v>
       </c>
-      <c r="D443" s="24"/>
-      <c r="E443" s="25"/>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C444" s="30" t="s">
+      <c r="D449" s="24"/>
+      <c r="E449" s="25"/>
+    </row>
+    <row r="450" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C450" s="30" t="s">
         <v>653</v>
       </c>
-      <c r="D444" s="24">
-        <f>COUNTIF($D$1:$D441, "=In process")</f>
-        <v>6</v>
-      </c>
-      <c r="E444" s="25">
-        <f>$D444/($D$441 - $D$442)</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C445" s="30" t="s">
+      <c r="D450" s="24">
+        <f>COUNTIF($D$1:$D447, "=In process")</f>
+        <v>5</v>
+      </c>
+      <c r="E450" s="25">
+        <f>$D450/($D$447 - $D$448)</f>
+        <v>0.14705882352941177</v>
+      </c>
+    </row>
+    <row r="451" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C451" s="30" t="s">
         <v>655</v>
       </c>
-      <c r="D445" s="24">
-        <f>COUNTIF($D$1:$D442, "=Pending")</f>
-        <v>10</v>
-      </c>
-      <c r="E445" s="25">
-        <f>$D445/($D$441 - $D$442)</f>
-        <v>0.27777777777777779</v>
+      <c r="D451" s="24">
+        <f>COUNTIF($D$1:$D448, "=Pending")</f>
+        <v>8</v>
+      </c>
+      <c r="E451" s="25">
+        <f>$D451/($D$447 - $D$448)</f>
+        <v>0.23529411764705882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S5.FB1: Added checkmarks to View All Systems and View Assigned Systems, which are mutually exclusive.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B919B1F1-6321-4212-BEAE-9C8466DDEB68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B5F29-58F7-4163-B0DB-3BA0A85515FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="16185" windowWidth="19845" windowHeight="14670" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="2130" yWindow="14340" windowWidth="19845" windowHeight="14670" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="783">
   <si>
     <t>ID</t>
   </si>
@@ -3361,6 +3361,9 @@
   </si>
   <si>
     <t>S18.FB2</t>
+  </si>
+  <si>
+    <t>S5.FB1</t>
   </si>
 </sst>
 </file>
@@ -3688,7 +3691,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3876,6 +3879,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4200,8 +4206,8 @@
   <dimension ref="A1:F451"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D407" sqref="D407"/>
+      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A390" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8290,15 +8296,20 @@
     </row>
     <row r="390" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>739</v>
+        <v>782</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C390" s="11" t="s">
+      <c r="C390" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="E390"/>
+      <c r="D390" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E390" s="46">
+        <v>43568</v>
+      </c>
       <c r="F390" s="47"/>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
@@ -8308,10 +8319,15 @@
       <c r="B391" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C391" s="11" t="s">
+      <c r="C391" t="s">
         <v>742</v>
       </c>
-      <c r="E391"/>
+      <c r="D391" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E391" s="46">
+        <v>43528</v>
+      </c>
       <c r="F391" s="47"/>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
@@ -8369,7 +8385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="s">
         <v>153</v>
       </c>
@@ -8381,13 +8397,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="3"/>
       <c r="B398" s="3"/>
-      <c r="C398" s="61" t="s">
+      <c r="C398" s="72" t="s">
         <v>482</v>
       </c>
-      <c r="D398" s="62"/>
+      <c r="D398"/>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
@@ -8936,7 +8952,7 @@
       </c>
       <c r="D447" s="28">
         <f>COUNTA($D$1:$D444)</f>
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E447" s="33"/>
     </row>
@@ -8946,11 +8962,11 @@
       </c>
       <c r="D448" s="24">
         <f>COUNTIF($D$1:$D444, "=Done")</f>
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E448" s="25">
         <f>$D448/$D$447</f>
-        <v>0.86507936507936511</v>
+        <v>0.86614173228346458</v>
       </c>
     </row>
     <row r="449" spans="3:5" x14ac:dyDescent="0.25">
@@ -8987,9 +9003,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C398:D398"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{09484B62-D5BF-4D5E-8BE0-935A927A1E23}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
S21.FB: Added an active BG to the Inventory and Inspection toolbar buttons so that could indicate what mode operating in.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E125436B-2189-4DFE-8350-F7127148D0E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BAFE4-DAE5-4C87-B6A2-621D24B1853C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="15" windowWidth="18270" windowHeight="31770" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
@@ -867,7 +867,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2676" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="891">
   <si>
     <t>ID</t>
   </si>
@@ -3926,7 +3926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4004,6 +4004,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4135,7 +4141,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4270,9 +4276,6 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4315,9 +4318,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4351,12 +4351,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4487,6 +4481,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4811,8 +4829,8 @@
   <dimension ref="A1:F498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C506" sqref="C506"/>
+      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A459" sqref="A459:E459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,27 +4867,27 @@
       <c r="B3" s="27" t="s">
         <v>641</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="61" t="s">
         <v>642</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>643</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="75" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="76" t="s">
         <v>644</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="73" t="s">
         <v>645</v>
       </c>
       <c r="D5" s="15"/>
@@ -4884,7 +4902,7 @@
       <c r="D6" s="11" t="s">
         <v>820</v>
       </c>
-      <c r="E6" s="82">
+      <c r="E6" s="78">
         <v>43570</v>
       </c>
     </row>
@@ -4935,7 +4953,7 @@
       <c r="C11" s="11" t="s">
         <v>821</v>
       </c>
-      <c r="D11" s="83"/>
+      <c r="D11" s="79"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4945,10 +4963,10 @@
       <c r="C12" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D12" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="85">
+      <c r="D12" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="81">
         <v>43563</v>
       </c>
     </row>
@@ -4959,10 +4977,10 @@
       <c r="C13" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D13" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="87">
+      <c r="D13" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="83">
         <v>43563</v>
       </c>
     </row>
@@ -5016,10 +5034,10 @@
       <c r="C18" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="89">
+      <c r="D18" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="85">
         <v>43563</v>
       </c>
     </row>
@@ -5030,10 +5048,10 @@
       <c r="C19" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D19" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="89">
+      <c r="D19" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="85">
         <v>43563</v>
       </c>
     </row>
@@ -5124,10 +5142,10 @@
       <c r="C29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="90" t="s">
+      <c r="D29" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="91">
+      <c r="E29" s="87">
         <v>43555</v>
       </c>
     </row>
@@ -5138,10 +5156,10 @@
       <c r="C30" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="D30" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="89">
+      <c r="D30" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="85">
         <v>43563</v>
       </c>
     </row>
@@ -5156,7 +5174,7 @@
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="90"/>
+      <c r="C32" s="86"/>
       <c r="D32"/>
       <c r="E32"/>
     </row>
@@ -5192,11 +5210,11 @@
       <c r="B35" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C35" s="90" t="s">
+      <c r="C35" s="86" t="s">
         <v>653</v>
       </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="87"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -5205,13 +5223,13 @@
       <c r="B36" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C36" s="86" t="s">
         <v>655</v>
       </c>
-      <c r="D36" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="89">
+      <c r="D36" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5222,13 +5240,13 @@
       <c r="B37" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C37" s="90" t="s">
+      <c r="C37" s="86" t="s">
         <v>657</v>
       </c>
-      <c r="D37" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="89">
+      <c r="D37" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5239,13 +5257,13 @@
       <c r="B38" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C38" s="90" t="s">
+      <c r="C38" s="86" t="s">
         <v>659</v>
       </c>
-      <c r="D38" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="89">
+      <c r="D38" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5256,13 +5274,13 @@
       <c r="B39" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C39" s="90" t="s">
+      <c r="C39" s="86" t="s">
         <v>661</v>
       </c>
-      <c r="D39" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="89">
+      <c r="D39" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5273,11 +5291,11 @@
       <c r="B40" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C40" s="90" t="s">
+      <c r="C40" s="86" t="s">
         <v>663</v>
       </c>
-      <c r="D40" s="90"/>
-      <c r="E40" s="91"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="87"/>
     </row>
     <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -5286,13 +5304,13 @@
       <c r="B41" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="C41" s="86" t="s">
         <v>665</v>
       </c>
-      <c r="D41" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="89">
+      <c r="D41" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5303,13 +5321,13 @@
       <c r="B42" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C42" s="86" t="s">
         <v>667</v>
       </c>
-      <c r="D42" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="89">
+      <c r="D42" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5320,8 +5338,8 @@
       <c r="C43" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="D43" s="88"/>
-      <c r="E43" s="89"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="85"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -5432,10 +5450,10 @@
       <c r="C52" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D52" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="89">
+      <c r="D52" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5444,7 +5462,7 @@
         <v>780</v>
       </c>
       <c r="B53"/>
-      <c r="C53" s="54" t="s">
+      <c r="C53" s="53" t="s">
         <v>781</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -5455,11 +5473,11 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="56" t="s">
         <v>782</v>
       </c>
       <c r="B54"/>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="57" t="s">
         <v>783</v>
       </c>
     </row>
@@ -5515,13 +5533,13 @@
       <c r="A61" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="90" t="s">
+      <c r="C61" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="D61" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="89">
+      <c r="D61" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5532,13 +5550,13 @@
       <c r="B62" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C62" s="90" t="s">
+      <c r="C62" s="86" t="s">
         <v>668</v>
       </c>
-      <c r="D62" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="89">
+      <c r="D62" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5546,38 +5564,38 @@
       <c r="A63" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C63" s="90" t="s">
+      <c r="C63" s="86" t="s">
         <v>670</v>
       </c>
-      <c r="D63" s="90"/>
-      <c r="E63" s="92"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="88"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C64" s="90" t="s">
+      <c r="C64" s="86" t="s">
         <v>334</v>
       </c>
-      <c r="D64" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="89">
+      <c r="D64" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="85">
         <v>43563</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="94" t="s">
+      <c r="A65" s="90" t="s">
         <v>631</v>
       </c>
-      <c r="B65" s="94"/>
-      <c r="C65" s="93" t="s">
+      <c r="B65" s="90"/>
+      <c r="C65" s="89" t="s">
         <v>632</v>
       </c>
-      <c r="D65" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" s="89">
+      <c r="D65" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5635,10 +5653,10 @@
       <c r="C71" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D71" s="88" t="s">
+      <c r="D71" s="84" t="s">
         <v>510</v>
       </c>
-      <c r="E71" s="95"/>
+      <c r="E71" s="91"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -5647,10 +5665,10 @@
       <c r="C72" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D72" s="96" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="92"/>
+      <c r="D72" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="88"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -5659,10 +5677,10 @@
       <c r="C73" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="D73" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="89">
+      <c r="D73" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5673,11 +5691,11 @@
       <c r="B74" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C74" s="101" t="s">
+      <c r="C74" s="97" t="s">
         <v>604</v>
       </c>
-      <c r="D74" s="90"/>
-      <c r="E74" s="92"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="88"/>
     </row>
     <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -5686,13 +5704,13 @@
       <c r="B75" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C75" s="101" t="s">
+      <c r="C75" s="97" t="s">
         <v>672</v>
       </c>
-      <c r="D75" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" s="89">
+      <c r="D75" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="85">
         <v>43570</v>
       </c>
     </row>
@@ -5703,13 +5721,13 @@
       <c r="B76" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C76" s="101" t="s">
+      <c r="C76" s="97" t="s">
         <v>606</v>
       </c>
-      <c r="D76" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="92"/>
+      <c r="D76" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="88"/>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -5718,13 +5736,13 @@
       <c r="B77" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C77" s="101" t="s">
+      <c r="C77" s="97" t="s">
         <v>674</v>
       </c>
-      <c r="D77" s="97" t="s">
+      <c r="D77" s="93" t="s">
         <v>814</v>
       </c>
-      <c r="E77" s="98"/>
+      <c r="E77" s="94"/>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
@@ -5733,13 +5751,13 @@
       <c r="B78" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C78" s="101" t="s">
+      <c r="C78" s="97" t="s">
         <v>608</v>
       </c>
-      <c r="D78" s="99" t="s">
+      <c r="D78" s="95" t="s">
         <v>815</v>
       </c>
-      <c r="E78" s="100">
+      <c r="E78" s="96">
         <v>43570</v>
       </c>
     </row>
@@ -5750,18 +5768,18 @@
       <c r="B79" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C79" s="90" t="s">
+      <c r="C79" s="86" t="s">
         <v>676</v>
       </c>
-      <c r="D79" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" s="89">
+      <c r="D79" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="85">
         <v>43572</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C80" s="54"/>
+      <c r="C80" s="53"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="25"/>
@@ -5795,13 +5813,13 @@
       <c r="B83" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C83" s="90" t="s">
+      <c r="C83" s="86" t="s">
         <v>678</v>
       </c>
-      <c r="D83" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="89">
+      <c r="D83" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5812,11 +5830,11 @@
       <c r="B84" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C84" s="90" t="s">
+      <c r="C84" s="86" t="s">
         <v>680</v>
       </c>
-      <c r="D84" s="90"/>
-      <c r="E84" s="91"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="87"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -5825,13 +5843,13 @@
       <c r="B85" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C85" s="90" t="s">
+      <c r="C85" s="86" t="s">
         <v>682</v>
       </c>
-      <c r="D85" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="89">
+      <c r="D85" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="85">
         <v>43569</v>
       </c>
     </row>
@@ -5849,26 +5867,26 @@
       <c r="A87" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C87" s="104" t="s">
+      <c r="C87" s="100" t="s">
         <v>279</v>
       </c>
-      <c r="D87" s="105" t="s">
+      <c r="D87" s="101" t="s">
         <v>839</v>
       </c>
-      <c r="E87" s="106"/>
+      <c r="E87" s="102"/>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="92" t="s">
+      <c r="A88" s="88" t="s">
         <v>778</v>
       </c>
-      <c r="B88" s="92"/>
-      <c r="C88" s="104" t="s">
+      <c r="B88" s="88"/>
+      <c r="C88" s="100" t="s">
         <v>779</v>
       </c>
-      <c r="D88" s="105" t="s">
+      <c r="D88" s="101" t="s">
         <v>840</v>
       </c>
-      <c r="E88" s="106"/>
+      <c r="E88" s="102"/>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -5877,19 +5895,19 @@
       <c r="C89" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="D89" s="105"/>
-      <c r="E89" s="106"/>
+      <c r="D89" s="101"/>
+      <c r="E89" s="102"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="92" t="s">
+      <c r="A90" s="88" t="s">
         <v>280</v>
       </c>
-      <c r="B90" s="92"/>
-      <c r="C90" s="104" t="s">
+      <c r="B90" s="88"/>
+      <c r="C90" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="D90" s="107"/>
-      <c r="E90" s="106"/>
+      <c r="D90" s="103"/>
+      <c r="E90" s="102"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
@@ -5898,21 +5916,21 @@
       <c r="C91" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="D91" s="102"/>
-      <c r="E91" s="106"/>
+      <c r="D91" s="98"/>
+      <c r="E91" s="102"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="92" t="s">
+      <c r="A92" s="88" t="s">
         <v>282</v>
       </c>
-      <c r="B92" s="92"/>
-      <c r="C92" s="104" t="s">
+      <c r="B92" s="88"/>
+      <c r="C92" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="D92" s="105" t="s">
+      <c r="D92" s="101" t="s">
         <v>839</v>
       </c>
-      <c r="E92" s="106"/>
+      <c r="E92" s="102"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -5921,39 +5939,39 @@
       <c r="C93" s="11" t="s">
         <v>848</v>
       </c>
-      <c r="D93" s="102"/>
-      <c r="E93" s="106"/>
+      <c r="D93" s="98"/>
+      <c r="E93" s="102"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="92" t="s">
+      <c r="A94" s="88" t="s">
         <v>284</v>
       </c>
-      <c r="B94" s="92"/>
-      <c r="C94" s="104" t="s">
+      <c r="B94" s="88"/>
+      <c r="C94" s="100" t="s">
         <v>285</v>
       </c>
-      <c r="D94" s="105"/>
-      <c r="E94" s="106"/>
+      <c r="D94" s="101"/>
+      <c r="E94" s="102"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C95" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="D95" s="102"/>
-      <c r="E95" s="106"/>
+      <c r="D95" s="98"/>
+      <c r="E95" s="102"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="92" t="s">
+      <c r="A96" s="88" t="s">
         <v>286</v>
       </c>
-      <c r="B96" s="92"/>
-      <c r="C96" s="104" t="s">
+      <c r="B96" s="88"/>
+      <c r="C96" s="100" t="s">
         <v>287</v>
       </c>
-      <c r="D96" s="105" t="s">
+      <c r="D96" s="101" t="s">
         <v>839</v>
       </c>
-      <c r="E96" s="108"/>
+      <c r="E96" s="104"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
@@ -5963,34 +5981,34 @@
       <c r="C97" s="13" t="s">
         <v>633</v>
       </c>
-      <c r="D97" s="102" t="s">
+      <c r="D97" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="E97" s="106"/>
+      <c r="E97" s="102"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="92" t="s">
+      <c r="A98" s="88" t="s">
         <v>288</v>
       </c>
-      <c r="B98" s="92"/>
-      <c r="C98" s="104" t="s">
+      <c r="B98" s="88"/>
+      <c r="C98" s="100" t="s">
         <v>271</v>
       </c>
-      <c r="D98" s="105" t="s">
+      <c r="D98" s="101" t="s">
         <v>839</v>
       </c>
-      <c r="E98" s="108"/>
+      <c r="E98" s="104"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="92" t="s">
+      <c r="A99" s="88" t="s">
         <v>322</v>
       </c>
-      <c r="B99" s="92"/>
-      <c r="C99" s="90" t="s">
+      <c r="B99" s="88"/>
+      <c r="C99" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="D99" s="103"/>
-      <c r="E99" s="95"/>
+      <c r="D99" s="99"/>
+      <c r="E99" s="91"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="25"/>
@@ -6007,13 +6025,13 @@
       <c r="A103" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C103" s="90" t="s">
+      <c r="C103" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="D103" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" s="91">
+      <c r="D103" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="87">
         <v>43555</v>
       </c>
     </row>
@@ -6021,13 +6039,13 @@
       <c r="A104" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C104" s="90" t="s">
+      <c r="C104" s="86" t="s">
         <v>304</v>
       </c>
-      <c r="D104" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" s="91">
+      <c r="D104" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="87">
         <v>43555</v>
       </c>
     </row>
@@ -6038,13 +6056,13 @@
       <c r="B105" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C105" s="90" t="s">
+      <c r="C105" s="86" t="s">
         <v>684</v>
       </c>
-      <c r="D105" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E105" s="89">
+      <c r="D105" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="85">
         <v>43570</v>
       </c>
     </row>
@@ -6055,13 +6073,13 @@
       <c r="B106" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C106" s="90" t="s">
+      <c r="C106" s="86" t="s">
         <v>686</v>
       </c>
-      <c r="D106" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E106" s="89">
+      <c r="D106" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="85">
         <v>43570</v>
       </c>
     </row>
@@ -6069,13 +6087,13 @@
       <c r="A107" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C107" s="90" t="s">
+      <c r="C107" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="D107" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E107" s="91">
+      <c r="D107" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="87">
         <v>43555</v>
       </c>
     </row>
@@ -6086,13 +6104,13 @@
       <c r="B108" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C108" s="90" t="s">
+      <c r="C108" s="86" t="s">
         <v>688</v>
       </c>
-      <c r="D108" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E108" s="89">
+      <c r="D108" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" s="85">
         <v>43570</v>
       </c>
     </row>
@@ -6100,49 +6118,49 @@
       <c r="A109" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C109" s="90" t="s">
+      <c r="C109" s="86" t="s">
         <v>308</v>
       </c>
-      <c r="D109" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E109" s="95"/>
+      <c r="D109" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" s="91"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C110" s="90" t="s">
+      <c r="C110" s="86" t="s">
         <v>310</v>
       </c>
-      <c r="D110" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E110" s="95"/>
+      <c r="D110" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="91"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C111" s="90" t="s">
+      <c r="C111" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="D111" s="84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E111" s="95"/>
+      <c r="D111" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="91"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="C112" s="90" t="s">
+      <c r="C112" s="86" t="s">
         <v>817</v>
       </c>
-      <c r="D112" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E112" s="89">
+      <c r="D112" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="85">
         <v>43570</v>
       </c>
     </row>
@@ -6332,7 +6350,7 @@
       <c r="A128" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C128" s="63" t="s">
+      <c r="C128" s="62" t="s">
         <v>341</v>
       </c>
       <c r="D128" s="2" t="s">
@@ -6346,7 +6364,7 @@
       <c r="A129" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C129" s="54" t="s">
+      <c r="C129" s="53" t="s">
         <v>343</v>
       </c>
       <c r="D129" s="2" t="s">
@@ -6363,7 +6381,7 @@
       <c r="A130" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C130" s="54" t="s">
+      <c r="C130" s="53" t="s">
         <v>345</v>
       </c>
       <c r="D130" s="2" t="s">
@@ -6377,7 +6395,7 @@
       <c r="A131" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C131" s="109" t="s">
+      <c r="C131" s="105" t="s">
         <v>348</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -6389,7 +6407,7 @@
       <c r="A132" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C132" s="54" t="s">
+      <c r="C132" s="53" t="s">
         <v>501</v>
       </c>
       <c r="D132" s="2" t="s">
@@ -6405,7 +6423,7 @@
         <v>634</v>
       </c>
       <c r="B133" s="12"/>
-      <c r="C133" s="64" t="s">
+      <c r="C133" s="63" t="s">
         <v>635</v>
       </c>
       <c r="E133" s="21"/>
@@ -6415,7 +6433,7 @@
         <v>854</v>
       </c>
       <c r="B134" s="12"/>
-      <c r="C134" s="110" t="s">
+      <c r="C134" s="106" t="s">
         <v>855</v>
       </c>
       <c r="E134" s="21"/>
@@ -6427,7 +6445,7 @@
       <c r="B135" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C135" s="54" t="s">
+      <c r="C135" s="53" t="s">
         <v>691</v>
       </c>
       <c r="D135" s="16" t="s">
@@ -6438,7 +6456,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C136" s="54"/>
+      <c r="C136" s="53"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="25"/>
@@ -6971,19 +6989,19 @@
       </c>
     </row>
     <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="92" t="s">
+      <c r="A185" s="88" t="s">
         <v>694</v>
       </c>
-      <c r="B185" s="92" t="s">
+      <c r="B185" s="88" t="s">
         <v>367</v>
       </c>
-      <c r="C185" s="111" t="s">
+      <c r="C185" s="107" t="s">
         <v>691</v>
       </c>
-      <c r="D185" s="112" t="s">
-        <v>7</v>
-      </c>
-      <c r="E185" s="113">
+      <c r="D185" s="108" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" s="109">
         <v>43569</v>
       </c>
       <c r="F185" s="33" t="s">
@@ -7191,13 +7209,13 @@
       <c r="B208" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C208" s="90" t="s">
+      <c r="C208" s="86" t="s">
         <v>698</v>
       </c>
-      <c r="D208" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E208" s="89">
+      <c r="D208" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E208" s="85">
         <v>43568</v>
       </c>
     </row>
@@ -7324,7 +7342,7 @@
       <c r="E219" s="21">
         <v>43555</v>
       </c>
-      <c r="F219" s="116"/>
+      <c r="F219" s="112"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
@@ -7436,7 +7454,7 @@
       <c r="A229" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C229" s="72" t="s">
+      <c r="C229" s="70" t="s">
         <v>516</v>
       </c>
       <c r="D229" s="2" t="s">
@@ -7447,15 +7465,15 @@
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="59" t="s">
+      <c r="A230" s="58" t="s">
         <v>813</v>
       </c>
-      <c r="B230" s="59"/>
-      <c r="C230" s="73" t="s">
+      <c r="B230" s="58"/>
+      <c r="C230" s="71" t="s">
         <v>812</v>
       </c>
-      <c r="D230" s="60"/>
-      <c r="E230" s="74"/>
+      <c r="D230" s="59"/>
+      <c r="E230" s="72"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
@@ -7475,7 +7493,7 @@
       <c r="A232" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C232" s="115" t="s">
+      <c r="C232" s="111" t="s">
         <v>809</v>
       </c>
       <c r="D232" s="2" t="s">
@@ -7489,7 +7507,7 @@
       <c r="A233" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="C233" s="114" t="s">
+      <c r="C233" s="110" t="s">
         <v>859</v>
       </c>
       <c r="E233" s="21"/>
@@ -7499,7 +7517,7 @@
       <c r="A234" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="C234" s="115" t="s">
+      <c r="C234" s="111" t="s">
         <v>811</v>
       </c>
       <c r="D234" s="2" t="s">
@@ -7513,7 +7531,7 @@
       <c r="A235" s="1" t="s">
         <v>860</v>
       </c>
-      <c r="C235" s="114" t="s">
+      <c r="C235" s="110" t="s">
         <v>861</v>
       </c>
       <c r="E235" s="21"/>
@@ -7559,7 +7577,7 @@
         <v>523</v>
       </c>
       <c r="B239"/>
-      <c r="C239" s="54" t="s">
+      <c r="C239" s="53" t="s">
         <v>617</v>
       </c>
       <c r="D239" s="2" t="s">
@@ -7592,7 +7610,7 @@
         <v>526</v>
       </c>
       <c r="B241"/>
-      <c r="C241" s="54" t="s">
+      <c r="C241" s="53" t="s">
         <v>527</v>
       </c>
       <c r="D241" s="2" t="s">
@@ -7607,7 +7625,7 @@
         <v>528</v>
       </c>
       <c r="B242"/>
-      <c r="C242" s="54" t="s">
+      <c r="C242" s="53" t="s">
         <v>529</v>
       </c>
       <c r="D242" s="2" t="s">
@@ -7622,7 +7640,7 @@
         <v>530</v>
       </c>
       <c r="B243"/>
-      <c r="C243" s="54" t="s">
+      <c r="C243" s="53" t="s">
         <v>531</v>
       </c>
       <c r="D243" s="2" t="s">
@@ -7633,19 +7651,19 @@
       </c>
     </row>
     <row r="244" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A244" s="92" t="s">
+      <c r="A244" s="88" t="s">
         <v>703</v>
       </c>
-      <c r="B244" s="92" t="s">
+      <c r="B244" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="C244" s="117" t="s">
+      <c r="C244" s="113" t="s">
         <v>691</v>
       </c>
-      <c r="D244" s="118" t="s">
-        <v>7</v>
-      </c>
-      <c r="E244" s="119">
+      <c r="D244" s="114" t="s">
+        <v>7</v>
+      </c>
+      <c r="E244" s="115">
         <v>43569</v>
       </c>
     </row>
@@ -7654,7 +7672,7 @@
         <v>532</v>
       </c>
       <c r="B245"/>
-      <c r="C245" s="54" t="s">
+      <c r="C245" s="53" t="s">
         <v>533</v>
       </c>
       <c r="D245" s="2" t="s">
@@ -7669,7 +7687,7 @@
         <v>534</v>
       </c>
       <c r="B246"/>
-      <c r="C246" s="54" t="s">
+      <c r="C246" s="53" t="s">
         <v>535</v>
       </c>
       <c r="D246" s="21" t="s">
@@ -7684,7 +7702,7 @@
         <v>536</v>
       </c>
       <c r="B247"/>
-      <c r="C247" s="54" t="s">
+      <c r="C247" s="53" t="s">
         <v>537</v>
       </c>
       <c r="D247" s="2" t="s">
@@ -7699,7 +7717,7 @@
         <v>538</v>
       </c>
       <c r="B248"/>
-      <c r="C248" s="54" t="s">
+      <c r="C248" s="53" t="s">
         <v>539</v>
       </c>
       <c r="D248" s="2" t="s">
@@ -7714,7 +7732,7 @@
         <v>618</v>
       </c>
       <c r="B249"/>
-      <c r="C249" s="54" t="s">
+      <c r="C249" s="53" t="s">
         <v>619</v>
       </c>
       <c r="D249" s="2" t="s">
@@ -7729,7 +7747,7 @@
         <v>620</v>
       </c>
       <c r="B250"/>
-      <c r="C250" s="54" t="s">
+      <c r="C250" s="53" t="s">
         <v>621</v>
       </c>
       <c r="D250" s="11" t="s">
@@ -7740,11 +7758,11 @@
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="69" t="s">
+      <c r="A251" s="67" t="s">
         <v>639</v>
       </c>
-      <c r="B251" s="70"/>
-      <c r="C251" s="71" t="s">
+      <c r="B251" s="68"/>
+      <c r="C251" s="69" t="s">
         <v>638</v>
       </c>
       <c r="D251" s="11" t="s">
@@ -7757,7 +7775,7 @@
         <v>622</v>
       </c>
       <c r="B252"/>
-      <c r="C252" s="54" t="s">
+      <c r="C252" s="53" t="s">
         <v>623</v>
       </c>
       <c r="D252" s="11" t="s">
@@ -7770,7 +7788,7 @@
         <v>624</v>
       </c>
       <c r="B253"/>
-      <c r="C253" s="54" t="s">
+      <c r="C253" s="53" t="s">
         <v>625</v>
       </c>
       <c r="D253" s="1" t="s">
@@ -7779,11 +7797,11 @@
       <c r="F253" s="37"/>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A254" s="92" t="s">
+      <c r="A254" s="88" t="s">
         <v>626</v>
       </c>
-      <c r="B254" s="120"/>
-      <c r="C254" s="121" t="s">
+      <c r="B254" s="116"/>
+      <c r="C254" s="117" t="s">
         <v>627</v>
       </c>
       <c r="D254" s="1" t="s">
@@ -7791,13 +7809,13 @@
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A255" s="92" t="s">
+      <c r="A255" s="88" t="s">
         <v>707</v>
       </c>
-      <c r="B255" s="92" t="s">
+      <c r="B255" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="C255" s="121" t="s">
+      <c r="C255" s="117" t="s">
         <v>708</v>
       </c>
       <c r="D255" s="1" t="s">
@@ -7805,13 +7823,13 @@
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" s="92" t="s">
+      <c r="A256" s="88" t="s">
         <v>709</v>
       </c>
-      <c r="B256" s="92" t="s">
+      <c r="B256" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="C256" s="121" t="s">
+      <c r="C256" s="117" t="s">
         <v>710</v>
       </c>
       <c r="D256" s="1" t="s">
@@ -7819,13 +7837,13 @@
       </c>
     </row>
     <row r="257" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A257" s="92" t="s">
+      <c r="A257" s="88" t="s">
         <v>711</v>
       </c>
-      <c r="B257" s="92" t="s">
+      <c r="B257" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="C257" s="121" t="s">
+      <c r="C257" s="117" t="s">
         <v>712</v>
       </c>
       <c r="D257" s="1" t="s">
@@ -7871,11 +7889,11 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B265"/>
-      <c r="C265" s="54"/>
+      <c r="C265" s="53"/>
       <c r="D265" s="1"/>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C266" s="54"/>
+      <c r="C266" s="53"/>
       <c r="E266" s="21"/>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -8056,7 +8074,7 @@
       <c r="B280" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="C280" s="68" t="s">
+      <c r="C280" s="66" t="s">
         <v>715</v>
       </c>
       <c r="D280" s="2" t="s">
@@ -8097,7 +8115,7 @@
       <c r="B283" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="C283" s="68" t="s">
+      <c r="C283" s="66" t="s">
         <v>715</v>
       </c>
       <c r="D283" s="2" t="s">
@@ -8233,7 +8251,7 @@
       <c r="A293" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C293" s="54" t="s">
+      <c r="C293" s="53" t="s">
         <v>463</v>
       </c>
       <c r="D293" s="2" t="s">
@@ -8774,7 +8792,7 @@
       <c r="A345" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C345" s="54" t="s">
+      <c r="C345" s="53" t="s">
         <v>166</v>
       </c>
       <c r="D345" s="2" t="s">
@@ -8934,39 +8952,39 @@
       <c r="F356" s="37"/>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C357" s="54"/>
+      <c r="C357" s="53"/>
       <c r="E357" s="21"/>
       <c r="F357" s="37"/>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C358" s="54"/>
+      <c r="C358" s="53"/>
       <c r="E358" s="21"/>
       <c r="F358" s="37"/>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C359" s="54"/>
+      <c r="C359" s="53"/>
       <c r="E359" s="21"/>
       <c r="F359" s="37"/>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C360" s="54"/>
+      <c r="C360" s="53"/>
       <c r="E360" s="21"/>
       <c r="F360" s="37"/>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C361" s="54"/>
+      <c r="C361" s="53"/>
       <c r="E361" s="21"/>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C362" s="54"/>
+      <c r="C362" s="53"/>
       <c r="E362" s="21"/>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C363" s="54"/>
+      <c r="C363" s="53"/>
       <c r="E363" s="21"/>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C364" s="54"/>
+      <c r="C364" s="53"/>
       <c r="E364" s="21"/>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.25">
@@ -9053,7 +9071,7 @@
       <c r="B371" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C371" s="90" t="s">
+      <c r="C371" s="86" t="s">
         <v>728</v>
       </c>
       <c r="D371" s="2" t="s">
@@ -9130,7 +9148,7 @@
       <c r="B384" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C384" s="90" t="s">
+      <c r="C384" s="86" t="s">
         <v>730</v>
       </c>
       <c r="D384" s="2" t="s">
@@ -9525,38 +9543,38 @@
       </c>
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A422" s="123" t="s">
+      <c r="A422" s="119" t="s">
         <v>804</v>
       </c>
-      <c r="B422" s="123"/>
-      <c r="C422" s="101" t="s">
+      <c r="B422" s="119"/>
+      <c r="C422" s="97" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A423" s="61" t="s">
+      <c r="A423" s="60" t="s">
         <v>879</v>
       </c>
-      <c r="B423" s="61"/>
-      <c r="C423" s="122" t="s">
+      <c r="B423" s="60"/>
+      <c r="C423" s="118" t="s">
         <v>880</v>
       </c>
     </row>
     <row r="424" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A424" s="61" t="s">
+      <c r="A424" s="60" t="s">
         <v>806</v>
       </c>
-      <c r="B424" s="61"/>
+      <c r="B424" s="60"/>
       <c r="C424" s="51" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="425" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A425" s="61" t="s">
+      <c r="A425" s="60" t="s">
         <v>881</v>
       </c>
-      <c r="B425" s="61"/>
-      <c r="C425" s="122" t="s">
+      <c r="B425" s="60"/>
+      <c r="C425" s="118" t="s">
         <v>882</v>
       </c>
     </row>
@@ -9605,11 +9623,11 @@
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A431" s="55" t="s">
+      <c r="A431" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="B431" s="55"/>
-      <c r="C431" s="56" t="s">
+      <c r="B431" s="54"/>
+      <c r="C431" s="55" t="s">
         <v>353</v>
       </c>
       <c r="F431" s="33" t="s">
@@ -9617,11 +9635,11 @@
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A432" s="55" t="s">
+      <c r="A432" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B432" s="55"/>
-      <c r="C432" s="56" t="s">
+      <c r="B432" s="54"/>
+      <c r="C432" s="55" t="s">
         <v>354</v>
       </c>
       <c r="F432" s="33" t="s">
@@ -9657,10 +9675,10 @@
       <c r="B435" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C435" s="101" t="s">
+      <c r="C435" s="97" t="s">
         <v>736</v>
       </c>
-      <c r="D435" s="101" t="s">
+      <c r="D435" s="97" t="s">
         <v>7</v>
       </c>
       <c r="E435" s="21">
@@ -9675,7 +9693,7 @@
       <c r="B436" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C436" s="54" t="s">
+      <c r="C436" s="53" t="s">
         <v>738</v>
       </c>
       <c r="D436" s="2" t="s">
@@ -9750,10 +9768,10 @@
       </c>
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A443" s="55" t="s">
+      <c r="A443" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="B443" s="55"/>
+      <c r="B443" s="54"/>
       <c r="C443" s="28" t="s">
         <v>339</v>
       </c>
@@ -9764,7 +9782,7 @@
     <row r="444" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A444" s="3"/>
       <c r="B444" s="3"/>
-      <c r="C444" s="54" t="s">
+      <c r="C444" s="53" t="s">
         <v>482</v>
       </c>
       <c r="D444" s="1"/>
@@ -9878,7 +9896,7 @@
       <c r="A454" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="C454" s="122" t="s">
+      <c r="C454" s="118" t="s">
         <v>886</v>
       </c>
       <c r="D454" s="2" t="s">
@@ -9886,17 +9904,17 @@
       </c>
     </row>
     <row r="455" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A455" s="92" t="s">
+      <c r="A455" s="88" t="s">
         <v>776</v>
       </c>
-      <c r="B455" s="92"/>
-      <c r="C455" s="124" t="s">
+      <c r="B455" s="88"/>
+      <c r="C455" s="120" t="s">
         <v>484</v>
       </c>
-      <c r="D455" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E455" s="91">
+      <c r="D455" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E455" s="87">
         <v>43568</v>
       </c>
     </row>
@@ -9932,17 +9950,19 @@
       </c>
     </row>
     <row r="459" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A459" s="67" t="s">
+      <c r="A459" s="128" t="s">
         <v>183</v>
       </c>
-      <c r="B459" s="67"/>
-      <c r="C459" s="5" t="s">
+      <c r="B459" s="128"/>
+      <c r="C459" s="127" t="s">
         <v>359</v>
       </c>
-      <c r="D459" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E459" s="67"/>
+      <c r="D459" s="127" t="s">
+        <v>7</v>
+      </c>
+      <c r="E459" s="129">
+        <v>43572</v>
+      </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
@@ -10118,7 +10138,7 @@
       <c r="A472" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="C472" s="5" t="s">
+      <c r="C472" s="28" t="s">
         <v>756</v>
       </c>
       <c r="D472" s="28" t="s">
@@ -10129,40 +10149,41 @@
       </c>
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A473" s="120" t="s">
+      <c r="A473" s="116" t="s">
         <v>767</v>
       </c>
-      <c r="B473" s="120"/>
-      <c r="C473" s="111" t="s">
+      <c r="B473" s="116"/>
+      <c r="C473" s="107" t="s">
         <v>768</v>
       </c>
-      <c r="D473" s="92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E473" s="92">
+      <c r="D473" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="E473" s="88">
         <v>43568</v>
       </c>
     </row>
     <row r="474" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A474" s="92" t="s">
+      <c r="A474" s="88" t="s">
         <v>757</v>
       </c>
-      <c r="B474" s="92"/>
-      <c r="C474" s="101" t="s">
+      <c r="B474" s="88"/>
+      <c r="C474" s="120" t="s">
         <v>758</v>
       </c>
-      <c r="D474" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E474" s="91">
+      <c r="D474" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E474" s="87">
         <v>43568</v>
       </c>
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A475" s="52" t="s">
+      <c r="A475" s="126" t="s">
         <v>766</v>
       </c>
-      <c r="C475" s="51" t="s">
+      <c r="B475" s="126"/>
+      <c r="C475" s="127" t="s">
         <v>759</v>
       </c>
       <c r="D475" s="28"/>
@@ -10203,8 +10224,8 @@
       <c r="B483" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="C483" s="53"/>
-      <c r="D483" s="53"/>
+      <c r="C483" s="52"/>
+      <c r="D483" s="52"/>
       <c r="E483" s="35"/>
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.25">
@@ -10228,7 +10249,12 @@
       <c r="C485" s="11" t="s">
         <v>888</v>
       </c>
-      <c r="E485" s="21"/>
+      <c r="D485" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="E485" s="125">
+        <v>43572</v>
+      </c>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
@@ -10245,14 +10271,14 @@
       </c>
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A487" s="92" t="s">
+      <c r="A487" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="B487" s="92"/>
-      <c r="C487" s="111" t="s">
+      <c r="B487" s="88"/>
+      <c r="C487" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="D487" s="90" t="s">
+      <c r="D487" s="86" t="s">
         <v>7</v>
       </c>
       <c r="E487" s="21">
@@ -10260,17 +10286,17 @@
       </c>
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A488" s="92" t="s">
+      <c r="A488" s="88" t="s">
         <v>764</v>
       </c>
-      <c r="B488" s="92"/>
-      <c r="C488" s="101" t="s">
+      <c r="B488" s="88"/>
+      <c r="C488" s="97" t="s">
         <v>765</v>
       </c>
-      <c r="D488" s="90" t="s">
-        <v>7</v>
-      </c>
-      <c r="E488" s="91">
+      <c r="D488" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E488" s="87">
         <v>43571</v>
       </c>
     </row>
@@ -10278,7 +10304,7 @@
       <c r="A489" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C489" s="54" t="s">
+      <c r="C489" s="53" t="s">
         <v>235</v>
       </c>
       <c r="D489" s="2" t="s">
@@ -10295,7 +10321,7 @@
       <c r="B490" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C490" s="54" t="s">
+      <c r="C490" s="53" t="s">
         <v>742</v>
       </c>
       <c r="D490" s="2" t="s">
@@ -10310,7 +10336,7 @@
       <c r="A491" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="C491" s="54" t="s">
+      <c r="C491" s="53" t="s">
         <v>890</v>
       </c>
       <c r="D491" s="2" t="s">
@@ -10328,7 +10354,7 @@
       <c r="B492" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C492" s="90" t="s">
+      <c r="C492" s="86" t="s">
         <v>760</v>
       </c>
       <c r="D492" s="2" t="s">
@@ -10343,7 +10369,7 @@
       <c r="A493" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="C493" s="125" t="s">
+      <c r="C493" s="121" t="s">
         <v>762</v>
       </c>
       <c r="D493" s="2" t="s">
@@ -10357,7 +10383,7 @@
     <row r="494" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A494" s="19"/>
       <c r="B494" s="19"/>
-      <c r="C494" s="65" t="s">
+      <c r="C494" s="64" t="s">
         <v>647</v>
       </c>
       <c r="D494" s="20">
@@ -10367,27 +10393,27 @@
       <c r="E494" s="23"/>
     </row>
     <row r="495" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C495" s="66" t="s">
+      <c r="C495" s="65" t="s">
         <v>648</v>
       </c>
       <c r="D495" s="17">
         <f>COUNTIF($D$1:$D490, "=Done")</f>
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E495" s="18">
         <f>$D495/$D$494</f>
-        <v>0.68641975308641978</v>
+        <v>0.69135802469135799</v>
       </c>
     </row>
     <row r="496" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C496" s="66" t="s">
+      <c r="C496" s="65" t="s">
         <v>650</v>
       </c>
       <c r="D496" s="17"/>
       <c r="E496" s="18"/>
     </row>
     <row r="497" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C497" s="66" t="s">
+      <c r="C497" s="65" t="s">
         <v>649</v>
       </c>
       <c r="D497" s="17">
@@ -10396,20 +10422,20 @@
       </c>
       <c r="E497" s="18">
         <f>$D497/($D$494 - $D$495)</f>
-        <v>1.5748031496062992E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="498" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C498" s="66" t="s">
+      <c r="C498" s="65" t="s">
         <v>651</v>
       </c>
       <c r="D498" s="17">
         <f>COUNTIF($D$1:$D495, "=Pending")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E498" s="18">
         <f>$D498/($D$494 - $D$495)</f>
-        <v>4.7244094488188976E-2</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -15187,10 +15213,10 @@
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="122" t="s">
         <v>482</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="123"/>
       <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
G3: Mike on/off toggle indicators.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD15F80D-4286-4A9F-97DD-0BB471101032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC66F92-10FB-4BE5-8A22-9E34D7F34E28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="13845" windowWidth="23520" windowHeight="16095" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="9600" yWindow="14265" windowWidth="23520" windowHeight="16095" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3038" uniqueCount="1028">
   <si>
     <t>ID</t>
   </si>
@@ -3698,7 +3698,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3752,6 +3752,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3826,7 +3832,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4133,9 +4139,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4144,6 +4147,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4476,8 +4491,8 @@
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C583" sqref="C583"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4629,15 +4644,19 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="117" t="s">
         <v>1011</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="112" t="s">
+      <c r="B12" s="118"/>
+      <c r="C12" s="119" t="s">
         <v>1012</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="120">
+        <v>43580</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="88"/>
@@ -9784,11 +9803,11 @@
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A435" s="115" t="s">
+      <c r="A435" s="114" t="s">
         <v>1008</v>
       </c>
-      <c r="B435" s="115"/>
-      <c r="C435" s="116" t="s">
+      <c r="B435" s="114"/>
+      <c r="C435" s="115" t="s">
         <v>1026</v>
       </c>
     </row>
@@ -9832,7 +9851,7 @@
       <c r="B444" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C444" s="117" t="s">
+      <c r="C444" s="116" t="s">
         <v>1027</v>
       </c>
       <c r="D444" s="2" t="s">
@@ -11573,7 +11592,7 @@
       </c>
       <c r="D589" s="11">
         <f>COUNTA($D$1:$D577)</f>
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E589" s="13"/>
     </row>
@@ -11583,11 +11602,11 @@
       </c>
       <c r="D590" s="8">
         <f>COUNTIF($D$1:$D577, "=Done")</f>
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E590" s="9">
         <f>$D590/$D$589</f>
-        <v>0.90338164251207731</v>
+        <v>0.90361445783132532</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
T7-9: Tighten up the toolbar button size requirements. A little shorter. Buttons a little closer to each other and the mike buttons mo longer hug the right of the screen.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC66F92-10FB-4BE5-8A22-9E34D7F34E28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AD84C-AEF9-4BEC-9D80-7ECBA1726FA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="14265" windowWidth="23520" windowHeight="16095" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="870" yWindow="14310" windowWidth="23520" windowHeight="16095" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3038" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1028">
   <si>
     <t>ID</t>
   </si>
@@ -3832,7 +3832,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4160,6 +4160,10 @@
     <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -4491,8 +4495,8 @@
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A565" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C581" sqref="A581:C581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11535,34 +11539,49 @@
       </c>
     </row>
     <row r="581" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A581" s="109" t="s">
+      <c r="A581" s="118" t="s">
         <v>913</v>
       </c>
-      <c r="B581" s="109"/>
-      <c r="C581" s="111" t="s">
+      <c r="B581" s="118"/>
+      <c r="C581" s="121" t="s">
         <v>914</v>
       </c>
-      <c r="E581" s="25"/>
+      <c r="D581" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E581" s="122">
+        <v>43580</v>
+      </c>
     </row>
     <row r="582" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A582" s="109" t="s">
+      <c r="A582" s="118" t="s">
         <v>915</v>
       </c>
-      <c r="B582" s="109"/>
-      <c r="C582" s="111" t="s">
+      <c r="B582" s="118"/>
+      <c r="C582" s="121" t="s">
         <v>916</v>
       </c>
-      <c r="E582" s="25"/>
+      <c r="D582" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E582" s="122">
+        <v>43580</v>
+      </c>
     </row>
     <row r="583" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A583" s="109" t="s">
+      <c r="A583" s="118" t="s">
         <v>917</v>
       </c>
-      <c r="B583" s="109"/>
-      <c r="C583" s="111" t="s">
+      <c r="B583" s="118"/>
+      <c r="C583" s="121" t="s">
         <v>918</v>
       </c>
-      <c r="E583" s="25"/>
+      <c r="D583" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E583" s="122">
+        <v>43580</v>
+      </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C584" s="32"/>

</xml_diff>

<commit_message>
SB 1 and 2: Reduce the vertical requirements of the status bar.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hagga\source\repos\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AD84C-AEF9-4BEC-9D80-7ECBA1726FA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE1A8BB-5D10-4DF4-B5EF-93C4D6C2EA6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="14310" windowWidth="23520" windowHeight="16095" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="1028">
   <si>
     <t>ID</t>
   </si>
@@ -3832,7 +3832,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4164,6 +4164,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -4495,8 +4501,8 @@
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A565" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C581" sqref="A581:C581"/>
+      <pane ySplit="1" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A562" sqref="A562:E563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11331,26 +11337,34 @@
       <c r="E561" s="24"/>
     </row>
     <row r="562" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A562" s="109" t="s">
+      <c r="A562" s="118" t="s">
         <v>921</v>
       </c>
-      <c r="B562" s="109"/>
-      <c r="C562" s="110" t="s">
+      <c r="B562" s="118"/>
+      <c r="C562" s="123" t="s">
         <v>922</v>
       </c>
-      <c r="D562" s="73"/>
-      <c r="E562" s="56"/>
+      <c r="D562" s="123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E562" s="124">
+        <v>43580</v>
+      </c>
     </row>
     <row r="563" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A563" s="109" t="s">
+      <c r="A563" s="118" t="s">
         <v>923</v>
       </c>
-      <c r="B563" s="109"/>
-      <c r="C563" s="110" t="s">
+      <c r="B563" s="118"/>
+      <c r="C563" s="123" t="s">
         <v>924</v>
       </c>
-      <c r="D563" s="18"/>
-      <c r="E563" s="12"/>
+      <c r="D563" s="123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E563" s="124">
+        <v>43580</v>
+      </c>
     </row>
     <row r="564" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C564" s="18"/>
@@ -11611,7 +11625,7 @@
       </c>
       <c r="D589" s="11">
         <f>COUNTA($D$1:$D577)</f>
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E589" s="13"/>
     </row>
@@ -11621,11 +11635,11 @@
       </c>
       <c r="D590" s="8">
         <f>COUNTIF($D$1:$D577, "=Done")</f>
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E590" s="9">
         <f>$D590/$D$589</f>
-        <v>0.90361445783132532</v>
+        <v>0.90407673860911275</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated InventoryView and tasklist.
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill_\source\Projects\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74530FE1-2DD5-4FDB-9F4B-5A91BAD3AD3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80A74EC-D1E9-4126-B9E8-93E6C62E959F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27060" yWindow="2400" windowWidth="26580" windowHeight="13485" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="1031">
   <si>
     <t>ID</t>
   </si>
@@ -3309,9 +3308,6 @@
     <t>F26</t>
   </si>
   <si>
-    <t>Remove Funtioinal Area row.</t>
-  </si>
-  <si>
     <t>IS48</t>
   </si>
   <si>
@@ -3587,6 +3583,9 @@
   </si>
   <si>
     <t>Closed (reduced white space)</t>
+  </si>
+  <si>
+    <t>Remove Funtional Area row.</t>
   </si>
 </sst>
 </file>
@@ -4472,7 +4471,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D171" sqref="D171:E171"/>
+      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4585,7 +4584,7 @@
         <v>876</v>
       </c>
       <c r="D8" s="62" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E8" s="63">
         <v>43581</v>
@@ -4638,11 +4637,11 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="76" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B12" s="77"/>
       <c r="C12" s="78" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D12" s="78" t="s">
         <v>7</v>
@@ -5639,11 +5638,11 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="70" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B92" s="70"/>
       <c r="C92" s="71" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D92" s="34" t="s">
         <v>7</v>
@@ -5654,14 +5653,14 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="70" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B93" s="70"/>
       <c r="C93" s="71" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D93" s="34" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E93" s="35">
         <v>43581</v>
@@ -5669,14 +5668,14 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="70" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B94" s="70"/>
       <c r="C94" s="71" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D94" s="34" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E94" s="35">
         <v>43581</v>
@@ -6016,11 +6015,11 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="85" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B121" s="85"/>
       <c r="C121" s="86" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D121" s="40" t="s">
         <v>7</v>
@@ -6031,14 +6030,14 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="44" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B122" s="44"/>
       <c r="C122" s="26" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D122" s="40" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E122" s="41">
         <v>43581</v>
@@ -6046,14 +6045,14 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="44" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B123" s="44"/>
       <c r="C123" s="26" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D123" s="40" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E123" s="41">
         <v>43581</v>
@@ -6061,11 +6060,11 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="44" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B124" s="44"/>
       <c r="C124" s="26" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D124" s="40" t="s">
         <v>7</v>
@@ -6644,7 +6643,12 @@
       <c r="C170" s="72" t="s">
         <v>939</v>
       </c>
-      <c r="E170" s="42"/>
+      <c r="D170" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E170" s="37">
+        <v>43581</v>
+      </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="70" t="s">
@@ -6669,6 +6673,12 @@
       <c r="C172" s="72" t="s">
         <v>943</v>
       </c>
+      <c r="D172" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="37">
+        <v>43581</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="70" t="s">
@@ -6678,6 +6688,12 @@
       <c r="C173" s="72" t="s">
         <v>945</v>
       </c>
+      <c r="D173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="37">
+        <v>43581</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="70" t="s">
@@ -6687,6 +6703,12 @@
       <c r="C174" s="72" t="s">
         <v>947</v>
       </c>
+      <c r="D174" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E174" s="37">
+        <v>43581</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="70" t="s">
@@ -6696,6 +6718,12 @@
       <c r="C175" s="72" t="s">
         <v>949</v>
       </c>
+      <c r="D175" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E175" s="37">
+        <v>43581</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="70" t="s">
@@ -6703,7 +6731,13 @@
       </c>
       <c r="B176" s="70"/>
       <c r="C176" s="72" t="s">
-        <v>951</v>
+        <v>1030</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" s="37">
+        <v>43581</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
@@ -7399,29 +7433,29 @@
     </row>
     <row r="234" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A234" s="70" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B234" s="70"/>
       <c r="C234" s="72" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" s="70" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B235" s="70"/>
       <c r="C235" s="72" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" s="70" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B236" s="70"/>
       <c r="C236" s="72" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.35">
@@ -8311,11 +8345,11 @@
     </row>
     <row r="308" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A308" s="70" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B308" s="70"/>
       <c r="C308" s="71" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D308" s="40"/>
       <c r="E308" s="41"/>
@@ -8323,11 +8357,11 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A309" s="70" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B309" s="70"/>
       <c r="C309" s="71" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D309" s="40"/>
       <c r="E309" s="41"/>
@@ -8335,11 +8369,11 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A310" s="70" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B310" s="70"/>
       <c r="C310" s="71" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D310" s="40"/>
       <c r="E310" s="41"/>
@@ -8347,11 +8381,11 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A311" s="70" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B311" s="70"/>
       <c r="C311" s="71" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D311" s="40"/>
       <c r="E311" s="41"/>
@@ -8359,11 +8393,11 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A312" s="70" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B312" s="70"/>
       <c r="C312" s="71" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D312" s="40"/>
       <c r="E312" s="41"/>
@@ -8371,11 +8405,11 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A313" s="70" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B313" s="70"/>
       <c r="C313" s="71" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D313" s="40"/>
       <c r="E313" s="41"/>
@@ -9031,56 +9065,56 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="70" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B360" s="70"/>
       <c r="C360" s="72" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="70" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B361" s="70"/>
       <c r="C361" s="72" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="70" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B362" s="70"/>
       <c r="C362" s="72" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="70" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B363" s="70"/>
       <c r="C363" s="72" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="70" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B364" s="70"/>
       <c r="C364" s="72" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="70" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B365" s="70"/>
       <c r="C365" s="72" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
@@ -9808,90 +9842,90 @@
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A427" s="70" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B427" s="70"/>
       <c r="C427" s="72" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E427" s="12"/>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A428" s="70" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B428" s="70"/>
       <c r="C428" s="72" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E428" s="12"/>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A429" s="70" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B429" s="70"/>
       <c r="C429" s="72" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E429" s="12"/>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A430" s="70" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B430" s="70"/>
       <c r="C430" s="72" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E430" s="12"/>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A431" s="70" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B431" s="70"/>
       <c r="C431" s="72" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E431" s="12"/>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A432" s="70" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B432" s="70"/>
       <c r="C432" s="72" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E432" s="12"/>
     </row>
     <row r="433" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A433" s="70" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B433" s="70"/>
       <c r="C433" s="72" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E433" s="12"/>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A434" s="70" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B434" s="70"/>
       <c r="C434" s="72" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A435" s="73" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B435" s="73"/>
       <c r="C435" s="74" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="441" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
@@ -9935,7 +9969,7 @@
         <v>465</v>
       </c>
       <c r="C444" s="75" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D444" s="2" t="s">
         <v>7</v>
@@ -10000,7 +10034,7 @@
         <v>703</v>
       </c>
       <c r="D448" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E448" s="12"/>
     </row>
@@ -10205,71 +10239,71 @@
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A464" s="70" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B464" s="70"/>
       <c r="C464" s="72" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E464" s="12"/>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A465" s="70" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B465" s="70"/>
       <c r="C465" s="72" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E465" s="12"/>
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A466" s="70" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B466" s="70"/>
       <c r="C466" s="72" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E466" s="12"/>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A467" s="70" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B467" s="70"/>
       <c r="C467" s="72" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E467" s="12"/>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A468" s="70" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B468" s="70"/>
       <c r="C468" s="72" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E468" s="12"/>
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A469" s="70" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B469" s="70"/>
       <c r="C469" s="72" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E469" s="12"/>
     </row>
     <row r="470" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A470" s="70" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B470" s="70"/>
       <c r="C470" s="72" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E470" s="12"/>
     </row>
@@ -11309,7 +11343,7 @@
       </c>
       <c r="B549" s="77"/>
       <c r="C549" s="80" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D549" s="80" t="s">
         <v>7</v>
@@ -11749,11 +11783,11 @@
       </c>
       <c r="D590" s="8">
         <f>COUNTIF($D$2:$D588, "=Done*")+COUNTIF($D$2:$D588, "=OK*")+COUNTIF($D$2:$D588, "=Skip*")+COUNTIF($D$2:$D588, "=Defer*")+COUNTIF($D$2:$D588, "=Close*")+COUNTIF($D$2:$D588, "=Address*")+COUNTIF($D$2:$D588, "=See*")+COUNTIF($D$2:$D588, "=PT*")</f>
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E590" s="9">
         <f>$D590/$D$589</f>
-        <v>0.89452332657200806</v>
+        <v>0.90669371196754567</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.35">
@@ -11784,15 +11818,15 @@
     </row>
     <row r="593" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C593" s="28" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D593" s="8">
         <f>D589-SUM(D590:D592)</f>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E593" s="9">
         <f>$D593/$D$589</f>
-        <v>8.7221095334685597E-2</v>
+        <v>7.5050709939148072E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated InventoryDetails and task list
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill_\source\Projects\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0429584E-41BF-4AA5-B3C3-40BFC7245982}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D827164B-4C51-464E-82B3-ED341557F890}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1031">
   <si>
     <t>ID</t>
   </si>
@@ -4470,8 +4470,8 @@
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D233" sqref="D233:E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7430,6 +7430,12 @@
       <c r="C233" s="2" t="s">
         <v>865</v>
       </c>
+      <c r="D233" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E233" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="234" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A234" s="70" t="s">
@@ -7439,6 +7445,12 @@
       <c r="C234" s="72" t="s">
         <v>964</v>
       </c>
+      <c r="D234" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E234" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" s="70" t="s">
@@ -7448,6 +7460,12 @@
       <c r="C235" s="72" t="s">
         <v>966</v>
       </c>
+      <c r="D235" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E235" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" s="70" t="s">
@@ -7456,6 +7474,12 @@
       <c r="B236" s="70"/>
       <c r="C236" s="72" t="s">
         <v>968</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E236" s="12">
+        <v>43581</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.35">
@@ -11783,11 +11807,11 @@
       </c>
       <c r="D590" s="8">
         <f>COUNTIF($D$2:$D588, "=Done*")+COUNTIF($D$2:$D588, "=OK*")+COUNTIF($D$2:$D588, "=Skip*")+COUNTIF($D$2:$D588, "=Defer*")+COUNTIF($D$2:$D588, "=Close*")+COUNTIF($D$2:$D588, "=Address*")+COUNTIF($D$2:$D588, "=See*")+COUNTIF($D$2:$D588, "=PT*")</f>
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="E590" s="9">
         <f>$D590/$D$589</f>
-        <v>0.90669371196754567</v>
+        <v>0.9148073022312373</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.35">
@@ -11822,11 +11846,11 @@
       </c>
       <c r="D593" s="8">
         <f>D589-SUM(D590:D592)</f>
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E593" s="9">
         <f>$D593/$D$589</f>
-        <v>7.5050709939148072E-2</v>
+        <v>6.6937119675456389E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated QaInspection, QaInventory and task list
</commit_message>
<xml_diff>
--- a/BDC_V1/BDC_V1/Documents/Tasks.xlsx
+++ b/BDC_V1/BDC_V1/Documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill_\source\Projects\BDC\BDC_V1\BDC_V1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D827164B-4C51-464E-82B3-ED341557F890}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80EBF86-C937-42D1-8451-3CAF1C6A42AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="851" xr2:uid="{DACDA871-CB87-4368-8EE2-A4303C9959DA}"/>
   </bookViews>
@@ -253,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F504" authorId="0" shapeId="0" xr:uid="{C5459F54-D6E7-4473-9002-16DC428624B9}">
+    <comment ref="F507" authorId="0" shapeId="0" xr:uid="{C5459F54-D6E7-4473-9002-16DC428624B9}">
       <text>
         <r>
           <rPr>
@@ -277,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F505" authorId="0" shapeId="0" xr:uid="{78B09D58-01F3-49E7-B51F-38F363D04C92}">
+    <comment ref="F508" authorId="0" shapeId="0" xr:uid="{78B09D58-01F3-49E7-B51F-38F363D04C92}">
       <text>
         <r>
           <rPr>
@@ -301,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F534" authorId="0" shapeId="0" xr:uid="{219F0334-9C0D-4B0E-9917-EC384D011BEF}">
+    <comment ref="F537" authorId="0" shapeId="0" xr:uid="{219F0334-9C0D-4B0E-9917-EC384D011BEF}">
       <text>
         <r>
           <rPr>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1031">
   <si>
     <t>ID</t>
   </si>
@@ -4467,11 +4467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD8496-2E51-4D60-8137-BF15E4B09450}">
-  <dimension ref="A1:F593"/>
+  <dimension ref="A1:F596"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D233" sqref="D233:E233"/>
+      <pane ySplit="1" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D430" sqref="D430:E430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8375,8 +8375,12 @@
       <c r="C308" s="71" t="s">
         <v>952</v>
       </c>
-      <c r="D308" s="40"/>
-      <c r="E308" s="41"/>
+      <c r="D308" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E308" s="12">
+        <v>43581</v>
+      </c>
       <c r="F308" s="101"/>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.35">
@@ -8387,8 +8391,12 @@
       <c r="C309" s="71" t="s">
         <v>954</v>
       </c>
-      <c r="D309" s="40"/>
-      <c r="E309" s="41"/>
+      <c r="D309" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E309" s="12">
+        <v>43581</v>
+      </c>
       <c r="F309" s="101"/>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.35">
@@ -8399,8 +8407,12 @@
       <c r="C310" s="71" t="s">
         <v>956</v>
       </c>
-      <c r="D310" s="40"/>
-      <c r="E310" s="41"/>
+      <c r="D310" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E310" s="12">
+        <v>43581</v>
+      </c>
       <c r="F310" s="101"/>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.35">
@@ -8411,8 +8423,12 @@
       <c r="C311" s="71" t="s">
         <v>958</v>
       </c>
-      <c r="D311" s="40"/>
-      <c r="E311" s="41"/>
+      <c r="D311" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E311" s="12">
+        <v>43581</v>
+      </c>
       <c r="F311" s="101"/>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.35">
@@ -8423,8 +8439,12 @@
       <c r="C312" s="71" t="s">
         <v>960</v>
       </c>
-      <c r="D312" s="40"/>
-      <c r="E312" s="41"/>
+      <c r="D312" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E312" s="12">
+        <v>43581</v>
+      </c>
       <c r="F312" s="101"/>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.35">
@@ -8435,8 +8455,12 @@
       <c r="C313" s="71" t="s">
         <v>962</v>
       </c>
-      <c r="D313" s="40"/>
-      <c r="E313" s="41"/>
+      <c r="D313" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E313" s="12">
+        <v>43581</v>
+      </c>
       <c r="F313" s="101"/>
     </row>
     <row r="314" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -9095,6 +9119,12 @@
       <c r="C360" s="72" t="s">
         <v>969</v>
       </c>
+      <c r="D360" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E360" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="70" t="s">
@@ -9104,6 +9134,12 @@
       <c r="C361" s="72" t="s">
         <v>972</v>
       </c>
+      <c r="D361" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E361" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="70" t="s">
@@ -9113,6 +9149,12 @@
       <c r="C362" s="72" t="s">
         <v>974</v>
       </c>
+      <c r="D362" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E362" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="70" t="s">
@@ -9122,6 +9164,12 @@
       <c r="C363" s="72" t="s">
         <v>976</v>
       </c>
+      <c r="D363" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E363" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="70" t="s">
@@ -9131,6 +9179,12 @@
       <c r="C364" s="72" t="s">
         <v>978</v>
       </c>
+      <c r="D364" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E364" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="70" t="s">
@@ -9139,6 +9193,12 @@
       <c r="B365" s="70"/>
       <c r="C365" s="72" t="s">
         <v>980</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E365" s="12">
+        <v>43581</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
@@ -9682,347 +9742,352 @@
       <c r="E413" s="12"/>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A414" s="15"/>
-      <c r="B414" s="15" t="s">
+      <c r="E414" s="12"/>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E415" s="12"/>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E416" s="12"/>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A417" s="15"/>
+      <c r="B417" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="C414" s="16" t="s">
+      <c r="C417" s="16" t="s">
         <v>719</v>
       </c>
-      <c r="D414" s="16"/>
-      <c r="E414" s="15"/>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A415" s="1" t="s">
+      <c r="D417" s="16"/>
+      <c r="E417" s="15"/>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A418" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="C415" s="2" t="s">
+      <c r="C418" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D415" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E415" s="12">
+      <c r="D418" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E418" s="12">
         <v>43555</v>
       </c>
-      <c r="F415" s="98"/>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A416" s="1" t="s">
+      <c r="F418" s="98"/>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A419" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C416" s="2" t="s">
+      <c r="C419" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D416" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E416" s="12">
+      <c r="D419" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E419" s="12">
         <v>43555</v>
       </c>
-      <c r="F416" s="98"/>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A417" s="1" t="s">
+      <c r="F419" s="98"/>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A420" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C417" s="2" t="s">
+      <c r="C420" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="D417" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E417" s="12">
+      <c r="D420" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E420" s="12">
         <v>43555</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A418" s="1" t="s">
+    <row r="421" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A421" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="B418" s="1" t="s">
+      <c r="B421" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C418" s="7" t="s">
+      <c r="C421" s="7" t="s">
         <v>703</v>
       </c>
-      <c r="D418" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E418" s="37">
+      <c r="D421" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E421" s="37">
         <v>43581</v>
       </c>
-      <c r="F418" s="98"/>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A419" s="65" t="s">
+      <c r="F421" s="98"/>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A422" s="65" t="s">
         <v>868</v>
       </c>
-      <c r="B419" s="57"/>
-      <c r="C419" s="49" t="s">
+      <c r="B422" s="57"/>
+      <c r="C422" s="49" t="s">
         <v>704</v>
       </c>
-      <c r="D419" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E419" s="69">
+      <c r="D422" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E422" s="69">
         <v>43573</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A420" s="65" t="s">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A423" s="65" t="s">
         <v>869</v>
       </c>
-      <c r="B420" s="65"/>
-      <c r="C420" s="64" t="s">
+      <c r="B423" s="65"/>
+      <c r="C423" s="64" t="s">
         <v>564</v>
       </c>
-      <c r="D420" s="66" t="s">
+      <c r="D423" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="E420" s="67">
+      <c r="E423" s="67">
         <v>43574</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A421" s="25"/>
-      <c r="B421" s="25"/>
-      <c r="C421" s="64" t="s">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A424" s="25"/>
+      <c r="B424" s="25"/>
+      <c r="C424" s="64" t="s">
         <v>887</v>
       </c>
-      <c r="D421" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E421" s="52"/>
-      <c r="F421" s="42"/>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A422" s="1" t="s">
+      <c r="D424" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E424" s="52"/>
+      <c r="F424" s="42"/>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A425" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B422" s="1" t="s">
+      <c r="B425" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C422" s="2" t="s">
+      <c r="C425" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="D422" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E422" s="12">
+      <c r="D425" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E425" s="12">
         <v>43569</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A423" s="1" t="s">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A426" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C423" s="2" t="s">
+      <c r="C426" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="D423" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E423" s="12">
+      <c r="D426" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E426" s="12">
         <v>43568</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A424" s="1" t="s">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A427" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C424" s="2" t="s">
+      <c r="C427" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="D424" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A425" s="1" t="s">
+      <c r="D427" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A428" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="C425" s="36" t="s">
+      <c r="C428" s="36" t="s">
         <v>827</v>
       </c>
-      <c r="D425" s="2" t="s">
+      <c r="D428" s="2" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A426" s="42" t="s">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A429" s="42" t="s">
         <v>581</v>
       </c>
-      <c r="B426" s="42"/>
-      <c r="C426" s="36" t="s">
+      <c r="B429" s="42"/>
+      <c r="C429" s="36" t="s">
         <v>582</v>
       </c>
-      <c r="D426" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E426" s="37">
+      <c r="D429" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E429" s="37">
         <v>43573</v>
       </c>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A427" s="70" t="s">
-        <v>995</v>
-      </c>
-      <c r="B427" s="70"/>
-      <c r="C427" s="72" t="s">
-        <v>981</v>
-      </c>
-      <c r="E427" s="12"/>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A428" s="70" t="s">
-        <v>996</v>
-      </c>
-      <c r="B428" s="70"/>
-      <c r="C428" s="72" t="s">
-        <v>982</v>
-      </c>
-      <c r="E428" s="12"/>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A429" s="70" t="s">
-        <v>997</v>
-      </c>
-      <c r="B429" s="70"/>
-      <c r="C429" s="72" t="s">
-        <v>983</v>
-      </c>
-      <c r="E429" s="12"/>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A430" s="70" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B430" s="70"/>
       <c r="C430" s="72" t="s">
-        <v>984</v>
-      </c>
-      <c r="E430" s="12"/>
+        <v>981</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E430" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A431" s="70" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="B431" s="70"/>
       <c r="C431" s="72" t="s">
-        <v>985</v>
-      </c>
-      <c r="E431" s="12"/>
+        <v>982</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E431" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A432" s="70" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B432" s="70"/>
       <c r="C432" s="72" t="s">
-        <v>986</v>
-      </c>
-      <c r="E432" s="12"/>
-    </row>
-    <row r="433" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>983</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E432" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A433" s="70" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="B433" s="70"/>
       <c r="C433" s="72" t="s">
-        <v>987</v>
-      </c>
-      <c r="E433" s="12"/>
+        <v>984</v>
+      </c>
+      <c r="D433" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E433" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A434" s="70" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="B434" s="70"/>
       <c r="C434" s="72" t="s">
+        <v>985</v>
+      </c>
+      <c r="E434" s="12"/>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A435" s="70" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B435" s="70"/>
+      <c r="C435" s="72" t="s">
+        <v>986</v>
+      </c>
+      <c r="D435" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E435" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A436" s="70" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B436" s="70"/>
+      <c r="C436" s="72" t="s">
+        <v>987</v>
+      </c>
+      <c r="D436" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E436" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A437" s="70" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B437" s="70"/>
+      <c r="C437" s="72" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A435" s="73" t="s">
+      <c r="D437" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E437" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A438" s="73" t="s">
         <v>1004</v>
       </c>
-      <c r="B435" s="73"/>
-      <c r="C435" s="74" t="s">
+      <c r="B438" s="73"/>
+      <c r="C438" s="74" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="441" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A441" s="1"/>
-      <c r="B441" s="1"/>
-      <c r="C441" s="2"/>
-      <c r="D441" s="2"/>
-      <c r="E441" s="1"/>
-      <c r="F441" s="98"/>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A442" s="15"/>
-      <c r="B442" s="15" t="s">
+      <c r="D438" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E438" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A444" s="1"/>
+      <c r="B444" s="1"/>
+      <c r="C444" s="2"/>
+      <c r="D444" s="2"/>
+      <c r="E444" s="1"/>
+      <c r="F444" s="98"/>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A445" s="15"/>
+      <c r="B445" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="C442" s="16" t="s">
+      <c r="C445" s="16" t="s">
         <v>720</v>
       </c>
-      <c r="D442" s="16"/>
-      <c r="E442" s="15"/>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A443" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C443" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D443" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E443" s="12">
-        <v>43555</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A444" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="B444" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C444" s="75" t="s">
-        <v>1023</v>
-      </c>
-      <c r="D444" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E444" s="12">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A445" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="C445" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D445" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E445" s="12">
-        <v>43555</v>
-      </c>
-      <c r="F445" s="98"/>
+      <c r="D445" s="16"/>
+      <c r="E445" s="15"/>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A446" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C446" s="2" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="D446" s="2" t="s">
         <v>7</v>
@@ -10030,434 +10095,470 @@
       <c r="E446" s="12">
         <v>43555</v>
       </c>
-      <c r="F446" s="98"/>
     </row>
     <row r="447" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A447" s="42" t="s">
-        <v>563</v>
-      </c>
-      <c r="B447" s="42"/>
-      <c r="C447" s="36" t="s">
-        <v>562</v>
-      </c>
-      <c r="D447" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E447" s="37">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A447" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C447" s="75" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E447" s="12">
+        <v>43569</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A448" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="B448" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="C448" s="36" t="s">
-        <v>703</v>
+        <v>467</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>458</v>
       </c>
       <c r="D448" s="2" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E448" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="E448" s="12">
+        <v>43555</v>
+      </c>
+      <c r="F448" s="98"/>
     </row>
     <row r="449" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A449" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E449" s="12">
+        <v>43555</v>
+      </c>
+      <c r="F449" s="98"/>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A450" s="42" t="s">
+        <v>563</v>
+      </c>
+      <c r="B450" s="42"/>
+      <c r="C450" s="36" t="s">
+        <v>562</v>
+      </c>
+      <c r="D450" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E450" s="37">
+        <v>43576</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A451" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C451" s="36" t="s">
+        <v>703</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E451" s="12"/>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A452" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C449" s="36" t="s">
+      <c r="C452" s="36" t="s">
         <v>704</v>
       </c>
-      <c r="D449" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E449" s="37">
+      <c r="D452" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E452" s="37">
         <v>43581</v>
       </c>
-      <c r="F449" s="98"/>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A450" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="C450" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D450" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A451" s="44" t="s">
-        <v>870</v>
-      </c>
-      <c r="B451" s="44"/>
-      <c r="C451" s="38" t="s">
-        <v>564</v>
-      </c>
-      <c r="D451" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="E451" s="46">
-        <v>43574</v>
-      </c>
-    </row>
-    <row r="452" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A452" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="B452" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C452" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="D452" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="F452" s="98"/>
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A453" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C453" s="2" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="D453" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A454" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="C454" s="36" t="s">
-        <v>827</v>
-      </c>
-      <c r="D454" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A455" s="42" t="s">
-        <v>566</v>
-      </c>
-      <c r="B455" s="42"/>
-      <c r="C455" s="36" t="s">
-        <v>569</v>
-      </c>
-      <c r="D455" s="36" t="s">
-        <v>860</v>
-      </c>
-      <c r="E455" s="42"/>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A454" s="44" t="s">
+        <v>870</v>
+      </c>
+      <c r="B454" s="44"/>
+      <c r="C454" s="38" t="s">
+        <v>564</v>
+      </c>
+      <c r="D454" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="E454" s="46">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A455" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C455" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="D455" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A456" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C456" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D456" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A457" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C457" s="36" t="s">
+        <v>827</v>
+      </c>
+      <c r="D457" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A458" s="42" t="s">
+        <v>566</v>
+      </c>
+      <c r="B458" s="42"/>
+      <c r="C458" s="36" t="s">
+        <v>569</v>
+      </c>
+      <c r="D458" s="36" t="s">
+        <v>860</v>
+      </c>
+      <c r="E458" s="42"/>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A459" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C456" s="2" t="s">
+      <c r="C459" s="2" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A457" s="42" t="s">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A460" s="42" t="s">
         <v>571</v>
       </c>
-      <c r="B457" s="42"/>
-      <c r="C457" s="36" t="s">
+      <c r="B460" s="42"/>
+      <c r="C460" s="36" t="s">
         <v>572</v>
       </c>
-      <c r="D457" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E457" s="37">
+      <c r="D460" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E460" s="37">
         <v>43574</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A458" s="25" t="s">
+    <row r="461" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A461" s="25" t="s">
         <v>872</v>
       </c>
-      <c r="B458" s="25"/>
-      <c r="C458" s="64" t="s">
+      <c r="B461" s="25"/>
+      <c r="C461" s="64" t="s">
         <v>871</v>
       </c>
-      <c r="D458" s="51" t="s">
+      <c r="D461" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="E458" s="52">
+      <c r="E461" s="52">
         <v>43574</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A459" s="25"/>
-      <c r="B459" s="25"/>
-      <c r="C459" s="64" t="s">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A462" s="25"/>
+      <c r="B462" s="25"/>
+      <c r="C462" s="64" t="s">
         <v>888</v>
       </c>
-      <c r="D459" s="51" t="s">
+      <c r="D462" s="51" t="s">
         <v>857</v>
       </c>
-      <c r="E459" s="52"/>
-      <c r="F459" s="42"/>
-    </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A460" s="1" t="s">
+      <c r="E462" s="52"/>
+      <c r="F462" s="42"/>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A463" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="C460" s="2" t="s">
+      <c r="C463" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="D460" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E460" s="37">
+      <c r="D463" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E463" s="37">
         <v>43581</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A461" s="44" t="s">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A464" s="44" t="s">
         <v>873</v>
       </c>
-      <c r="B461" s="44"/>
-      <c r="C461" s="38" t="s">
+      <c r="B464" s="44"/>
+      <c r="C464" s="38" t="s">
         <v>874</v>
       </c>
-      <c r="D461" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E461" s="41">
+      <c r="D464" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E464" s="41">
         <v>43575</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A462" s="42" t="s">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A465" s="42" t="s">
         <v>575</v>
       </c>
-      <c r="B462" s="42"/>
-      <c r="C462" s="36" t="s">
+      <c r="B465" s="42"/>
+      <c r="C465" s="36" t="s">
         <v>576</v>
       </c>
-      <c r="D462" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E462" s="37">
+      <c r="D465" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E465" s="37">
         <v>43573</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A463" s="42" t="s">
+    <row r="466" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A466" s="42" t="s">
         <v>900</v>
       </c>
-      <c r="B463" s="42"/>
-      <c r="C463" s="36" t="s">
+      <c r="B466" s="42"/>
+      <c r="C466" s="36" t="s">
         <v>889</v>
       </c>
-      <c r="D463" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E463" s="37">
+      <c r="D466" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E466" s="37">
         <v>43579</v>
       </c>
-    </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A464" s="70" t="s">
-        <v>988</v>
-      </c>
-      <c r="B464" s="70"/>
-      <c r="C464" s="72" t="s">
-        <v>981</v>
-      </c>
-      <c r="E464" s="12"/>
-    </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A465" s="70" t="s">
-        <v>989</v>
-      </c>
-      <c r="B465" s="70"/>
-      <c r="C465" s="72" t="s">
-        <v>982</v>
-      </c>
-      <c r="E465" s="12"/>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A466" s="70" t="s">
-        <v>990</v>
-      </c>
-      <c r="B466" s="70"/>
-      <c r="C466" s="72" t="s">
-        <v>983</v>
-      </c>
-      <c r="E466" s="12"/>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A467" s="70" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B467" s="70"/>
       <c r="C467" s="72" t="s">
-        <v>984</v>
-      </c>
-      <c r="E467" s="12"/>
+        <v>981</v>
+      </c>
+      <c r="D467" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E467" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A468" s="70" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B468" s="70"/>
       <c r="C468" s="72" t="s">
-        <v>985</v>
-      </c>
-      <c r="E468" s="12"/>
+        <v>982</v>
+      </c>
+      <c r="D468" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E468" s="12">
+        <v>43581</v>
+      </c>
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A469" s="70" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B469" s="70"/>
       <c r="C469" s="72" t="s">
-        <v>986</v>
-      </c>
-      <c r="E469" s="12"/>
-    </row>
-    <row r="470" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>983</v>
+      </c>
+      <c r="D469" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E469" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A470" s="70" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B470" s="70"/>
       <c r="C470" s="72" t="s">
+        <v>984</v>
+      </c>
+      <c r="D470" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E470" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A471" s="70" t="s">
+        <v>992</v>
+      </c>
+      <c r="B471" s="70"/>
+      <c r="C471" s="72" t="s">
+        <v>985</v>
+      </c>
+      <c r="D471" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E471" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A472" s="70" t="s">
+        <v>993</v>
+      </c>
+      <c r="B472" s="70"/>
+      <c r="C472" s="72" t="s">
+        <v>986</v>
+      </c>
+      <c r="D472" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E472" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A473" s="70" t="s">
+        <v>994</v>
+      </c>
+      <c r="B473" s="70"/>
+      <c r="C473" s="72" t="s">
         <v>987</v>
       </c>
-      <c r="E470" s="12"/>
-    </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E471" s="12"/>
-    </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A472" s="15"/>
-      <c r="B472" s="15" t="s">
+      <c r="D473" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E473" s="12">
+        <v>43581</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E474" s="12"/>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A475" s="15"/>
+      <c r="B475" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C472" s="16" t="s">
+      <c r="C475" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="D472" s="16"/>
-      <c r="E472" s="15"/>
-    </row>
-    <row r="473" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A473" s="1" t="s">
+      <c r="D475" s="16"/>
+      <c r="E475" s="15"/>
+    </row>
+    <row r="476" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A476" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B473" s="1"/>
-      <c r="C473" s="2" t="s">
+      <c r="B476" s="1"/>
+      <c r="C476" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D473" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E473" s="12">
+      <c r="D476" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E476" s="12">
         <v>43555</v>
       </c>
-      <c r="F473" s="1"/>
-    </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A474" s="42" t="s">
-        <v>890</v>
-      </c>
-      <c r="B474" s="42"/>
-      <c r="C474" s="36" t="s">
-        <v>891</v>
-      </c>
-      <c r="D474" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E474" s="37">
-        <v>43579</v>
-      </c>
-    </row>
-    <row r="475" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A475" s="42" t="s">
-        <v>892</v>
-      </c>
-      <c r="B475" s="42"/>
-      <c r="C475" s="36" t="s">
-        <v>893</v>
-      </c>
-      <c r="D475" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E475" s="37">
-        <v>43579</v>
-      </c>
-    </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A476" s="42" t="s">
-        <v>894</v>
-      </c>
-      <c r="B476" s="42"/>
-      <c r="C476" s="36" t="s">
-        <v>895</v>
-      </c>
-      <c r="D476" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E476" s="37">
-        <v>43581</v>
-      </c>
+      <c r="F476" s="1"/>
     </row>
     <row r="477" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A477" s="42" t="s">
-        <v>283</v>
+        <v>890</v>
       </c>
       <c r="B477" s="42"/>
       <c r="C477" s="36" t="s">
-        <v>284</v>
+        <v>891</v>
       </c>
       <c r="D477" s="36" t="s">
         <v>7</v>
       </c>
       <c r="E477" s="37">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43579</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A478" s="42" t="s">
-        <v>285</v>
+        <v>892</v>
       </c>
       <c r="B478" s="42"/>
       <c r="C478" s="36" t="s">
-        <v>286</v>
+        <v>893</v>
       </c>
       <c r="D478" s="36" t="s">
         <v>7</v>
       </c>
       <c r="E478" s="37">
-        <v>43568</v>
+        <v>43579</v>
       </c>
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A479" s="42" t="s">
-        <v>287</v>
+        <v>894</v>
       </c>
       <c r="B479" s="42"/>
       <c r="C479" s="36" t="s">
-        <v>288</v>
+        <v>895</v>
       </c>
       <c r="D479" s="36" t="s">
         <v>7</v>
       </c>
       <c r="E479" s="37">
-        <v>43568</v>
+        <v>43581</v>
       </c>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A480" s="42" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B480" s="42"/>
       <c r="C480" s="36" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D480" s="36" t="s">
         <v>7</v>
@@ -10468,83 +10569,86 @@
     </row>
     <row r="481" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A481" s="42" t="s">
-        <v>829</v>
+        <v>285</v>
       </c>
       <c r="B481" s="42"/>
       <c r="C481" s="36" t="s">
-        <v>830</v>
-      </c>
-      <c r="D481" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E481" s="41">
-        <v>43574</v>
+        <v>286</v>
+      </c>
+      <c r="D481" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E481" s="37">
+        <v>43568</v>
       </c>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A482" s="42" t="s">
-        <v>896</v>
+        <v>287</v>
       </c>
       <c r="B482" s="42"/>
       <c r="C482" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="D482" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E482" s="37">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A483" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="B483" s="42"/>
+      <c r="C483" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="D483" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E483" s="37">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A484" s="42" t="s">
+        <v>829</v>
+      </c>
+      <c r="B484" s="42"/>
+      <c r="C484" s="36" t="s">
+        <v>830</v>
+      </c>
+      <c r="D484" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E484" s="41">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A485" s="42" t="s">
+        <v>896</v>
+      </c>
+      <c r="B485" s="42"/>
+      <c r="C485" s="36" t="s">
         <v>897</v>
       </c>
-      <c r="D482" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E482" s="41">
+      <c r="D485" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E485" s="41">
         <v>43579</v>
       </c>
-      <c r="F482" s="31"/>
-    </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A483" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C483" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D483" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E483" s="12">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A484" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="C484" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="D484" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E484" s="12">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="485" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A485" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="C485" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="D485" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E485" s="41">
-        <v>43574</v>
-      </c>
+      <c r="F485" s="31"/>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A486" s="1" t="s">
-        <v>752</v>
+        <v>312</v>
       </c>
       <c r="C486" s="2" t="s">
-        <v>753</v>
+        <v>310</v>
       </c>
       <c r="D486" s="2" t="s">
         <v>7</v>
@@ -10555,10 +10659,10 @@
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A487" s="1" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="C487" s="2" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="D487" s="2" t="s">
         <v>7</v>
@@ -10567,27 +10671,26 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A488" s="1" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="C488" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="D488" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E488" s="12">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="489" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
+        <v>751</v>
+      </c>
+      <c r="D488" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E488" s="41">
+        <v>43574</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A489" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="B489" s="1"/>
+        <v>752</v>
+      </c>
       <c r="C489" s="2" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="D489" s="2" t="s">
         <v>7</v>
@@ -10595,14 +10698,13 @@
       <c r="E489" s="12">
         <v>43569</v>
       </c>
-      <c r="F489" s="1"/>
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A490" s="1" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="D490" s="2" t="s">
         <v>7</v>
@@ -10613,10 +10715,10 @@
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A491" s="1" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="C491" s="2" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="D491" s="2" t="s">
         <v>7</v>
@@ -10625,12 +10727,13 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A492" s="1" t="s">
-        <v>764</v>
-      </c>
+        <v>758</v>
+      </c>
+      <c r="B492" s="1"/>
       <c r="C492" s="2" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="D492" s="2" t="s">
         <v>7</v>
@@ -10638,262 +10741,268 @@
       <c r="E492" s="12">
         <v>43569</v>
       </c>
+      <c r="F492" s="1"/>
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A493" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C493" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D493" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E493" s="12">
+        <v>43569</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A494" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="C494" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D494" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E494" s="12">
+        <v>43569</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A495" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C495" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="D495" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E495" s="12">
+        <v>43569</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A496" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="C493" s="2" t="s">
+      <c r="C496" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="D493" s="2" t="s">
+      <c r="D496" s="2" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A494" s="57" t="s">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A497" s="57" t="s">
         <v>768</v>
-      </c>
-      <c r="B494" s="48"/>
-      <c r="C494" s="49" t="s">
-        <v>769</v>
-      </c>
-      <c r="D494" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A495" s="57" t="s">
-        <v>831</v>
-      </c>
-      <c r="B495" s="48"/>
-      <c r="C495" s="49" t="s">
-        <v>832</v>
-      </c>
-      <c r="D495" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="496" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A496" s="48" t="s">
-        <v>770</v>
-      </c>
-      <c r="B496" s="48"/>
-      <c r="C496" s="49" t="s">
-        <v>771</v>
-      </c>
-      <c r="D496" s="36" t="s">
-        <v>493</v>
-      </c>
-      <c r="E496" s="42"/>
-    </row>
-    <row r="497" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A497" s="48" t="s">
-        <v>833</v>
       </c>
       <c r="B497" s="48"/>
       <c r="C497" s="49" t="s">
+        <v>769</v>
+      </c>
+      <c r="D497" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A498" s="57" t="s">
+        <v>831</v>
+      </c>
+      <c r="B498" s="48"/>
+      <c r="C498" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="D498" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A499" s="48" t="s">
+        <v>770</v>
+      </c>
+      <c r="B499" s="48"/>
+      <c r="C499" s="49" t="s">
+        <v>771</v>
+      </c>
+      <c r="D499" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="E499" s="42"/>
+    </row>
+    <row r="500" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A500" s="48" t="s">
+        <v>833</v>
+      </c>
+      <c r="B500" s="48"/>
+      <c r="C500" s="49" t="s">
         <v>834</v>
       </c>
-      <c r="D497" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E497" s="37">
+      <c r="D500" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E500" s="37">
         <v>43573</v>
       </c>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A498" s="48"/>
-      <c r="B498" s="48"/>
-      <c r="C498" s="49"/>
-      <c r="D498" s="36"/>
-      <c r="E498" s="37"/>
-    </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A500" s="15"/>
-      <c r="B500" s="15" t="s">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A501" s="48"/>
+      <c r="B501" s="48"/>
+      <c r="C501" s="49"/>
+      <c r="D501" s="36"/>
+      <c r="E501" s="37"/>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A503" s="15"/>
+      <c r="B503" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C500" s="16" t="s">
+      <c r="C503" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="D500" s="16"/>
-      <c r="E500" s="22"/>
-    </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A501" s="1" t="s">
+      <c r="D503" s="16"/>
+      <c r="E503" s="22"/>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A504" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C501" s="2" t="s">
+      <c r="C504" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D501" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A502" s="1" t="s">
+      <c r="D504" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A505" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C502" s="2" t="s">
+      <c r="C505" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D502" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A503" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C503" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D503" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A504" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="B504" s="50"/>
-      <c r="C504" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="D504" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F504" s="23" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A505" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="B505" s="50"/>
-      <c r="C505" s="17" t="s">
-        <v>344</v>
-      </c>
       <c r="D505" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F505" s="23" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A506" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C506" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D506" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F506" s="98"/>
     </row>
     <row r="507" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A507" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C507" s="2" t="s">
-        <v>65</v>
+      <c r="A507" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B507" s="50"/>
+      <c r="C507" s="17" t="s">
+        <v>343</v>
       </c>
       <c r="D507" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="508" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A508" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="B508" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="F507" s="23" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A508" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B508" s="50"/>
       <c r="C508" s="17" t="s">
-        <v>711</v>
-      </c>
-      <c r="D508" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E508" s="12">
-        <v>43568</v>
+        <v>344</v>
+      </c>
+      <c r="D508" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F508" s="23" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A509" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="B509" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C509" s="2" t="s">
-        <v>713</v>
+        <v>63</v>
       </c>
       <c r="D509" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E509" s="12">
-        <v>43528</v>
-      </c>
+      <c r="F509" s="98"/>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A510" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C510" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D510" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A511" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C511" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D511" s="2" t="s">
-        <v>7</v>
+        <v>741</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C511" s="17" t="s">
+        <v>711</v>
+      </c>
+      <c r="D511" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E511" s="12">
+        <v>43568</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A512" s="1" t="s">
-        <v>70</v>
+        <v>712</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C512" s="2" t="s">
-        <v>71</v>
+        <v>713</v>
       </c>
       <c r="D512" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="513" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A513" s="42" t="s">
-        <v>802</v>
-      </c>
-      <c r="B513" s="42"/>
-      <c r="C513" s="36" t="s">
-        <v>898</v>
-      </c>
-      <c r="D513" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E513" s="41">
-        <v>43579</v>
-      </c>
-    </row>
-    <row r="514" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E512" s="12">
+        <v>43528</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A513" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D513" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A514" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C514" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D514" s="2" t="s">
         <v>7</v>
@@ -10901,81 +11010,85 @@
     </row>
     <row r="515" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A515" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C515" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D515" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="516" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A516" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="B516" s="50"/>
-      <c r="C516" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="D516" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E516" s="50"/>
-    </row>
-    <row r="517" spans="1:6" s="54" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A517" s="57" t="s">
-        <v>855</v>
-      </c>
-      <c r="B517" s="68"/>
-      <c r="C517" s="103" t="s">
-        <v>856</v>
-      </c>
-      <c r="D517" s="36" t="s">
-        <v>857</v>
-      </c>
-      <c r="E517" s="42"/>
-      <c r="F517" s="42"/>
+    <row r="516" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A516" s="42" t="s">
+        <v>802</v>
+      </c>
+      <c r="B516" s="42"/>
+      <c r="C516" s="36" t="s">
+        <v>898</v>
+      </c>
+      <c r="D516" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E516" s="41">
+        <v>43579</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A517" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D517" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="518" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A518" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C518" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D518" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="519" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A519" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C519" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D519" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="520" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A520" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C520" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D520" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A519" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="B519" s="50"/>
+      <c r="C519" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="D519" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E519" s="50"/>
+    </row>
+    <row r="520" spans="1:6" s="54" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A520" s="57" t="s">
+        <v>855</v>
+      </c>
+      <c r="B520" s="68"/>
+      <c r="C520" s="103" t="s">
+        <v>856</v>
+      </c>
+      <c r="D520" s="36" t="s">
+        <v>857</v>
+      </c>
+      <c r="E520" s="42"/>
+      <c r="F520" s="42"/>
     </row>
     <row r="521" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A521" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C521" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D521" s="2" t="s">
         <v>7</v>
@@ -10983,10 +11096,10 @@
     </row>
     <row r="522" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A522" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C522" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D522" s="2" t="s">
         <v>7</v>
@@ -10994,189 +11107,179 @@
     </row>
     <row r="523" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A523" s="1" t="s">
-        <v>177</v>
+        <v>80</v>
       </c>
       <c r="C523" s="2" t="s">
-        <v>345</v>
+        <v>81</v>
       </c>
       <c r="D523" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E523" s="12">
-        <v>43554</v>
       </c>
     </row>
     <row r="524" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A524" s="1" t="s">
-        <v>210</v>
+        <v>82</v>
       </c>
       <c r="C524" s="2" t="s">
-        <v>213</v>
+        <v>83</v>
       </c>
       <c r="D524" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E524" s="12">
-        <v>43554</v>
       </c>
     </row>
     <row r="525" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A525" s="1" t="s">
-        <v>738</v>
+        <v>84</v>
       </c>
       <c r="C525" s="2" t="s">
-        <v>346</v>
+        <v>85</v>
       </c>
       <c r="D525" s="2" t="s">
-        <v>837</v>
-      </c>
-      <c r="E525" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A526" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C526" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D526" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E526" s="12">
         <v>43554</v>
-      </c>
-    </row>
-    <row r="526" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A526" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="C526" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D526" s="2" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="527" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A527" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="C527" s="49" t="s">
-        <v>836</v>
+        <v>210</v>
+      </c>
+      <c r="C527" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="D527" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="528" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A528" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="B528" s="2"/>
+      <c r="E527" s="12">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A528" s="1" t="s">
+        <v>738</v>
+      </c>
       <c r="C528" s="2" t="s">
-        <v>470</v>
+        <v>346</v>
       </c>
       <c r="D528" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E528" s="2">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="529" spans="1:6" x14ac:dyDescent="0.35">
+        <v>837</v>
+      </c>
+      <c r="E528" s="12">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A529" s="1" t="s">
-        <v>179</v>
+        <v>739</v>
       </c>
       <c r="C529" s="2" t="s">
-        <v>347</v>
+        <v>217</v>
       </c>
       <c r="D529" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E529" s="12">
-        <v>43554</v>
+        <v>837</v>
       </c>
     </row>
     <row r="530" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A530" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C530" s="2" t="s">
-        <v>348</v>
+        <v>835</v>
+      </c>
+      <c r="C530" s="49" t="s">
+        <v>836</v>
       </c>
       <c r="D530" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E530" s="12">
-        <v>43554</v>
-      </c>
     </row>
     <row r="531" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A531" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="B531" s="57"/>
-      <c r="C531" s="49" t="s">
-        <v>349</v>
-      </c>
-      <c r="D531" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E531" s="69">
-        <v>43572</v>
+      <c r="A531" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B531" s="2"/>
+      <c r="C531" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D531" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E531" s="2">
+        <v>43568</v>
       </c>
     </row>
     <row r="532" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A532" s="1" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="C532" s="2" t="s">
-        <v>212</v>
+        <v>347</v>
       </c>
       <c r="D532" s="2" t="s">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="E532" s="12">
         <v>43554</v>
       </c>
     </row>
-    <row r="533" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A533" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C533" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D533" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E533" s="12">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A534" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="B534" s="57"/>
+      <c r="C534" s="49" t="s">
+        <v>349</v>
+      </c>
+      <c r="D534" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E534" s="69">
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A535" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C535" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D535" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E535" s="12">
+        <v>43554</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A536" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="C533" s="2" t="s">
+      <c r="C536" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="D533" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E533" s="12">
-        <v>43559</v>
-      </c>
-    </row>
-    <row r="534" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A534" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="C534" s="17" t="s">
-        <v>328</v>
-      </c>
-      <c r="D534" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E534" s="12">
-        <v>43554</v>
-      </c>
-      <c r="F534" s="23" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="535" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A535" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="C535" s="49" t="s">
-        <v>471</v>
-      </c>
-      <c r="D535" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E535" s="12"/>
-    </row>
-    <row r="536" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A536" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="C536" s="47" t="s">
-        <v>733</v>
       </c>
       <c r="D536" s="2" t="s">
         <v>7</v>
@@ -11185,99 +11288,97 @@
         <v>43559</v>
       </c>
     </row>
-    <row r="537" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A537" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C537" s="2" t="s">
-        <v>230</v>
+        <v>735</v>
+      </c>
+      <c r="C537" s="17" t="s">
+        <v>328</v>
       </c>
       <c r="D537" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E537" s="12">
-        <v>43559</v>
-      </c>
-    </row>
-    <row r="538" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43554</v>
+      </c>
+      <c r="F537" s="23" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A538" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C538" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D538" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E538" s="12">
-        <v>43559</v>
-      </c>
+        <v>736</v>
+      </c>
+      <c r="C538" s="49" t="s">
+        <v>471</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E538" s="12"/>
     </row>
     <row r="539" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A539" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C539" s="2" t="s">
-        <v>354</v>
+        <v>737</v>
+      </c>
+      <c r="C539" s="47" t="s">
+        <v>733</v>
       </c>
       <c r="D539" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E539" s="12">
-        <v>43581</v>
+        <v>43559</v>
       </c>
     </row>
     <row r="540" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A540" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="C540" s="17" t="s">
-        <v>488</v>
-      </c>
-      <c r="D540" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C540" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D540" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E540" s="12">
         <v>43559</v>
       </c>
-      <c r="F540" s="23" t="s">
-        <v>715</v>
-      </c>
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A541" s="1" t="s">
-        <v>231</v>
+        <v>351</v>
       </c>
       <c r="C541" s="2" t="s">
-        <v>232</v>
+        <v>352</v>
       </c>
       <c r="D541" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E541" s="12">
-        <v>43555</v>
+        <v>43559</v>
       </c>
     </row>
     <row r="542" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A542" s="1" t="s">
-        <v>233</v>
+        <v>353</v>
       </c>
       <c r="C542" s="2" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="D542" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E542" s="12">
-        <v>43555</v>
+        <v>43581</v>
       </c>
     </row>
     <row r="543" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A543" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C543" s="17" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D543" s="17" t="s">
         <v>7</v>
@@ -11289,273 +11390,303 @@
         <v>715</v>
       </c>
     </row>
-    <row r="544" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="544" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A544" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="C544" s="17" t="s">
-        <v>722</v>
-      </c>
-      <c r="D544" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D544" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E544" s="12">
-        <v>43568</v>
+        <v>43555</v>
       </c>
     </row>
     <row r="545" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A545" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C545" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D545" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E545" s="12">
+        <v>43555</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A546" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C546" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="D546" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E546" s="12">
+        <v>43559</v>
+      </c>
+      <c r="F546" s="23" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A547" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="C547" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="D547" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E547" s="12">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A548" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="C545" s="2" t="s">
+      <c r="C548" s="2" t="s">
         <v>732</v>
       </c>
-      <c r="D545" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E545" s="12">
+      <c r="D548" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E548" s="12">
         <v>43568</v>
       </c>
     </row>
-    <row r="546" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A546" s="1" t="s">
+    <row r="549" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A549" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C546" s="2" t="s">
+      <c r="C549" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="D546" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E546" s="12">
+      <c r="D549" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E549" s="12">
         <v>43568</v>
       </c>
     </row>
-    <row r="547" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A547" s="1" t="s">
+    <row r="550" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A550" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="C547" s="2" t="s">
+      <c r="C550" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="D547" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E547" s="12">
+      <c r="D550" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E550" s="12">
         <v>43581</v>
       </c>
     </row>
-    <row r="548" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A548" s="42" t="s">
+    <row r="551" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A551" s="42" t="s">
         <v>858</v>
       </c>
-      <c r="B548" s="42"/>
-      <c r="C548" s="49" t="s">
+      <c r="B551" s="42"/>
+      <c r="C551" s="49" t="s">
         <v>859</v>
       </c>
-      <c r="D548" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E548" s="37">
+      <c r="D551" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E551" s="37">
         <v>43575</v>
       </c>
-      <c r="F548" s="42"/>
-    </row>
-    <row r="549" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A549" s="77" t="s">
+      <c r="F551" s="42"/>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A552" s="77" t="s">
         <v>901</v>
       </c>
-      <c r="B549" s="77"/>
-      <c r="C549" s="80" t="s">
+      <c r="B552" s="77"/>
+      <c r="C552" s="80" t="s">
         <v>1024</v>
       </c>
-      <c r="D549" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E549" s="81">
+      <c r="D552" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E552" s="81">
         <v>43580</v>
       </c>
     </row>
-    <row r="550" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A550" s="77" t="s">
+    <row r="553" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A553" s="77" t="s">
         <v>902</v>
       </c>
-      <c r="B550" s="77"/>
-      <c r="C550" s="80" t="s">
+      <c r="B553" s="77"/>
+      <c r="C553" s="80" t="s">
         <v>903</v>
       </c>
-      <c r="D550" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E550" s="81">
+      <c r="D553" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E553" s="81">
         <v>43580</v>
       </c>
     </row>
-    <row r="551" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A551" s="77" t="s">
+    <row r="554" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A554" s="77" t="s">
         <v>904</v>
       </c>
-      <c r="B551" s="77"/>
-      <c r="C551" s="80" t="s">
+      <c r="B554" s="77"/>
+      <c r="C554" s="80" t="s">
         <v>905</v>
       </c>
-      <c r="D551" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E551" s="81">
+      <c r="D554" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E554" s="81">
         <v>43580</v>
       </c>
-    </row>
-    <row r="552" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A552" s="70" t="s">
-        <v>906</v>
-      </c>
-      <c r="B552" s="70"/>
-      <c r="C552" s="71" t="s">
-        <v>907</v>
-      </c>
-      <c r="D552" s="49"/>
-      <c r="E552" s="37"/>
-    </row>
-    <row r="553" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A553" s="70" t="s">
-        <v>908</v>
-      </c>
-      <c r="B553" s="70"/>
-      <c r="C553" s="71" t="s">
-        <v>909</v>
-      </c>
-      <c r="D553" s="49"/>
-      <c r="E553" s="37"/>
-    </row>
-    <row r="554" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A554" s="70" t="s">
-        <v>922</v>
-      </c>
-      <c r="B554" s="70"/>
-      <c r="C554" s="71" t="s">
-        <v>923</v>
-      </c>
-      <c r="D554" s="49"/>
-      <c r="E554" s="37"/>
     </row>
     <row r="555" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A555" s="70" t="s">
-        <v>924</v>
+        <v>906</v>
       </c>
       <c r="B555" s="70"/>
       <c r="C555" s="71" t="s">
-        <v>925</v>
+        <v>907</v>
       </c>
       <c r="D555" s="49"/>
       <c r="E555" s="37"/>
     </row>
     <row r="556" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A556" s="77" t="s">
-        <v>926</v>
-      </c>
-      <c r="B556" s="77"/>
-      <c r="C556" s="80" t="s">
-        <v>927</v>
-      </c>
-      <c r="D556" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E556" s="81">
-        <v>43580</v>
-      </c>
+      <c r="A556" s="70" t="s">
+        <v>908</v>
+      </c>
+      <c r="B556" s="70"/>
+      <c r="C556" s="71" t="s">
+        <v>909</v>
+      </c>
+      <c r="D556" s="49"/>
+      <c r="E556" s="37"/>
     </row>
     <row r="557" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A557" s="77" t="s">
-        <v>928</v>
-      </c>
-      <c r="B557" s="77"/>
-      <c r="C557" s="80" t="s">
-        <v>929</v>
-      </c>
-      <c r="D557" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E557" s="81">
-        <v>43580</v>
-      </c>
+      <c r="A557" s="70" t="s">
+        <v>922</v>
+      </c>
+      <c r="B557" s="70"/>
+      <c r="C557" s="71" t="s">
+        <v>923</v>
+      </c>
+      <c r="D557" s="49"/>
+      <c r="E557" s="37"/>
     </row>
     <row r="558" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A558" s="42"/>
-      <c r="B558" s="42"/>
-      <c r="C558" s="49"/>
+      <c r="A558" s="70" t="s">
+        <v>924</v>
+      </c>
+      <c r="B558" s="70"/>
+      <c r="C558" s="71" t="s">
+        <v>925</v>
+      </c>
       <c r="D558" s="49"/>
       <c r="E558" s="37"/>
     </row>
     <row r="559" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A559" s="42"/>
-      <c r="B559" s="42"/>
-      <c r="C559" s="49"/>
-      <c r="D559" s="49"/>
-      <c r="E559" s="37"/>
+      <c r="A559" s="77" t="s">
+        <v>926</v>
+      </c>
+      <c r="B559" s="77"/>
+      <c r="C559" s="80" t="s">
+        <v>927</v>
+      </c>
+      <c r="D559" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E559" s="81">
+        <v>43580</v>
+      </c>
     </row>
     <row r="560" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A560" s="42"/>
-      <c r="B560" s="42"/>
-      <c r="C560" s="49"/>
-      <c r="D560" s="49"/>
-      <c r="E560" s="37"/>
+      <c r="A560" s="77" t="s">
+        <v>928</v>
+      </c>
+      <c r="B560" s="77"/>
+      <c r="C560" s="80" t="s">
+        <v>929</v>
+      </c>
+      <c r="D560" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E560" s="81">
+        <v>43580</v>
+      </c>
     </row>
     <row r="561" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A561" s="15"/>
-      <c r="B561" s="15" t="s">
+      <c r="A561" s="42"/>
+      <c r="B561" s="42"/>
+      <c r="C561" s="49"/>
+      <c r="D561" s="49"/>
+      <c r="E561" s="37"/>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A562" s="42"/>
+      <c r="B562" s="42"/>
+      <c r="C562" s="49"/>
+      <c r="D562" s="49"/>
+      <c r="E562" s="37"/>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A563" s="42"/>
+      <c r="B563" s="42"/>
+      <c r="C563" s="49"/>
+      <c r="D563" s="49"/>
+      <c r="E563" s="37"/>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A564" s="15"/>
+      <c r="B564" s="15" t="s">
         <v>916</v>
       </c>
-      <c r="C561" s="16" t="s">
+      <c r="C564" s="16" t="s">
         <v>917</v>
       </c>
-      <c r="D561" s="16"/>
-      <c r="E561" s="22"/>
-    </row>
-    <row r="562" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A562" s="77" t="s">
+      <c r="D564" s="16"/>
+      <c r="E564" s="22"/>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A565" s="77" t="s">
         <v>918</v>
       </c>
-      <c r="B562" s="77"/>
-      <c r="C562" s="80" t="s">
+      <c r="B565" s="77"/>
+      <c r="C565" s="80" t="s">
         <v>919</v>
       </c>
-      <c r="D562" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E562" s="81">
+      <c r="D565" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E565" s="81">
         <v>43580</v>
       </c>
     </row>
-    <row r="563" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A563" s="77" t="s">
+    <row r="566" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A566" s="77" t="s">
         <v>920</v>
       </c>
-      <c r="B563" s="77"/>
-      <c r="C563" s="80" t="s">
+      <c r="B566" s="77"/>
+      <c r="C566" s="80" t="s">
         <v>921</v>
       </c>
-      <c r="D563" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E563" s="81">
+      <c r="D566" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E566" s="81">
         <v>43580</v>
       </c>
-    </row>
-    <row r="564" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C564" s="17"/>
-      <c r="D564" s="17"/>
-      <c r="E564" s="12"/>
-    </row>
-    <row r="565" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C565" s="17"/>
-      <c r="D565" s="17"/>
-      <c r="E565" s="12"/>
-    </row>
-    <row r="566" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C566" s="17"/>
-      <c r="D566" s="17"/>
-      <c r="E566" s="12"/>
     </row>
     <row r="567" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C567" s="17"/>
@@ -11573,96 +11704,65 @@
       <c r="E569" s="12"/>
     </row>
     <row r="570" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A570" s="22"/>
-      <c r="B570" s="22" t="s">
+      <c r="C570" s="17"/>
+      <c r="D570" s="17"/>
+      <c r="E570" s="12"/>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C571" s="17"/>
+      <c r="D571" s="17"/>
+      <c r="E571" s="12"/>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C572" s="17"/>
+      <c r="D572" s="17"/>
+      <c r="E572" s="12"/>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A573" s="22"/>
+      <c r="B573" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C570" s="24"/>
-      <c r="D570" s="24"/>
-      <c r="E570" s="22"/>
-    </row>
-    <row r="571" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A571" s="1" t="s">
+      <c r="C573" s="24"/>
+      <c r="D573" s="24"/>
+      <c r="E573" s="22"/>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A574" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C571" s="2" t="s">
+      <c r="C574" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D571" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E571" s="12">
+      <c r="D574" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E574" s="12">
         <v>43554</v>
       </c>
     </row>
-    <row r="572" spans="1:6" s="54" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A572" s="42" t="s">
+    <row r="575" spans="1:6" s="54" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A575" s="42" t="s">
         <v>838</v>
       </c>
-      <c r="B572" s="42"/>
-      <c r="C572" s="36" t="s">
+      <c r="B575" s="42"/>
+      <c r="C575" s="36" t="s">
         <v>839</v>
       </c>
-      <c r="D572" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E572" s="53">
+      <c r="D575" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E575" s="53">
         <v>43572</v>
       </c>
-      <c r="F572" s="42"/>
-    </row>
-    <row r="573" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A573" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C573" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D573" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E573" s="12">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="574" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A574" s="42" t="s">
-        <v>224</v>
-      </c>
-      <c r="B574" s="42"/>
-      <c r="C574" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="D574" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="E574" s="37">
-        <v>43555</v>
-      </c>
-      <c r="F574" s="98"/>
-    </row>
-    <row r="575" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A575" s="42" t="s">
-        <v>728</v>
-      </c>
-      <c r="B575" s="42"/>
-      <c r="C575" s="49" t="s">
-        <v>729</v>
-      </c>
-      <c r="D575" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E575" s="37">
-        <v>43573</v>
-      </c>
-      <c r="F575" s="98"/>
+      <c r="F575" s="42"/>
     </row>
     <row r="576" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A576" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C576" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="D576" s="2" t="s">
         <v>7</v>
@@ -11670,57 +11770,63 @@
       <c r="E576" s="12">
         <v>43568</v>
       </c>
-      <c r="F576" s="98"/>
     </row>
     <row r="577" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A577" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="B577" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C577" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="D577" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E577" s="12">
-        <v>43537</v>
+      <c r="A577" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="B577" s="42"/>
+      <c r="C577" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="D577" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="E577" s="37">
+        <v>43555</v>
       </c>
       <c r="F577" s="98"/>
     </row>
     <row r="578" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A578" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="B578" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C578" s="75" t="s">
-        <v>899</v>
-      </c>
-      <c r="D578" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A578" s="42" t="s">
+        <v>728</v>
+      </c>
+      <c r="B578" s="42"/>
+      <c r="C578" s="49" t="s">
+        <v>729</v>
+      </c>
+      <c r="D578" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E578" s="37">
+        <v>43573</v>
+      </c>
+      <c r="F578" s="98"/>
     </row>
     <row r="579" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A579" s="1" t="s">
-        <v>840</v>
+        <v>225</v>
       </c>
       <c r="C579" s="2" t="s">
-        <v>841</v>
+        <v>228</v>
       </c>
       <c r="D579" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E579" s="12">
+        <v>43568</v>
+      </c>
+      <c r="F579" s="98"/>
     </row>
     <row r="580" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A580" s="1" t="s">
-        <v>726</v>
+        <v>716</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="D580" s="2" t="s">
         <v>7</v>
@@ -11728,129 +11834,169 @@
       <c r="E580" s="12">
         <v>43537</v>
       </c>
+      <c r="F580" s="98"/>
     </row>
     <row r="581" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A581" s="77" t="s">
+      <c r="A581" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C581" s="75" t="s">
+        <v>899</v>
+      </c>
+      <c r="D581" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A582" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C582" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="D582" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A583" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C583" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D583" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E583" s="12">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A584" s="77" t="s">
         <v>910</v>
       </c>
-      <c r="B581" s="77"/>
-      <c r="C581" s="78" t="s">
+      <c r="B584" s="77"/>
+      <c r="C584" s="78" t="s">
         <v>911</v>
       </c>
-      <c r="D581" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="E581" s="81">
+      <c r="D584" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E584" s="81">
         <v>43580</v>
       </c>
     </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A582" s="77" t="s">
+    <row r="585" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A585" s="77" t="s">
         <v>912</v>
       </c>
-      <c r="B582" s="77"/>
-      <c r="C582" s="78" t="s">
+      <c r="B585" s="77"/>
+      <c r="C585" s="78" t="s">
         <v>913</v>
       </c>
-      <c r="D582" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="E582" s="81">
+      <c r="D585" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E585" s="81">
         <v>43580</v>
       </c>
     </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A583" s="77" t="s">
+    <row r="586" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A586" s="77" t="s">
         <v>914</v>
       </c>
-      <c r="B583" s="77"/>
-      <c r="C583" s="78" t="s">
+      <c r="B586" s="77"/>
+      <c r="C586" s="78" t="s">
         <v>915</v>
       </c>
-      <c r="D583" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="E583" s="81">
+      <c r="D586" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E586" s="81">
         <v>43580</v>
       </c>
-    </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E584" s="12"/>
-    </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E585" s="12"/>
-    </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E586" s="12"/>
     </row>
     <row r="587" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E587" s="12"/>
     </row>
-    <row r="588" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="588" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E588" s="12"/>
     </row>
-    <row r="589" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A589" s="10"/>
-      <c r="B589" s="10"/>
-      <c r="C589" s="27" t="s">
+    <row r="589" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E589" s="12"/>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E590" s="12"/>
+    </row>
+    <row r="591" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E591" s="12"/>
+    </row>
+    <row r="592" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A592" s="10"/>
+      <c r="B592" s="10"/>
+      <c r="C592" s="27" t="s">
         <v>627</v>
       </c>
-      <c r="D589" s="11">
-        <f>COUNTA($A$2:$A592)</f>
+      <c r="D592" s="11">
+        <f>COUNTA($A$2:$A595)</f>
         <v>493</v>
       </c>
-      <c r="E589" s="13"/>
-    </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C590" s="28" t="s">
-        <v>628</v>
-      </c>
-      <c r="D590" s="8">
-        <f>COUNTIF($D$2:$D588, "=Done*")+COUNTIF($D$2:$D588, "=OK*")+COUNTIF($D$2:$D588, "=Skip*")+COUNTIF($D$2:$D588, "=Defer*")+COUNTIF($D$2:$D588, "=Close*")+COUNTIF($D$2:$D588, "=Address*")+COUNTIF($D$2:$D588, "=See*")+COUNTIF($D$2:$D588, "=PT*")</f>
-        <v>451</v>
-      </c>
-      <c r="E590" s="9">
-        <f>$D590/$D$589</f>
-        <v>0.9148073022312373</v>
-      </c>
-    </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C591" s="28" t="s">
-        <v>629</v>
-      </c>
-      <c r="D591" s="8">
-        <f>COUNTIF($D$1:$D589, "=In process*")</f>
-        <v>1</v>
-      </c>
-      <c r="E591" s="9">
-        <f>$D591/$D$589</f>
-        <v>2.0283975659229209E-3</v>
-      </c>
-    </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C592" s="28" t="s">
-        <v>630</v>
-      </c>
-      <c r="D592" s="8">
-        <f>COUNTIF($D$1:$D590, "=Pending*")</f>
-        <v>8</v>
-      </c>
-      <c r="E592" s="9">
-        <f>$D592/$D$589</f>
-        <v>1.6227180527383367E-2</v>
-      </c>
+      <c r="E592" s="13"/>
     </row>
     <row r="593" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C593" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="D593" s="8">
+        <f>COUNTIF($D$2:$D591, "=Done*")+COUNTIF($D$2:$D591, "=OK*")+COUNTIF($D$2:$D591, "=Skip*")+COUNTIF($D$2:$D591, "=Defer*")+COUNTIF($D$2:$D591, "=Close*")+COUNTIF($D$2:$D591, "=Address*")+COUNTIF($D$2:$D591, "=See*")+COUNTIF($D$2:$D591, "=PT*")</f>
+        <v>478</v>
+      </c>
+      <c r="E593" s="9">
+        <f>$D593/$D$592</f>
+        <v>0.96957403651115615</v>
+      </c>
+    </row>
+    <row r="594" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C594" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="D594" s="8">
+        <f>COUNTIF($D$1:$D592, "=In process*")</f>
+        <v>1</v>
+      </c>
+      <c r="E594" s="9">
+        <f>$D594/$D$592</f>
+        <v>2.0283975659229209E-3</v>
+      </c>
+    </row>
+    <row r="595" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C595" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="D595" s="8">
+        <f>COUNTIF($D$1:$D593, "=Pending*")</f>
+        <v>8</v>
+      </c>
+      <c r="E595" s="9">
+        <f>$D595/$D$592</f>
+        <v>1.6227180527383367E-2</v>
+      </c>
+    </row>
+    <row r="596" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C596" s="28" t="s">
         <v>1025</v>
       </c>
-      <c r="D593" s="8">
-        <f>D589-SUM(D590:D592)</f>
-        <v>33</v>
-      </c>
-      <c r="E593" s="9">
-        <f>$D593/$D$589</f>
-        <v>6.6937119675456389E-2</v>
+      <c r="D596" s="8">
+        <f>D592-SUM(D593:D595)</f>
+        <v>6</v>
+      </c>
+      <c r="E596" s="9">
+        <f>$D596/$D$592</f>
+        <v>1.2170385395537525E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>